<commit_message>
Indicador de llamadas - Que cargue las llamadas de la última semana y arreglar liga al historial
</commit_message>
<xml_diff>
--- a/Scrum Febrero.xlsx
+++ b/Scrum Febrero.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="114">
   <si>
     <t>TOÑO</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Todos - Actualizar de prospecto a actual</t>
   </si>
   <si>
-    <t>Cotización - Enviar como PDF y Excel</t>
-  </si>
-  <si>
     <t>Cotizaciones - Mostrar dirección fiscal ??</t>
   </si>
   <si>
@@ -356,13 +353,22 @@
   </si>
   <si>
     <t>Indicadores - Revisar diseño del detalle</t>
+  </si>
+  <si>
+    <t>Cotización - Enviar como PDF y Excel ??</t>
+  </si>
+  <si>
+    <t>Agregar liga a historial de llamadas</t>
+  </si>
+  <si>
+    <t>12/02/2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -376,12 +382,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -770,7 +770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -865,6 +865,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -893,10 +899,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2122,11 +2126,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -2221,11 +2225,11 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
       <c r="D10" s="19"/>
       <c r="E10" s="8"/>
     </row>
@@ -2306,20 +2310,20 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="80" t="s">
+      <c r="A21" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="82"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="88"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="88"/>
-      <c r="C22" s="89"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="95"/>
       <c r="D22" s="31"/>
       <c r="E22" s="32"/>
     </row>
@@ -2340,10 +2344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV25"/>
+  <dimension ref="A1:IV24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2355,11 +2359,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2495,14 +2499,14 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="84">
         <v>42778</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>24</v>
+      <c r="C10" s="101" t="s">
+        <v>113</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="19"/>
@@ -2512,26 +2516,22 @@
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="10">
         <v>42785</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="35"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="10">
-        <v>42785</v>
-      </c>
-      <c r="C12" s="11"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="7"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -2539,33 +2539,33 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="A13" s="37"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="96"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="A14" s="85" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="7"/>
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
@@ -2573,33 +2573,35 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="7"/>
+      <c r="A16" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="19"/>
+      <c r="A17" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="22"/>
+      <c r="A18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="7"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
@@ -2607,9 +2609,7 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1">
-      <c r="A19" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="A19" s="30"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24"/>
       <c r="D19" s="7"/>
@@ -2628,7 +2628,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
+    <row r="21" spans="1:8" ht="15" hidden="1" customHeight="1">
       <c r="A21" s="30"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
@@ -2648,10 +2648,12 @@
       <c r="G22" s="19"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" ht="15" hidden="1" customHeight="1">
-      <c r="A23" s="30"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
+    <row r="23" spans="1:8" ht="15" customHeight="1">
+      <c r="A23" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="87"/>
+      <c r="C23" s="88"/>
       <c r="D23" s="7"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
@@ -2659,35 +2661,23 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="80" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="87" t="s">
+      <c r="A24" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="88"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="32"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2699,10 +2689,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV33"/>
+  <dimension ref="A1:IV36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2713,19 +2703,19 @@
     <col min="4" max="256" width="8.85546875" style="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:256" ht="15" customHeight="1">
+      <c r="A1" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2741,7 +2731,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:256" ht="15" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>32</v>
       </c>
@@ -2757,7 +2747,7 @@
       <c r="G3" s="19"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:256" ht="15" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>33</v>
       </c>
@@ -2773,7 +2763,7 @@
       <c r="G4" s="19"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
+    <row r="5" spans="1:256" ht="15" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
@@ -2789,7 +2779,7 @@
       <c r="G5" s="18"/>
       <c r="H5" s="35"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" spans="1:256" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>35</v>
       </c>
@@ -2805,7 +2795,7 @@
       <c r="G6" s="19"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
+    <row r="7" spans="1:256" ht="15" customHeight="1">
       <c r="A7" s="12" t="s">
         <v>36</v>
       </c>
@@ -2821,7 +2811,7 @@
       <c r="G7" s="19"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
+    <row r="8" spans="1:256" ht="15" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>37</v>
       </c>
@@ -2837,14 +2827,14 @@
       <c r="G8" s="18"/>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="A9" s="94" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="95">
+    <row r="9" spans="1:256" ht="15" customHeight="1">
+      <c r="A9" s="83" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="84">
         <v>42785</v>
       </c>
-      <c r="C9" s="96">
+      <c r="C9" s="85">
         <v>42784</v>
       </c>
       <c r="D9" s="34"/>
@@ -2853,119 +2843,1123 @@
       <c r="G9" s="18"/>
       <c r="H9" s="35"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:256" ht="15" customHeight="1">
+      <c r="A10" s="83" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="84">
+        <v>42785</v>
+      </c>
+      <c r="C10" s="85">
+        <v>42785</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="75"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="75"/>
+      <c r="S10" s="75"/>
+      <c r="T10" s="75"/>
+      <c r="U10" s="75"/>
+      <c r="V10" s="75"/>
+      <c r="W10" s="75"/>
+      <c r="X10" s="75"/>
+      <c r="Y10" s="75"/>
+      <c r="Z10" s="75"/>
+      <c r="AA10" s="75"/>
+      <c r="AB10" s="75"/>
+      <c r="AC10" s="75"/>
+      <c r="AD10" s="75"/>
+      <c r="AE10" s="75"/>
+      <c r="AF10" s="75"/>
+      <c r="AG10" s="75"/>
+      <c r="AH10" s="75"/>
+      <c r="AI10" s="75"/>
+      <c r="AJ10" s="75"/>
+      <c r="AK10" s="75"/>
+      <c r="AL10" s="75"/>
+      <c r="AM10" s="75"/>
+      <c r="AN10" s="75"/>
+      <c r="AO10" s="75"/>
+      <c r="AP10" s="75"/>
+      <c r="AQ10" s="75"/>
+      <c r="AR10" s="75"/>
+      <c r="AS10" s="75"/>
+      <c r="AT10" s="75"/>
+      <c r="AU10" s="75"/>
+      <c r="AV10" s="75"/>
+      <c r="AW10" s="75"/>
+      <c r="AX10" s="75"/>
+      <c r="AY10" s="75"/>
+      <c r="AZ10" s="75"/>
+      <c r="BA10" s="75"/>
+      <c r="BB10" s="75"/>
+      <c r="BC10" s="75"/>
+      <c r="BD10" s="75"/>
+      <c r="BE10" s="75"/>
+      <c r="BF10" s="75"/>
+      <c r="BG10" s="75"/>
+      <c r="BH10" s="75"/>
+      <c r="BI10" s="75"/>
+      <c r="BJ10" s="75"/>
+      <c r="BK10" s="75"/>
+      <c r="BL10" s="75"/>
+      <c r="BM10" s="75"/>
+      <c r="BN10" s="75"/>
+      <c r="BO10" s="75"/>
+      <c r="BP10" s="75"/>
+      <c r="BQ10" s="75"/>
+      <c r="BR10" s="75"/>
+      <c r="BS10" s="75"/>
+      <c r="BT10" s="75"/>
+      <c r="BU10" s="75"/>
+      <c r="BV10" s="75"/>
+      <c r="BW10" s="75"/>
+      <c r="BX10" s="75"/>
+      <c r="BY10" s="75"/>
+      <c r="BZ10" s="75"/>
+      <c r="CA10" s="75"/>
+      <c r="CB10" s="75"/>
+      <c r="CC10" s="75"/>
+      <c r="CD10" s="75"/>
+      <c r="CE10" s="75"/>
+      <c r="CF10" s="75"/>
+      <c r="CG10" s="75"/>
+      <c r="CH10" s="75"/>
+      <c r="CI10" s="75"/>
+      <c r="CJ10" s="75"/>
+      <c r="CK10" s="75"/>
+      <c r="CL10" s="75"/>
+      <c r="CM10" s="75"/>
+      <c r="CN10" s="75"/>
+      <c r="CO10" s="75"/>
+      <c r="CP10" s="75"/>
+      <c r="CQ10" s="75"/>
+      <c r="CR10" s="75"/>
+      <c r="CS10" s="75"/>
+      <c r="CT10" s="75"/>
+      <c r="CU10" s="75"/>
+      <c r="CV10" s="75"/>
+      <c r="CW10" s="75"/>
+      <c r="CX10" s="75"/>
+      <c r="CY10" s="75"/>
+      <c r="CZ10" s="75"/>
+      <c r="DA10" s="75"/>
+      <c r="DB10" s="75"/>
+      <c r="DC10" s="75"/>
+      <c r="DD10" s="75"/>
+      <c r="DE10" s="75"/>
+      <c r="DF10" s="75"/>
+      <c r="DG10" s="75"/>
+      <c r="DH10" s="75"/>
+      <c r="DI10" s="75"/>
+      <c r="DJ10" s="75"/>
+      <c r="DK10" s="75"/>
+      <c r="DL10" s="75"/>
+      <c r="DM10" s="75"/>
+      <c r="DN10" s="75"/>
+      <c r="DO10" s="75"/>
+      <c r="DP10" s="75"/>
+      <c r="DQ10" s="75"/>
+      <c r="DR10" s="75"/>
+      <c r="DS10" s="75"/>
+      <c r="DT10" s="75"/>
+      <c r="DU10" s="75"/>
+      <c r="DV10" s="75"/>
+      <c r="DW10" s="75"/>
+      <c r="DX10" s="75"/>
+      <c r="DY10" s="75"/>
+      <c r="DZ10" s="75"/>
+      <c r="EA10" s="75"/>
+      <c r="EB10" s="75"/>
+      <c r="EC10" s="75"/>
+      <c r="ED10" s="75"/>
+      <c r="EE10" s="75"/>
+      <c r="EF10" s="75"/>
+      <c r="EG10" s="75"/>
+      <c r="EH10" s="75"/>
+      <c r="EI10" s="75"/>
+      <c r="EJ10" s="75"/>
+      <c r="EK10" s="75"/>
+      <c r="EL10" s="75"/>
+      <c r="EM10" s="75"/>
+      <c r="EN10" s="75"/>
+      <c r="EO10" s="75"/>
+      <c r="EP10" s="75"/>
+      <c r="EQ10" s="75"/>
+      <c r="ER10" s="75"/>
+      <c r="ES10" s="75"/>
+      <c r="ET10" s="75"/>
+      <c r="EU10" s="75"/>
+      <c r="EV10" s="75"/>
+      <c r="EW10" s="75"/>
+      <c r="EX10" s="75"/>
+      <c r="EY10" s="75"/>
+      <c r="EZ10" s="75"/>
+      <c r="FA10" s="75"/>
+      <c r="FB10" s="75"/>
+      <c r="FC10" s="75"/>
+      <c r="FD10" s="75"/>
+      <c r="FE10" s="75"/>
+      <c r="FF10" s="75"/>
+      <c r="FG10" s="75"/>
+      <c r="FH10" s="75"/>
+      <c r="FI10" s="75"/>
+      <c r="FJ10" s="75"/>
+      <c r="FK10" s="75"/>
+      <c r="FL10" s="75"/>
+      <c r="FM10" s="75"/>
+      <c r="FN10" s="75"/>
+      <c r="FO10" s="75"/>
+      <c r="FP10" s="75"/>
+      <c r="FQ10" s="75"/>
+      <c r="FR10" s="75"/>
+      <c r="FS10" s="75"/>
+      <c r="FT10" s="75"/>
+      <c r="FU10" s="75"/>
+      <c r="FV10" s="75"/>
+      <c r="FW10" s="75"/>
+      <c r="FX10" s="75"/>
+      <c r="FY10" s="75"/>
+      <c r="FZ10" s="75"/>
+      <c r="GA10" s="75"/>
+      <c r="GB10" s="75"/>
+      <c r="GC10" s="75"/>
+      <c r="GD10" s="75"/>
+      <c r="GE10" s="75"/>
+      <c r="GF10" s="75"/>
+      <c r="GG10" s="75"/>
+      <c r="GH10" s="75"/>
+      <c r="GI10" s="75"/>
+      <c r="GJ10" s="75"/>
+      <c r="GK10" s="75"/>
+      <c r="GL10" s="75"/>
+      <c r="GM10" s="75"/>
+      <c r="GN10" s="75"/>
+      <c r="GO10" s="75"/>
+      <c r="GP10" s="75"/>
+      <c r="GQ10" s="75"/>
+      <c r="GR10" s="75"/>
+      <c r="GS10" s="75"/>
+      <c r="GT10" s="75"/>
+      <c r="GU10" s="75"/>
+      <c r="GV10" s="75"/>
+      <c r="GW10" s="75"/>
+      <c r="GX10" s="75"/>
+      <c r="GY10" s="75"/>
+      <c r="GZ10" s="75"/>
+      <c r="HA10" s="75"/>
+      <c r="HB10" s="75"/>
+      <c r="HC10" s="75"/>
+      <c r="HD10" s="75"/>
+      <c r="HE10" s="75"/>
+      <c r="HF10" s="75"/>
+      <c r="HG10" s="75"/>
+      <c r="HH10" s="75"/>
+      <c r="HI10" s="75"/>
+      <c r="HJ10" s="75"/>
+      <c r="HK10" s="75"/>
+      <c r="HL10" s="75"/>
+      <c r="HM10" s="75"/>
+      <c r="HN10" s="75"/>
+      <c r="HO10" s="75"/>
+      <c r="HP10" s="75"/>
+      <c r="HQ10" s="75"/>
+      <c r="HR10" s="75"/>
+      <c r="HS10" s="75"/>
+      <c r="HT10" s="75"/>
+      <c r="HU10" s="75"/>
+      <c r="HV10" s="75"/>
+      <c r="HW10" s="75"/>
+      <c r="HX10" s="75"/>
+      <c r="HY10" s="75"/>
+      <c r="HZ10" s="75"/>
+      <c r="IA10" s="75"/>
+      <c r="IB10" s="75"/>
+      <c r="IC10" s="75"/>
+      <c r="ID10" s="75"/>
+      <c r="IE10" s="75"/>
+      <c r="IF10" s="75"/>
+      <c r="IG10" s="75"/>
+      <c r="IH10" s="75"/>
+      <c r="II10" s="75"/>
+      <c r="IJ10" s="75"/>
+      <c r="IK10" s="75"/>
+      <c r="IL10" s="75"/>
+      <c r="IM10" s="75"/>
+      <c r="IN10" s="75"/>
+      <c r="IO10" s="75"/>
+      <c r="IP10" s="75"/>
+      <c r="IQ10" s="75"/>
+      <c r="IR10" s="75"/>
+      <c r="IS10" s="75"/>
+      <c r="IT10" s="75"/>
+      <c r="IU10" s="75"/>
+      <c r="IV10" s="75"/>
+    </row>
+    <row r="11" spans="1:256" ht="15" customHeight="1">
+      <c r="A11" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="84">
+        <v>42785</v>
+      </c>
+      <c r="C11" s="85">
+        <v>42785</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="75"/>
+      <c r="O11" s="75"/>
+      <c r="P11" s="75"/>
+      <c r="Q11" s="75"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="75"/>
+      <c r="T11" s="75"/>
+      <c r="U11" s="75"/>
+      <c r="V11" s="75"/>
+      <c r="W11" s="75"/>
+      <c r="X11" s="75"/>
+      <c r="Y11" s="75"/>
+      <c r="Z11" s="75"/>
+      <c r="AA11" s="75"/>
+      <c r="AB11" s="75"/>
+      <c r="AC11" s="75"/>
+      <c r="AD11" s="75"/>
+      <c r="AE11" s="75"/>
+      <c r="AF11" s="75"/>
+      <c r="AG11" s="75"/>
+      <c r="AH11" s="75"/>
+      <c r="AI11" s="75"/>
+      <c r="AJ11" s="75"/>
+      <c r="AK11" s="75"/>
+      <c r="AL11" s="75"/>
+      <c r="AM11" s="75"/>
+      <c r="AN11" s="75"/>
+      <c r="AO11" s="75"/>
+      <c r="AP11" s="75"/>
+      <c r="AQ11" s="75"/>
+      <c r="AR11" s="75"/>
+      <c r="AS11" s="75"/>
+      <c r="AT11" s="75"/>
+      <c r="AU11" s="75"/>
+      <c r="AV11" s="75"/>
+      <c r="AW11" s="75"/>
+      <c r="AX11" s="75"/>
+      <c r="AY11" s="75"/>
+      <c r="AZ11" s="75"/>
+      <c r="BA11" s="75"/>
+      <c r="BB11" s="75"/>
+      <c r="BC11" s="75"/>
+      <c r="BD11" s="75"/>
+      <c r="BE11" s="75"/>
+      <c r="BF11" s="75"/>
+      <c r="BG11" s="75"/>
+      <c r="BH11" s="75"/>
+      <c r="BI11" s="75"/>
+      <c r="BJ11" s="75"/>
+      <c r="BK11" s="75"/>
+      <c r="BL11" s="75"/>
+      <c r="BM11" s="75"/>
+      <c r="BN11" s="75"/>
+      <c r="BO11" s="75"/>
+      <c r="BP11" s="75"/>
+      <c r="BQ11" s="75"/>
+      <c r="BR11" s="75"/>
+      <c r="BS11" s="75"/>
+      <c r="BT11" s="75"/>
+      <c r="BU11" s="75"/>
+      <c r="BV11" s="75"/>
+      <c r="BW11" s="75"/>
+      <c r="BX11" s="75"/>
+      <c r="BY11" s="75"/>
+      <c r="BZ11" s="75"/>
+      <c r="CA11" s="75"/>
+      <c r="CB11" s="75"/>
+      <c r="CC11" s="75"/>
+      <c r="CD11" s="75"/>
+      <c r="CE11" s="75"/>
+      <c r="CF11" s="75"/>
+      <c r="CG11" s="75"/>
+      <c r="CH11" s="75"/>
+      <c r="CI11" s="75"/>
+      <c r="CJ11" s="75"/>
+      <c r="CK11" s="75"/>
+      <c r="CL11" s="75"/>
+      <c r="CM11" s="75"/>
+      <c r="CN11" s="75"/>
+      <c r="CO11" s="75"/>
+      <c r="CP11" s="75"/>
+      <c r="CQ11" s="75"/>
+      <c r="CR11" s="75"/>
+      <c r="CS11" s="75"/>
+      <c r="CT11" s="75"/>
+      <c r="CU11" s="75"/>
+      <c r="CV11" s="75"/>
+      <c r="CW11" s="75"/>
+      <c r="CX11" s="75"/>
+      <c r="CY11" s="75"/>
+      <c r="CZ11" s="75"/>
+      <c r="DA11" s="75"/>
+      <c r="DB11" s="75"/>
+      <c r="DC11" s="75"/>
+      <c r="DD11" s="75"/>
+      <c r="DE11" s="75"/>
+      <c r="DF11" s="75"/>
+      <c r="DG11" s="75"/>
+      <c r="DH11" s="75"/>
+      <c r="DI11" s="75"/>
+      <c r="DJ11" s="75"/>
+      <c r="DK11" s="75"/>
+      <c r="DL11" s="75"/>
+      <c r="DM11" s="75"/>
+      <c r="DN11" s="75"/>
+      <c r="DO11" s="75"/>
+      <c r="DP11" s="75"/>
+      <c r="DQ11" s="75"/>
+      <c r="DR11" s="75"/>
+      <c r="DS11" s="75"/>
+      <c r="DT11" s="75"/>
+      <c r="DU11" s="75"/>
+      <c r="DV11" s="75"/>
+      <c r="DW11" s="75"/>
+      <c r="DX11" s="75"/>
+      <c r="DY11" s="75"/>
+      <c r="DZ11" s="75"/>
+      <c r="EA11" s="75"/>
+      <c r="EB11" s="75"/>
+      <c r="EC11" s="75"/>
+      <c r="ED11" s="75"/>
+      <c r="EE11" s="75"/>
+      <c r="EF11" s="75"/>
+      <c r="EG11" s="75"/>
+      <c r="EH11" s="75"/>
+      <c r="EI11" s="75"/>
+      <c r="EJ11" s="75"/>
+      <c r="EK11" s="75"/>
+      <c r="EL11" s="75"/>
+      <c r="EM11" s="75"/>
+      <c r="EN11" s="75"/>
+      <c r="EO11" s="75"/>
+      <c r="EP11" s="75"/>
+      <c r="EQ11" s="75"/>
+      <c r="ER11" s="75"/>
+      <c r="ES11" s="75"/>
+      <c r="ET11" s="75"/>
+      <c r="EU11" s="75"/>
+      <c r="EV11" s="75"/>
+      <c r="EW11" s="75"/>
+      <c r="EX11" s="75"/>
+      <c r="EY11" s="75"/>
+      <c r="EZ11" s="75"/>
+      <c r="FA11" s="75"/>
+      <c r="FB11" s="75"/>
+      <c r="FC11" s="75"/>
+      <c r="FD11" s="75"/>
+      <c r="FE11" s="75"/>
+      <c r="FF11" s="75"/>
+      <c r="FG11" s="75"/>
+      <c r="FH11" s="75"/>
+      <c r="FI11" s="75"/>
+      <c r="FJ11" s="75"/>
+      <c r="FK11" s="75"/>
+      <c r="FL11" s="75"/>
+      <c r="FM11" s="75"/>
+      <c r="FN11" s="75"/>
+      <c r="FO11" s="75"/>
+      <c r="FP11" s="75"/>
+      <c r="FQ11" s="75"/>
+      <c r="FR11" s="75"/>
+      <c r="FS11" s="75"/>
+      <c r="FT11" s="75"/>
+      <c r="FU11" s="75"/>
+      <c r="FV11" s="75"/>
+      <c r="FW11" s="75"/>
+      <c r="FX11" s="75"/>
+      <c r="FY11" s="75"/>
+      <c r="FZ11" s="75"/>
+      <c r="GA11" s="75"/>
+      <c r="GB11" s="75"/>
+      <c r="GC11" s="75"/>
+      <c r="GD11" s="75"/>
+      <c r="GE11" s="75"/>
+      <c r="GF11" s="75"/>
+      <c r="GG11" s="75"/>
+      <c r="GH11" s="75"/>
+      <c r="GI11" s="75"/>
+      <c r="GJ11" s="75"/>
+      <c r="GK11" s="75"/>
+      <c r="GL11" s="75"/>
+      <c r="GM11" s="75"/>
+      <c r="GN11" s="75"/>
+      <c r="GO11" s="75"/>
+      <c r="GP11" s="75"/>
+      <c r="GQ11" s="75"/>
+      <c r="GR11" s="75"/>
+      <c r="GS11" s="75"/>
+      <c r="GT11" s="75"/>
+      <c r="GU11" s="75"/>
+      <c r="GV11" s="75"/>
+      <c r="GW11" s="75"/>
+      <c r="GX11" s="75"/>
+      <c r="GY11" s="75"/>
+      <c r="GZ11" s="75"/>
+      <c r="HA11" s="75"/>
+      <c r="HB11" s="75"/>
+      <c r="HC11" s="75"/>
+      <c r="HD11" s="75"/>
+      <c r="HE11" s="75"/>
+      <c r="HF11" s="75"/>
+      <c r="HG11" s="75"/>
+      <c r="HH11" s="75"/>
+      <c r="HI11" s="75"/>
+      <c r="HJ11" s="75"/>
+      <c r="HK11" s="75"/>
+      <c r="HL11" s="75"/>
+      <c r="HM11" s="75"/>
+      <c r="HN11" s="75"/>
+      <c r="HO11" s="75"/>
+      <c r="HP11" s="75"/>
+      <c r="HQ11" s="75"/>
+      <c r="HR11" s="75"/>
+      <c r="HS11" s="75"/>
+      <c r="HT11" s="75"/>
+      <c r="HU11" s="75"/>
+      <c r="HV11" s="75"/>
+      <c r="HW11" s="75"/>
+      <c r="HX11" s="75"/>
+      <c r="HY11" s="75"/>
+      <c r="HZ11" s="75"/>
+      <c r="IA11" s="75"/>
+      <c r="IB11" s="75"/>
+      <c r="IC11" s="75"/>
+      <c r="ID11" s="75"/>
+      <c r="IE11" s="75"/>
+      <c r="IF11" s="75"/>
+      <c r="IG11" s="75"/>
+      <c r="IH11" s="75"/>
+      <c r="II11" s="75"/>
+      <c r="IJ11" s="75"/>
+      <c r="IK11" s="75"/>
+      <c r="IL11" s="75"/>
+      <c r="IM11" s="75"/>
+      <c r="IN11" s="75"/>
+      <c r="IO11" s="75"/>
+      <c r="IP11" s="75"/>
+      <c r="IQ11" s="75"/>
+      <c r="IR11" s="75"/>
+      <c r="IS11" s="75"/>
+      <c r="IT11" s="75"/>
+      <c r="IU11" s="75"/>
+      <c r="IV11" s="75"/>
+    </row>
+    <row r="12" spans="1:256" ht="15" customHeight="1">
+      <c r="A12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B12" s="10">
         <v>42785</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="35"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="1:256" ht="15" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="10">
+        <v>42785</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="75"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="75"/>
+      <c r="S13" s="75"/>
+      <c r="T13" s="75"/>
+      <c r="U13" s="75"/>
+      <c r="V13" s="75"/>
+      <c r="W13" s="75"/>
+      <c r="X13" s="75"/>
+      <c r="Y13" s="75"/>
+      <c r="Z13" s="75"/>
+      <c r="AA13" s="75"/>
+      <c r="AB13" s="75"/>
+      <c r="AC13" s="75"/>
+      <c r="AD13" s="75"/>
+      <c r="AE13" s="75"/>
+      <c r="AF13" s="75"/>
+      <c r="AG13" s="75"/>
+      <c r="AH13" s="75"/>
+      <c r="AI13" s="75"/>
+      <c r="AJ13" s="75"/>
+      <c r="AK13" s="75"/>
+      <c r="AL13" s="75"/>
+      <c r="AM13" s="75"/>
+      <c r="AN13" s="75"/>
+      <c r="AO13" s="75"/>
+      <c r="AP13" s="75"/>
+      <c r="AQ13" s="75"/>
+      <c r="AR13" s="75"/>
+      <c r="AS13" s="75"/>
+      <c r="AT13" s="75"/>
+      <c r="AU13" s="75"/>
+      <c r="AV13" s="75"/>
+      <c r="AW13" s="75"/>
+      <c r="AX13" s="75"/>
+      <c r="AY13" s="75"/>
+      <c r="AZ13" s="75"/>
+      <c r="BA13" s="75"/>
+      <c r="BB13" s="75"/>
+      <c r="BC13" s="75"/>
+      <c r="BD13" s="75"/>
+      <c r="BE13" s="75"/>
+      <c r="BF13" s="75"/>
+      <c r="BG13" s="75"/>
+      <c r="BH13" s="75"/>
+      <c r="BI13" s="75"/>
+      <c r="BJ13" s="75"/>
+      <c r="BK13" s="75"/>
+      <c r="BL13" s="75"/>
+      <c r="BM13" s="75"/>
+      <c r="BN13" s="75"/>
+      <c r="BO13" s="75"/>
+      <c r="BP13" s="75"/>
+      <c r="BQ13" s="75"/>
+      <c r="BR13" s="75"/>
+      <c r="BS13" s="75"/>
+      <c r="BT13" s="75"/>
+      <c r="BU13" s="75"/>
+      <c r="BV13" s="75"/>
+      <c r="BW13" s="75"/>
+      <c r="BX13" s="75"/>
+      <c r="BY13" s="75"/>
+      <c r="BZ13" s="75"/>
+      <c r="CA13" s="75"/>
+      <c r="CB13" s="75"/>
+      <c r="CC13" s="75"/>
+      <c r="CD13" s="75"/>
+      <c r="CE13" s="75"/>
+      <c r="CF13" s="75"/>
+      <c r="CG13" s="75"/>
+      <c r="CH13" s="75"/>
+      <c r="CI13" s="75"/>
+      <c r="CJ13" s="75"/>
+      <c r="CK13" s="75"/>
+      <c r="CL13" s="75"/>
+      <c r="CM13" s="75"/>
+      <c r="CN13" s="75"/>
+      <c r="CO13" s="75"/>
+      <c r="CP13" s="75"/>
+      <c r="CQ13" s="75"/>
+      <c r="CR13" s="75"/>
+      <c r="CS13" s="75"/>
+      <c r="CT13" s="75"/>
+      <c r="CU13" s="75"/>
+      <c r="CV13" s="75"/>
+      <c r="CW13" s="75"/>
+      <c r="CX13" s="75"/>
+      <c r="CY13" s="75"/>
+      <c r="CZ13" s="75"/>
+      <c r="DA13" s="75"/>
+      <c r="DB13" s="75"/>
+      <c r="DC13" s="75"/>
+      <c r="DD13" s="75"/>
+      <c r="DE13" s="75"/>
+      <c r="DF13" s="75"/>
+      <c r="DG13" s="75"/>
+      <c r="DH13" s="75"/>
+      <c r="DI13" s="75"/>
+      <c r="DJ13" s="75"/>
+      <c r="DK13" s="75"/>
+      <c r="DL13" s="75"/>
+      <c r="DM13" s="75"/>
+      <c r="DN13" s="75"/>
+      <c r="DO13" s="75"/>
+      <c r="DP13" s="75"/>
+      <c r="DQ13" s="75"/>
+      <c r="DR13" s="75"/>
+      <c r="DS13" s="75"/>
+      <c r="DT13" s="75"/>
+      <c r="DU13" s="75"/>
+      <c r="DV13" s="75"/>
+      <c r="DW13" s="75"/>
+      <c r="DX13" s="75"/>
+      <c r="DY13" s="75"/>
+      <c r="DZ13" s="75"/>
+      <c r="EA13" s="75"/>
+      <c r="EB13" s="75"/>
+      <c r="EC13" s="75"/>
+      <c r="ED13" s="75"/>
+      <c r="EE13" s="75"/>
+      <c r="EF13" s="75"/>
+      <c r="EG13" s="75"/>
+      <c r="EH13" s="75"/>
+      <c r="EI13" s="75"/>
+      <c r="EJ13" s="75"/>
+      <c r="EK13" s="75"/>
+      <c r="EL13" s="75"/>
+      <c r="EM13" s="75"/>
+      <c r="EN13" s="75"/>
+      <c r="EO13" s="75"/>
+      <c r="EP13" s="75"/>
+      <c r="EQ13" s="75"/>
+      <c r="ER13" s="75"/>
+      <c r="ES13" s="75"/>
+      <c r="ET13" s="75"/>
+      <c r="EU13" s="75"/>
+      <c r="EV13" s="75"/>
+      <c r="EW13" s="75"/>
+      <c r="EX13" s="75"/>
+      <c r="EY13" s="75"/>
+      <c r="EZ13" s="75"/>
+      <c r="FA13" s="75"/>
+      <c r="FB13" s="75"/>
+      <c r="FC13" s="75"/>
+      <c r="FD13" s="75"/>
+      <c r="FE13" s="75"/>
+      <c r="FF13" s="75"/>
+      <c r="FG13" s="75"/>
+      <c r="FH13" s="75"/>
+      <c r="FI13" s="75"/>
+      <c r="FJ13" s="75"/>
+      <c r="FK13" s="75"/>
+      <c r="FL13" s="75"/>
+      <c r="FM13" s="75"/>
+      <c r="FN13" s="75"/>
+      <c r="FO13" s="75"/>
+      <c r="FP13" s="75"/>
+      <c r="FQ13" s="75"/>
+      <c r="FR13" s="75"/>
+      <c r="FS13" s="75"/>
+      <c r="FT13" s="75"/>
+      <c r="FU13" s="75"/>
+      <c r="FV13" s="75"/>
+      <c r="FW13" s="75"/>
+      <c r="FX13" s="75"/>
+      <c r="FY13" s="75"/>
+      <c r="FZ13" s="75"/>
+      <c r="GA13" s="75"/>
+      <c r="GB13" s="75"/>
+      <c r="GC13" s="75"/>
+      <c r="GD13" s="75"/>
+      <c r="GE13" s="75"/>
+      <c r="GF13" s="75"/>
+      <c r="GG13" s="75"/>
+      <c r="GH13" s="75"/>
+      <c r="GI13" s="75"/>
+      <c r="GJ13" s="75"/>
+      <c r="GK13" s="75"/>
+      <c r="GL13" s="75"/>
+      <c r="GM13" s="75"/>
+      <c r="GN13" s="75"/>
+      <c r="GO13" s="75"/>
+      <c r="GP13" s="75"/>
+      <c r="GQ13" s="75"/>
+      <c r="GR13" s="75"/>
+      <c r="GS13" s="75"/>
+      <c r="GT13" s="75"/>
+      <c r="GU13" s="75"/>
+      <c r="GV13" s="75"/>
+      <c r="GW13" s="75"/>
+      <c r="GX13" s="75"/>
+      <c r="GY13" s="75"/>
+      <c r="GZ13" s="75"/>
+      <c r="HA13" s="75"/>
+      <c r="HB13" s="75"/>
+      <c r="HC13" s="75"/>
+      <c r="HD13" s="75"/>
+      <c r="HE13" s="75"/>
+      <c r="HF13" s="75"/>
+      <c r="HG13" s="75"/>
+      <c r="HH13" s="75"/>
+      <c r="HI13" s="75"/>
+      <c r="HJ13" s="75"/>
+      <c r="HK13" s="75"/>
+      <c r="HL13" s="75"/>
+      <c r="HM13" s="75"/>
+      <c r="HN13" s="75"/>
+      <c r="HO13" s="75"/>
+      <c r="HP13" s="75"/>
+      <c r="HQ13" s="75"/>
+      <c r="HR13" s="75"/>
+      <c r="HS13" s="75"/>
+      <c r="HT13" s="75"/>
+      <c r="HU13" s="75"/>
+      <c r="HV13" s="75"/>
+      <c r="HW13" s="75"/>
+      <c r="HX13" s="75"/>
+      <c r="HY13" s="75"/>
+      <c r="HZ13" s="75"/>
+      <c r="IA13" s="75"/>
+      <c r="IB13" s="75"/>
+      <c r="IC13" s="75"/>
+      <c r="ID13" s="75"/>
+      <c r="IE13" s="75"/>
+      <c r="IF13" s="75"/>
+      <c r="IG13" s="75"/>
+      <c r="IH13" s="75"/>
+      <c r="II13" s="75"/>
+      <c r="IJ13" s="75"/>
+      <c r="IK13" s="75"/>
+      <c r="IL13" s="75"/>
+      <c r="IM13" s="75"/>
+      <c r="IN13" s="75"/>
+      <c r="IO13" s="75"/>
+      <c r="IP13" s="75"/>
+      <c r="IQ13" s="75"/>
+      <c r="IR13" s="75"/>
+      <c r="IS13" s="75"/>
+      <c r="IT13" s="75"/>
+      <c r="IU13" s="75"/>
+      <c r="IV13" s="75"/>
+    </row>
+    <row r="14" spans="1:256" ht="15" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="10">
+        <v>42785</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="75"/>
+      <c r="N14" s="75"/>
+      <c r="O14" s="75"/>
+      <c r="P14" s="75"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="75"/>
+      <c r="S14" s="75"/>
+      <c r="T14" s="75"/>
+      <c r="U14" s="75"/>
+      <c r="V14" s="75"/>
+      <c r="W14" s="75"/>
+      <c r="X14" s="75"/>
+      <c r="Y14" s="75"/>
+      <c r="Z14" s="75"/>
+      <c r="AA14" s="75"/>
+      <c r="AB14" s="75"/>
+      <c r="AC14" s="75"/>
+      <c r="AD14" s="75"/>
+      <c r="AE14" s="75"/>
+      <c r="AF14" s="75"/>
+      <c r="AG14" s="75"/>
+      <c r="AH14" s="75"/>
+      <c r="AI14" s="75"/>
+      <c r="AJ14" s="75"/>
+      <c r="AK14" s="75"/>
+      <c r="AL14" s="75"/>
+      <c r="AM14" s="75"/>
+      <c r="AN14" s="75"/>
+      <c r="AO14" s="75"/>
+      <c r="AP14" s="75"/>
+      <c r="AQ14" s="75"/>
+      <c r="AR14" s="75"/>
+      <c r="AS14" s="75"/>
+      <c r="AT14" s="75"/>
+      <c r="AU14" s="75"/>
+      <c r="AV14" s="75"/>
+      <c r="AW14" s="75"/>
+      <c r="AX14" s="75"/>
+      <c r="AY14" s="75"/>
+      <c r="AZ14" s="75"/>
+      <c r="BA14" s="75"/>
+      <c r="BB14" s="75"/>
+      <c r="BC14" s="75"/>
+      <c r="BD14" s="75"/>
+      <c r="BE14" s="75"/>
+      <c r="BF14" s="75"/>
+      <c r="BG14" s="75"/>
+      <c r="BH14" s="75"/>
+      <c r="BI14" s="75"/>
+      <c r="BJ14" s="75"/>
+      <c r="BK14" s="75"/>
+      <c r="BL14" s="75"/>
+      <c r="BM14" s="75"/>
+      <c r="BN14" s="75"/>
+      <c r="BO14" s="75"/>
+      <c r="BP14" s="75"/>
+      <c r="BQ14" s="75"/>
+      <c r="BR14" s="75"/>
+      <c r="BS14" s="75"/>
+      <c r="BT14" s="75"/>
+      <c r="BU14" s="75"/>
+      <c r="BV14" s="75"/>
+      <c r="BW14" s="75"/>
+      <c r="BX14" s="75"/>
+      <c r="BY14" s="75"/>
+      <c r="BZ14" s="75"/>
+      <c r="CA14" s="75"/>
+      <c r="CB14" s="75"/>
+      <c r="CC14" s="75"/>
+      <c r="CD14" s="75"/>
+      <c r="CE14" s="75"/>
+      <c r="CF14" s="75"/>
+      <c r="CG14" s="75"/>
+      <c r="CH14" s="75"/>
+      <c r="CI14" s="75"/>
+      <c r="CJ14" s="75"/>
+      <c r="CK14" s="75"/>
+      <c r="CL14" s="75"/>
+      <c r="CM14" s="75"/>
+      <c r="CN14" s="75"/>
+      <c r="CO14" s="75"/>
+      <c r="CP14" s="75"/>
+      <c r="CQ14" s="75"/>
+      <c r="CR14" s="75"/>
+      <c r="CS14" s="75"/>
+      <c r="CT14" s="75"/>
+      <c r="CU14" s="75"/>
+      <c r="CV14" s="75"/>
+      <c r="CW14" s="75"/>
+      <c r="CX14" s="75"/>
+      <c r="CY14" s="75"/>
+      <c r="CZ14" s="75"/>
+      <c r="DA14" s="75"/>
+      <c r="DB14" s="75"/>
+      <c r="DC14" s="75"/>
+      <c r="DD14" s="75"/>
+      <c r="DE14" s="75"/>
+      <c r="DF14" s="75"/>
+      <c r="DG14" s="75"/>
+      <c r="DH14" s="75"/>
+      <c r="DI14" s="75"/>
+      <c r="DJ14" s="75"/>
+      <c r="DK14" s="75"/>
+      <c r="DL14" s="75"/>
+      <c r="DM14" s="75"/>
+      <c r="DN14" s="75"/>
+      <c r="DO14" s="75"/>
+      <c r="DP14" s="75"/>
+      <c r="DQ14" s="75"/>
+      <c r="DR14" s="75"/>
+      <c r="DS14" s="75"/>
+      <c r="DT14" s="75"/>
+      <c r="DU14" s="75"/>
+      <c r="DV14" s="75"/>
+      <c r="DW14" s="75"/>
+      <c r="DX14" s="75"/>
+      <c r="DY14" s="75"/>
+      <c r="DZ14" s="75"/>
+      <c r="EA14" s="75"/>
+      <c r="EB14" s="75"/>
+      <c r="EC14" s="75"/>
+      <c r="ED14" s="75"/>
+      <c r="EE14" s="75"/>
+      <c r="EF14" s="75"/>
+      <c r="EG14" s="75"/>
+      <c r="EH14" s="75"/>
+      <c r="EI14" s="75"/>
+      <c r="EJ14" s="75"/>
+      <c r="EK14" s="75"/>
+      <c r="EL14" s="75"/>
+      <c r="EM14" s="75"/>
+      <c r="EN14" s="75"/>
+      <c r="EO14" s="75"/>
+      <c r="EP14" s="75"/>
+      <c r="EQ14" s="75"/>
+      <c r="ER14" s="75"/>
+      <c r="ES14" s="75"/>
+      <c r="ET14" s="75"/>
+      <c r="EU14" s="75"/>
+      <c r="EV14" s="75"/>
+      <c r="EW14" s="75"/>
+      <c r="EX14" s="75"/>
+      <c r="EY14" s="75"/>
+      <c r="EZ14" s="75"/>
+      <c r="FA14" s="75"/>
+      <c r="FB14" s="75"/>
+      <c r="FC14" s="75"/>
+      <c r="FD14" s="75"/>
+      <c r="FE14" s="75"/>
+      <c r="FF14" s="75"/>
+      <c r="FG14" s="75"/>
+      <c r="FH14" s="75"/>
+      <c r="FI14" s="75"/>
+      <c r="FJ14" s="75"/>
+      <c r="FK14" s="75"/>
+      <c r="FL14" s="75"/>
+      <c r="FM14" s="75"/>
+      <c r="FN14" s="75"/>
+      <c r="FO14" s="75"/>
+      <c r="FP14" s="75"/>
+      <c r="FQ14" s="75"/>
+      <c r="FR14" s="75"/>
+      <c r="FS14" s="75"/>
+      <c r="FT14" s="75"/>
+      <c r="FU14" s="75"/>
+      <c r="FV14" s="75"/>
+      <c r="FW14" s="75"/>
+      <c r="FX14" s="75"/>
+      <c r="FY14" s="75"/>
+      <c r="FZ14" s="75"/>
+      <c r="GA14" s="75"/>
+      <c r="GB14" s="75"/>
+      <c r="GC14" s="75"/>
+      <c r="GD14" s="75"/>
+      <c r="GE14" s="75"/>
+      <c r="GF14" s="75"/>
+      <c r="GG14" s="75"/>
+      <c r="GH14" s="75"/>
+      <c r="GI14" s="75"/>
+      <c r="GJ14" s="75"/>
+      <c r="GK14" s="75"/>
+      <c r="GL14" s="75"/>
+      <c r="GM14" s="75"/>
+      <c r="GN14" s="75"/>
+      <c r="GO14" s="75"/>
+      <c r="GP14" s="75"/>
+      <c r="GQ14" s="75"/>
+      <c r="GR14" s="75"/>
+      <c r="GS14" s="75"/>
+      <c r="GT14" s="75"/>
+      <c r="GU14" s="75"/>
+      <c r="GV14" s="75"/>
+      <c r="GW14" s="75"/>
+      <c r="GX14" s="75"/>
+      <c r="GY14" s="75"/>
+      <c r="GZ14" s="75"/>
+      <c r="HA14" s="75"/>
+      <c r="HB14" s="75"/>
+      <c r="HC14" s="75"/>
+      <c r="HD14" s="75"/>
+      <c r="HE14" s="75"/>
+      <c r="HF14" s="75"/>
+      <c r="HG14" s="75"/>
+      <c r="HH14" s="75"/>
+      <c r="HI14" s="75"/>
+      <c r="HJ14" s="75"/>
+      <c r="HK14" s="75"/>
+      <c r="HL14" s="75"/>
+      <c r="HM14" s="75"/>
+      <c r="HN14" s="75"/>
+      <c r="HO14" s="75"/>
+      <c r="HP14" s="75"/>
+      <c r="HQ14" s="75"/>
+      <c r="HR14" s="75"/>
+      <c r="HS14" s="75"/>
+      <c r="HT14" s="75"/>
+      <c r="HU14" s="75"/>
+      <c r="HV14" s="75"/>
+      <c r="HW14" s="75"/>
+      <c r="HX14" s="75"/>
+      <c r="HY14" s="75"/>
+      <c r="HZ14" s="75"/>
+      <c r="IA14" s="75"/>
+      <c r="IB14" s="75"/>
+      <c r="IC14" s="75"/>
+      <c r="ID14" s="75"/>
+      <c r="IE14" s="75"/>
+      <c r="IF14" s="75"/>
+      <c r="IG14" s="75"/>
+      <c r="IH14" s="75"/>
+      <c r="II14" s="75"/>
+      <c r="IJ14" s="75"/>
+      <c r="IK14" s="75"/>
+      <c r="IL14" s="75"/>
+      <c r="IM14" s="75"/>
+      <c r="IN14" s="75"/>
+      <c r="IO14" s="75"/>
+      <c r="IP14" s="75"/>
+      <c r="IQ14" s="75"/>
+      <c r="IR14" s="75"/>
+      <c r="IS14" s="75"/>
+      <c r="IT14" s="75"/>
+      <c r="IU14" s="75"/>
+      <c r="IV14" s="75"/>
+    </row>
+    <row r="15" spans="1:256" ht="15" customHeight="1">
+      <c r="A15" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B15" s="10">
         <v>42785</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="A13" s="91" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="34"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
       <c r="H15" s="35"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="35"/>
+    <row r="16" spans="1:256" ht="15" customHeight="1">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:256" ht="15" customHeight="1">
-      <c r="A17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="35"/>
+      <c r="A17" s="97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:256" ht="15" customHeight="1">
-      <c r="A18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="35"/>
+      <c r="A18" s="100" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:256" ht="15" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="24"/>
@@ -2977,7 +3971,7 @@
     </row>
     <row r="20" spans="1:256" ht="15" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B20" s="23"/>
       <c r="C20" s="24"/>
@@ -2988,8 +3982,8 @@
       <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:256" ht="15" customHeight="1">
-      <c r="A21" s="97" t="s">
-        <v>111</v>
+      <c r="A21" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
@@ -2998,258 +3992,10 @@
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="35"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="75"/>
-      <c r="N21" s="75"/>
-      <c r="O21" s="75"/>
-      <c r="P21" s="75"/>
-      <c r="Q21" s="75"/>
-      <c r="R21" s="75"/>
-      <c r="S21" s="75"/>
-      <c r="T21" s="75"/>
-      <c r="U21" s="75"/>
-      <c r="V21" s="75"/>
-      <c r="W21" s="75"/>
-      <c r="X21" s="75"/>
-      <c r="Y21" s="75"/>
-      <c r="Z21" s="75"/>
-      <c r="AA21" s="75"/>
-      <c r="AB21" s="75"/>
-      <c r="AC21" s="75"/>
-      <c r="AD21" s="75"/>
-      <c r="AE21" s="75"/>
-      <c r="AF21" s="75"/>
-      <c r="AG21" s="75"/>
-      <c r="AH21" s="75"/>
-      <c r="AI21" s="75"/>
-      <c r="AJ21" s="75"/>
-      <c r="AK21" s="75"/>
-      <c r="AL21" s="75"/>
-      <c r="AM21" s="75"/>
-      <c r="AN21" s="75"/>
-      <c r="AO21" s="75"/>
-      <c r="AP21" s="75"/>
-      <c r="AQ21" s="75"/>
-      <c r="AR21" s="75"/>
-      <c r="AS21" s="75"/>
-      <c r="AT21" s="75"/>
-      <c r="AU21" s="75"/>
-      <c r="AV21" s="75"/>
-      <c r="AW21" s="75"/>
-      <c r="AX21" s="75"/>
-      <c r="AY21" s="75"/>
-      <c r="AZ21" s="75"/>
-      <c r="BA21" s="75"/>
-      <c r="BB21" s="75"/>
-      <c r="BC21" s="75"/>
-      <c r="BD21" s="75"/>
-      <c r="BE21" s="75"/>
-      <c r="BF21" s="75"/>
-      <c r="BG21" s="75"/>
-      <c r="BH21" s="75"/>
-      <c r="BI21" s="75"/>
-      <c r="BJ21" s="75"/>
-      <c r="BK21" s="75"/>
-      <c r="BL21" s="75"/>
-      <c r="BM21" s="75"/>
-      <c r="BN21" s="75"/>
-      <c r="BO21" s="75"/>
-      <c r="BP21" s="75"/>
-      <c r="BQ21" s="75"/>
-      <c r="BR21" s="75"/>
-      <c r="BS21" s="75"/>
-      <c r="BT21" s="75"/>
-      <c r="BU21" s="75"/>
-      <c r="BV21" s="75"/>
-      <c r="BW21" s="75"/>
-      <c r="BX21" s="75"/>
-      <c r="BY21" s="75"/>
-      <c r="BZ21" s="75"/>
-      <c r="CA21" s="75"/>
-      <c r="CB21" s="75"/>
-      <c r="CC21" s="75"/>
-      <c r="CD21" s="75"/>
-      <c r="CE21" s="75"/>
-      <c r="CF21" s="75"/>
-      <c r="CG21" s="75"/>
-      <c r="CH21" s="75"/>
-      <c r="CI21" s="75"/>
-      <c r="CJ21" s="75"/>
-      <c r="CK21" s="75"/>
-      <c r="CL21" s="75"/>
-      <c r="CM21" s="75"/>
-      <c r="CN21" s="75"/>
-      <c r="CO21" s="75"/>
-      <c r="CP21" s="75"/>
-      <c r="CQ21" s="75"/>
-      <c r="CR21" s="75"/>
-      <c r="CS21" s="75"/>
-      <c r="CT21" s="75"/>
-      <c r="CU21" s="75"/>
-      <c r="CV21" s="75"/>
-      <c r="CW21" s="75"/>
-      <c r="CX21" s="75"/>
-      <c r="CY21" s="75"/>
-      <c r="CZ21" s="75"/>
-      <c r="DA21" s="75"/>
-      <c r="DB21" s="75"/>
-      <c r="DC21" s="75"/>
-      <c r="DD21" s="75"/>
-      <c r="DE21" s="75"/>
-      <c r="DF21" s="75"/>
-      <c r="DG21" s="75"/>
-      <c r="DH21" s="75"/>
-      <c r="DI21" s="75"/>
-      <c r="DJ21" s="75"/>
-      <c r="DK21" s="75"/>
-      <c r="DL21" s="75"/>
-      <c r="DM21" s="75"/>
-      <c r="DN21" s="75"/>
-      <c r="DO21" s="75"/>
-      <c r="DP21" s="75"/>
-      <c r="DQ21" s="75"/>
-      <c r="DR21" s="75"/>
-      <c r="DS21" s="75"/>
-      <c r="DT21" s="75"/>
-      <c r="DU21" s="75"/>
-      <c r="DV21" s="75"/>
-      <c r="DW21" s="75"/>
-      <c r="DX21" s="75"/>
-      <c r="DY21" s="75"/>
-      <c r="DZ21" s="75"/>
-      <c r="EA21" s="75"/>
-      <c r="EB21" s="75"/>
-      <c r="EC21" s="75"/>
-      <c r="ED21" s="75"/>
-      <c r="EE21" s="75"/>
-      <c r="EF21" s="75"/>
-      <c r="EG21" s="75"/>
-      <c r="EH21" s="75"/>
-      <c r="EI21" s="75"/>
-      <c r="EJ21" s="75"/>
-      <c r="EK21" s="75"/>
-      <c r="EL21" s="75"/>
-      <c r="EM21" s="75"/>
-      <c r="EN21" s="75"/>
-      <c r="EO21" s="75"/>
-      <c r="EP21" s="75"/>
-      <c r="EQ21" s="75"/>
-      <c r="ER21" s="75"/>
-      <c r="ES21" s="75"/>
-      <c r="ET21" s="75"/>
-      <c r="EU21" s="75"/>
-      <c r="EV21" s="75"/>
-      <c r="EW21" s="75"/>
-      <c r="EX21" s="75"/>
-      <c r="EY21" s="75"/>
-      <c r="EZ21" s="75"/>
-      <c r="FA21" s="75"/>
-      <c r="FB21" s="75"/>
-      <c r="FC21" s="75"/>
-      <c r="FD21" s="75"/>
-      <c r="FE21" s="75"/>
-      <c r="FF21" s="75"/>
-      <c r="FG21" s="75"/>
-      <c r="FH21" s="75"/>
-      <c r="FI21" s="75"/>
-      <c r="FJ21" s="75"/>
-      <c r="FK21" s="75"/>
-      <c r="FL21" s="75"/>
-      <c r="FM21" s="75"/>
-      <c r="FN21" s="75"/>
-      <c r="FO21" s="75"/>
-      <c r="FP21" s="75"/>
-      <c r="FQ21" s="75"/>
-      <c r="FR21" s="75"/>
-      <c r="FS21" s="75"/>
-      <c r="FT21" s="75"/>
-      <c r="FU21" s="75"/>
-      <c r="FV21" s="75"/>
-      <c r="FW21" s="75"/>
-      <c r="FX21" s="75"/>
-      <c r="FY21" s="75"/>
-      <c r="FZ21" s="75"/>
-      <c r="GA21" s="75"/>
-      <c r="GB21" s="75"/>
-      <c r="GC21" s="75"/>
-      <c r="GD21" s="75"/>
-      <c r="GE21" s="75"/>
-      <c r="GF21" s="75"/>
-      <c r="GG21" s="75"/>
-      <c r="GH21" s="75"/>
-      <c r="GI21" s="75"/>
-      <c r="GJ21" s="75"/>
-      <c r="GK21" s="75"/>
-      <c r="GL21" s="75"/>
-      <c r="GM21" s="75"/>
-      <c r="GN21" s="75"/>
-      <c r="GO21" s="75"/>
-      <c r="GP21" s="75"/>
-      <c r="GQ21" s="75"/>
-      <c r="GR21" s="75"/>
-      <c r="GS21" s="75"/>
-      <c r="GT21" s="75"/>
-      <c r="GU21" s="75"/>
-      <c r="GV21" s="75"/>
-      <c r="GW21" s="75"/>
-      <c r="GX21" s="75"/>
-      <c r="GY21" s="75"/>
-      <c r="GZ21" s="75"/>
-      <c r="HA21" s="75"/>
-      <c r="HB21" s="75"/>
-      <c r="HC21" s="75"/>
-      <c r="HD21" s="75"/>
-      <c r="HE21" s="75"/>
-      <c r="HF21" s="75"/>
-      <c r="HG21" s="75"/>
-      <c r="HH21" s="75"/>
-      <c r="HI21" s="75"/>
-      <c r="HJ21" s="75"/>
-      <c r="HK21" s="75"/>
-      <c r="HL21" s="75"/>
-      <c r="HM21" s="75"/>
-      <c r="HN21" s="75"/>
-      <c r="HO21" s="75"/>
-      <c r="HP21" s="75"/>
-      <c r="HQ21" s="75"/>
-      <c r="HR21" s="75"/>
-      <c r="HS21" s="75"/>
-      <c r="HT21" s="75"/>
-      <c r="HU21" s="75"/>
-      <c r="HV21" s="75"/>
-      <c r="HW21" s="75"/>
-      <c r="HX21" s="75"/>
-      <c r="HY21" s="75"/>
-      <c r="HZ21" s="75"/>
-      <c r="IA21" s="75"/>
-      <c r="IB21" s="75"/>
-      <c r="IC21" s="75"/>
-      <c r="ID21" s="75"/>
-      <c r="IE21" s="75"/>
-      <c r="IF21" s="75"/>
-      <c r="IG21" s="75"/>
-      <c r="IH21" s="75"/>
-      <c r="II21" s="75"/>
-      <c r="IJ21" s="75"/>
-      <c r="IK21" s="75"/>
-      <c r="IL21" s="75"/>
-      <c r="IM21" s="75"/>
-      <c r="IN21" s="75"/>
-      <c r="IO21" s="75"/>
-      <c r="IP21" s="75"/>
-      <c r="IQ21" s="75"/>
-      <c r="IR21" s="75"/>
-      <c r="IS21" s="75"/>
-      <c r="IT21" s="75"/>
-      <c r="IU21" s="75"/>
-      <c r="IV21" s="75"/>
     </row>
     <row r="22" spans="1:256" ht="15" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B22" s="23"/>
       <c r="C22" s="24"/>
@@ -3261,7 +4007,7 @@
     </row>
     <row r="23" spans="1:256" ht="15" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="24"/>
@@ -3273,7 +4019,7 @@
     </row>
     <row r="24" spans="1:256" ht="15" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="24"/>
@@ -3284,8 +4030,8 @@
       <c r="H24" s="35"/>
     </row>
     <row r="25" spans="1:256" ht="15" customHeight="1">
-      <c r="A25" s="9" t="s">
-        <v>50</v>
+      <c r="A25" s="83" t="s">
+        <v>110</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="24"/>
@@ -3294,22 +4040,518 @@
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
       <c r="H25" s="35"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="75"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="75"/>
+      <c r="O25" s="75"/>
+      <c r="P25" s="75"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="75"/>
+      <c r="S25" s="75"/>
+      <c r="T25" s="75"/>
+      <c r="U25" s="75"/>
+      <c r="V25" s="75"/>
+      <c r="W25" s="75"/>
+      <c r="X25" s="75"/>
+      <c r="Y25" s="75"/>
+      <c r="Z25" s="75"/>
+      <c r="AA25" s="75"/>
+      <c r="AB25" s="75"/>
+      <c r="AC25" s="75"/>
+      <c r="AD25" s="75"/>
+      <c r="AE25" s="75"/>
+      <c r="AF25" s="75"/>
+      <c r="AG25" s="75"/>
+      <c r="AH25" s="75"/>
+      <c r="AI25" s="75"/>
+      <c r="AJ25" s="75"/>
+      <c r="AK25" s="75"/>
+      <c r="AL25" s="75"/>
+      <c r="AM25" s="75"/>
+      <c r="AN25" s="75"/>
+      <c r="AO25" s="75"/>
+      <c r="AP25" s="75"/>
+      <c r="AQ25" s="75"/>
+      <c r="AR25" s="75"/>
+      <c r="AS25" s="75"/>
+      <c r="AT25" s="75"/>
+      <c r="AU25" s="75"/>
+      <c r="AV25" s="75"/>
+      <c r="AW25" s="75"/>
+      <c r="AX25" s="75"/>
+      <c r="AY25" s="75"/>
+      <c r="AZ25" s="75"/>
+      <c r="BA25" s="75"/>
+      <c r="BB25" s="75"/>
+      <c r="BC25" s="75"/>
+      <c r="BD25" s="75"/>
+      <c r="BE25" s="75"/>
+      <c r="BF25" s="75"/>
+      <c r="BG25" s="75"/>
+      <c r="BH25" s="75"/>
+      <c r="BI25" s="75"/>
+      <c r="BJ25" s="75"/>
+      <c r="BK25" s="75"/>
+      <c r="BL25" s="75"/>
+      <c r="BM25" s="75"/>
+      <c r="BN25" s="75"/>
+      <c r="BO25" s="75"/>
+      <c r="BP25" s="75"/>
+      <c r="BQ25" s="75"/>
+      <c r="BR25" s="75"/>
+      <c r="BS25" s="75"/>
+      <c r="BT25" s="75"/>
+      <c r="BU25" s="75"/>
+      <c r="BV25" s="75"/>
+      <c r="BW25" s="75"/>
+      <c r="BX25" s="75"/>
+      <c r="BY25" s="75"/>
+      <c r="BZ25" s="75"/>
+      <c r="CA25" s="75"/>
+      <c r="CB25" s="75"/>
+      <c r="CC25" s="75"/>
+      <c r="CD25" s="75"/>
+      <c r="CE25" s="75"/>
+      <c r="CF25" s="75"/>
+      <c r="CG25" s="75"/>
+      <c r="CH25" s="75"/>
+      <c r="CI25" s="75"/>
+      <c r="CJ25" s="75"/>
+      <c r="CK25" s="75"/>
+      <c r="CL25" s="75"/>
+      <c r="CM25" s="75"/>
+      <c r="CN25" s="75"/>
+      <c r="CO25" s="75"/>
+      <c r="CP25" s="75"/>
+      <c r="CQ25" s="75"/>
+      <c r="CR25" s="75"/>
+      <c r="CS25" s="75"/>
+      <c r="CT25" s="75"/>
+      <c r="CU25" s="75"/>
+      <c r="CV25" s="75"/>
+      <c r="CW25" s="75"/>
+      <c r="CX25" s="75"/>
+      <c r="CY25" s="75"/>
+      <c r="CZ25" s="75"/>
+      <c r="DA25" s="75"/>
+      <c r="DB25" s="75"/>
+      <c r="DC25" s="75"/>
+      <c r="DD25" s="75"/>
+      <c r="DE25" s="75"/>
+      <c r="DF25" s="75"/>
+      <c r="DG25" s="75"/>
+      <c r="DH25" s="75"/>
+      <c r="DI25" s="75"/>
+      <c r="DJ25" s="75"/>
+      <c r="DK25" s="75"/>
+      <c r="DL25" s="75"/>
+      <c r="DM25" s="75"/>
+      <c r="DN25" s="75"/>
+      <c r="DO25" s="75"/>
+      <c r="DP25" s="75"/>
+      <c r="DQ25" s="75"/>
+      <c r="DR25" s="75"/>
+      <c r="DS25" s="75"/>
+      <c r="DT25" s="75"/>
+      <c r="DU25" s="75"/>
+      <c r="DV25" s="75"/>
+      <c r="DW25" s="75"/>
+      <c r="DX25" s="75"/>
+      <c r="DY25" s="75"/>
+      <c r="DZ25" s="75"/>
+      <c r="EA25" s="75"/>
+      <c r="EB25" s="75"/>
+      <c r="EC25" s="75"/>
+      <c r="ED25" s="75"/>
+      <c r="EE25" s="75"/>
+      <c r="EF25" s="75"/>
+      <c r="EG25" s="75"/>
+      <c r="EH25" s="75"/>
+      <c r="EI25" s="75"/>
+      <c r="EJ25" s="75"/>
+      <c r="EK25" s="75"/>
+      <c r="EL25" s="75"/>
+      <c r="EM25" s="75"/>
+      <c r="EN25" s="75"/>
+      <c r="EO25" s="75"/>
+      <c r="EP25" s="75"/>
+      <c r="EQ25" s="75"/>
+      <c r="ER25" s="75"/>
+      <c r="ES25" s="75"/>
+      <c r="ET25" s="75"/>
+      <c r="EU25" s="75"/>
+      <c r="EV25" s="75"/>
+      <c r="EW25" s="75"/>
+      <c r="EX25" s="75"/>
+      <c r="EY25" s="75"/>
+      <c r="EZ25" s="75"/>
+      <c r="FA25" s="75"/>
+      <c r="FB25" s="75"/>
+      <c r="FC25" s="75"/>
+      <c r="FD25" s="75"/>
+      <c r="FE25" s="75"/>
+      <c r="FF25" s="75"/>
+      <c r="FG25" s="75"/>
+      <c r="FH25" s="75"/>
+      <c r="FI25" s="75"/>
+      <c r="FJ25" s="75"/>
+      <c r="FK25" s="75"/>
+      <c r="FL25" s="75"/>
+      <c r="FM25" s="75"/>
+      <c r="FN25" s="75"/>
+      <c r="FO25" s="75"/>
+      <c r="FP25" s="75"/>
+      <c r="FQ25" s="75"/>
+      <c r="FR25" s="75"/>
+      <c r="FS25" s="75"/>
+      <c r="FT25" s="75"/>
+      <c r="FU25" s="75"/>
+      <c r="FV25" s="75"/>
+      <c r="FW25" s="75"/>
+      <c r="FX25" s="75"/>
+      <c r="FY25" s="75"/>
+      <c r="FZ25" s="75"/>
+      <c r="GA25" s="75"/>
+      <c r="GB25" s="75"/>
+      <c r="GC25" s="75"/>
+      <c r="GD25" s="75"/>
+      <c r="GE25" s="75"/>
+      <c r="GF25" s="75"/>
+      <c r="GG25" s="75"/>
+      <c r="GH25" s="75"/>
+      <c r="GI25" s="75"/>
+      <c r="GJ25" s="75"/>
+      <c r="GK25" s="75"/>
+      <c r="GL25" s="75"/>
+      <c r="GM25" s="75"/>
+      <c r="GN25" s="75"/>
+      <c r="GO25" s="75"/>
+      <c r="GP25" s="75"/>
+      <c r="GQ25" s="75"/>
+      <c r="GR25" s="75"/>
+      <c r="GS25" s="75"/>
+      <c r="GT25" s="75"/>
+      <c r="GU25" s="75"/>
+      <c r="GV25" s="75"/>
+      <c r="GW25" s="75"/>
+      <c r="GX25" s="75"/>
+      <c r="GY25" s="75"/>
+      <c r="GZ25" s="75"/>
+      <c r="HA25" s="75"/>
+      <c r="HB25" s="75"/>
+      <c r="HC25" s="75"/>
+      <c r="HD25" s="75"/>
+      <c r="HE25" s="75"/>
+      <c r="HF25" s="75"/>
+      <c r="HG25" s="75"/>
+      <c r="HH25" s="75"/>
+      <c r="HI25" s="75"/>
+      <c r="HJ25" s="75"/>
+      <c r="HK25" s="75"/>
+      <c r="HL25" s="75"/>
+      <c r="HM25" s="75"/>
+      <c r="HN25" s="75"/>
+      <c r="HO25" s="75"/>
+      <c r="HP25" s="75"/>
+      <c r="HQ25" s="75"/>
+      <c r="HR25" s="75"/>
+      <c r="HS25" s="75"/>
+      <c r="HT25" s="75"/>
+      <c r="HU25" s="75"/>
+      <c r="HV25" s="75"/>
+      <c r="HW25" s="75"/>
+      <c r="HX25" s="75"/>
+      <c r="HY25" s="75"/>
+      <c r="HZ25" s="75"/>
+      <c r="IA25" s="75"/>
+      <c r="IB25" s="75"/>
+      <c r="IC25" s="75"/>
+      <c r="ID25" s="75"/>
+      <c r="IE25" s="75"/>
+      <c r="IF25" s="75"/>
+      <c r="IG25" s="75"/>
+      <c r="IH25" s="75"/>
+      <c r="II25" s="75"/>
+      <c r="IJ25" s="75"/>
+      <c r="IK25" s="75"/>
+      <c r="IL25" s="75"/>
+      <c r="IM25" s="75"/>
+      <c r="IN25" s="75"/>
+      <c r="IO25" s="75"/>
+      <c r="IP25" s="75"/>
+      <c r="IQ25" s="75"/>
+      <c r="IR25" s="75"/>
+      <c r="IS25" s="75"/>
+      <c r="IT25" s="75"/>
+      <c r="IU25" s="75"/>
+      <c r="IV25" s="75"/>
     </row>
     <row r="26" spans="1:256" ht="15" customHeight="1">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="81"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="82"/>
       <c r="H26" s="35"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="75"/>
+      <c r="O26" s="75"/>
+      <c r="P26" s="75"/>
+      <c r="Q26" s="75"/>
+      <c r="R26" s="75"/>
+      <c r="S26" s="75"/>
+      <c r="T26" s="75"/>
+      <c r="U26" s="75"/>
+      <c r="V26" s="75"/>
+      <c r="W26" s="75"/>
+      <c r="X26" s="75"/>
+      <c r="Y26" s="75"/>
+      <c r="Z26" s="75"/>
+      <c r="AA26" s="75"/>
+      <c r="AB26" s="75"/>
+      <c r="AC26" s="75"/>
+      <c r="AD26" s="75"/>
+      <c r="AE26" s="75"/>
+      <c r="AF26" s="75"/>
+      <c r="AG26" s="75"/>
+      <c r="AH26" s="75"/>
+      <c r="AI26" s="75"/>
+      <c r="AJ26" s="75"/>
+      <c r="AK26" s="75"/>
+      <c r="AL26" s="75"/>
+      <c r="AM26" s="75"/>
+      <c r="AN26" s="75"/>
+      <c r="AO26" s="75"/>
+      <c r="AP26" s="75"/>
+      <c r="AQ26" s="75"/>
+      <c r="AR26" s="75"/>
+      <c r="AS26" s="75"/>
+      <c r="AT26" s="75"/>
+      <c r="AU26" s="75"/>
+      <c r="AV26" s="75"/>
+      <c r="AW26" s="75"/>
+      <c r="AX26" s="75"/>
+      <c r="AY26" s="75"/>
+      <c r="AZ26" s="75"/>
+      <c r="BA26" s="75"/>
+      <c r="BB26" s="75"/>
+      <c r="BC26" s="75"/>
+      <c r="BD26" s="75"/>
+      <c r="BE26" s="75"/>
+      <c r="BF26" s="75"/>
+      <c r="BG26" s="75"/>
+      <c r="BH26" s="75"/>
+      <c r="BI26" s="75"/>
+      <c r="BJ26" s="75"/>
+      <c r="BK26" s="75"/>
+      <c r="BL26" s="75"/>
+      <c r="BM26" s="75"/>
+      <c r="BN26" s="75"/>
+      <c r="BO26" s="75"/>
+      <c r="BP26" s="75"/>
+      <c r="BQ26" s="75"/>
+      <c r="BR26" s="75"/>
+      <c r="BS26" s="75"/>
+      <c r="BT26" s="75"/>
+      <c r="BU26" s="75"/>
+      <c r="BV26" s="75"/>
+      <c r="BW26" s="75"/>
+      <c r="BX26" s="75"/>
+      <c r="BY26" s="75"/>
+      <c r="BZ26" s="75"/>
+      <c r="CA26" s="75"/>
+      <c r="CB26" s="75"/>
+      <c r="CC26" s="75"/>
+      <c r="CD26" s="75"/>
+      <c r="CE26" s="75"/>
+      <c r="CF26" s="75"/>
+      <c r="CG26" s="75"/>
+      <c r="CH26" s="75"/>
+      <c r="CI26" s="75"/>
+      <c r="CJ26" s="75"/>
+      <c r="CK26" s="75"/>
+      <c r="CL26" s="75"/>
+      <c r="CM26" s="75"/>
+      <c r="CN26" s="75"/>
+      <c r="CO26" s="75"/>
+      <c r="CP26" s="75"/>
+      <c r="CQ26" s="75"/>
+      <c r="CR26" s="75"/>
+      <c r="CS26" s="75"/>
+      <c r="CT26" s="75"/>
+      <c r="CU26" s="75"/>
+      <c r="CV26" s="75"/>
+      <c r="CW26" s="75"/>
+      <c r="CX26" s="75"/>
+      <c r="CY26" s="75"/>
+      <c r="CZ26" s="75"/>
+      <c r="DA26" s="75"/>
+      <c r="DB26" s="75"/>
+      <c r="DC26" s="75"/>
+      <c r="DD26" s="75"/>
+      <c r="DE26" s="75"/>
+      <c r="DF26" s="75"/>
+      <c r="DG26" s="75"/>
+      <c r="DH26" s="75"/>
+      <c r="DI26" s="75"/>
+      <c r="DJ26" s="75"/>
+      <c r="DK26" s="75"/>
+      <c r="DL26" s="75"/>
+      <c r="DM26" s="75"/>
+      <c r="DN26" s="75"/>
+      <c r="DO26" s="75"/>
+      <c r="DP26" s="75"/>
+      <c r="DQ26" s="75"/>
+      <c r="DR26" s="75"/>
+      <c r="DS26" s="75"/>
+      <c r="DT26" s="75"/>
+      <c r="DU26" s="75"/>
+      <c r="DV26" s="75"/>
+      <c r="DW26" s="75"/>
+      <c r="DX26" s="75"/>
+      <c r="DY26" s="75"/>
+      <c r="DZ26" s="75"/>
+      <c r="EA26" s="75"/>
+      <c r="EB26" s="75"/>
+      <c r="EC26" s="75"/>
+      <c r="ED26" s="75"/>
+      <c r="EE26" s="75"/>
+      <c r="EF26" s="75"/>
+      <c r="EG26" s="75"/>
+      <c r="EH26" s="75"/>
+      <c r="EI26" s="75"/>
+      <c r="EJ26" s="75"/>
+      <c r="EK26" s="75"/>
+      <c r="EL26" s="75"/>
+      <c r="EM26" s="75"/>
+      <c r="EN26" s="75"/>
+      <c r="EO26" s="75"/>
+      <c r="EP26" s="75"/>
+      <c r="EQ26" s="75"/>
+      <c r="ER26" s="75"/>
+      <c r="ES26" s="75"/>
+      <c r="ET26" s="75"/>
+      <c r="EU26" s="75"/>
+      <c r="EV26" s="75"/>
+      <c r="EW26" s="75"/>
+      <c r="EX26" s="75"/>
+      <c r="EY26" s="75"/>
+      <c r="EZ26" s="75"/>
+      <c r="FA26" s="75"/>
+      <c r="FB26" s="75"/>
+      <c r="FC26" s="75"/>
+      <c r="FD26" s="75"/>
+      <c r="FE26" s="75"/>
+      <c r="FF26" s="75"/>
+      <c r="FG26" s="75"/>
+      <c r="FH26" s="75"/>
+      <c r="FI26" s="75"/>
+      <c r="FJ26" s="75"/>
+      <c r="FK26" s="75"/>
+      <c r="FL26" s="75"/>
+      <c r="FM26" s="75"/>
+      <c r="FN26" s="75"/>
+      <c r="FO26" s="75"/>
+      <c r="FP26" s="75"/>
+      <c r="FQ26" s="75"/>
+      <c r="FR26" s="75"/>
+      <c r="FS26" s="75"/>
+      <c r="FT26" s="75"/>
+      <c r="FU26" s="75"/>
+      <c r="FV26" s="75"/>
+      <c r="FW26" s="75"/>
+      <c r="FX26" s="75"/>
+      <c r="FY26" s="75"/>
+      <c r="FZ26" s="75"/>
+      <c r="GA26" s="75"/>
+      <c r="GB26" s="75"/>
+      <c r="GC26" s="75"/>
+      <c r="GD26" s="75"/>
+      <c r="GE26" s="75"/>
+      <c r="GF26" s="75"/>
+      <c r="GG26" s="75"/>
+      <c r="GH26" s="75"/>
+      <c r="GI26" s="75"/>
+      <c r="GJ26" s="75"/>
+      <c r="GK26" s="75"/>
+      <c r="GL26" s="75"/>
+      <c r="GM26" s="75"/>
+      <c r="GN26" s="75"/>
+      <c r="GO26" s="75"/>
+      <c r="GP26" s="75"/>
+      <c r="GQ26" s="75"/>
+      <c r="GR26" s="75"/>
+      <c r="GS26" s="75"/>
+      <c r="GT26" s="75"/>
+      <c r="GU26" s="75"/>
+      <c r="GV26" s="75"/>
+      <c r="GW26" s="75"/>
+      <c r="GX26" s="75"/>
+      <c r="GY26" s="75"/>
+      <c r="GZ26" s="75"/>
+      <c r="HA26" s="75"/>
+      <c r="HB26" s="75"/>
+      <c r="HC26" s="75"/>
+      <c r="HD26" s="75"/>
+      <c r="HE26" s="75"/>
+      <c r="HF26" s="75"/>
+      <c r="HG26" s="75"/>
+      <c r="HH26" s="75"/>
+      <c r="HI26" s="75"/>
+      <c r="HJ26" s="75"/>
+      <c r="HK26" s="75"/>
+      <c r="HL26" s="75"/>
+      <c r="HM26" s="75"/>
+      <c r="HN26" s="75"/>
+      <c r="HO26" s="75"/>
+      <c r="HP26" s="75"/>
+      <c r="HQ26" s="75"/>
+      <c r="HR26" s="75"/>
+      <c r="HS26" s="75"/>
+      <c r="HT26" s="75"/>
+      <c r="HU26" s="75"/>
+      <c r="HV26" s="75"/>
+      <c r="HW26" s="75"/>
+      <c r="HX26" s="75"/>
+      <c r="HY26" s="75"/>
+      <c r="HZ26" s="75"/>
+      <c r="IA26" s="75"/>
+      <c r="IB26" s="75"/>
+      <c r="IC26" s="75"/>
+      <c r="ID26" s="75"/>
+      <c r="IE26" s="75"/>
+      <c r="IF26" s="75"/>
+      <c r="IG26" s="75"/>
+      <c r="IH26" s="75"/>
+      <c r="II26" s="75"/>
+      <c r="IJ26" s="75"/>
+      <c r="IK26" s="75"/>
+      <c r="IL26" s="75"/>
+      <c r="IM26" s="75"/>
+      <c r="IN26" s="75"/>
+      <c r="IO26" s="75"/>
+      <c r="IP26" s="75"/>
+      <c r="IQ26" s="75"/>
+      <c r="IR26" s="75"/>
+      <c r="IS26" s="75"/>
+      <c r="IT26" s="75"/>
+      <c r="IU26" s="75"/>
+      <c r="IV26" s="75"/>
     </row>
     <row r="27" spans="1:256" ht="15" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="24"/>
@@ -3320,31 +4562,35 @@
       <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:256" ht="15" customHeight="1">
-      <c r="A28" s="15"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="8"/>
+      <c r="A28" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="35"/>
     </row>
     <row r="29" spans="1:256" ht="15" customHeight="1">
-      <c r="A29" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="18"/>
+      <c r="A29" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="34"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
       <c r="H29" s="35"/>
     </row>
     <row r="30" spans="1:256" ht="15" customHeight="1">
-      <c r="A30" s="29"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
+      <c r="A30" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="34"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
@@ -3352,45 +4598,573 @@
       <c r="H30" s="35"/>
     </row>
     <row r="31" spans="1:256" ht="15" customHeight="1">
-      <c r="A31" s="30"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="35"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:256" ht="15" customHeight="1">
-      <c r="A32" s="80" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="81"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="34"/>
+      <c r="A32" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
       <c r="H32" s="35"/>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1">
-      <c r="A33" s="87" t="s">
+    <row r="33" spans="1:256" ht="15" customHeight="1">
+      <c r="A33" s="29"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="35"/>
+    </row>
+    <row r="34" spans="1:256" ht="15" customHeight="1">
+      <c r="A34" s="30"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="35"/>
+    </row>
+    <row r="35" spans="1:256" ht="15" customHeight="1">
+      <c r="A35" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="87"/>
+      <c r="C35" s="88"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+      <c r="AB35"/>
+      <c r="AC35"/>
+      <c r="AD35"/>
+      <c r="AE35"/>
+      <c r="AF35"/>
+      <c r="AG35"/>
+      <c r="AH35"/>
+      <c r="AI35"/>
+      <c r="AJ35"/>
+      <c r="AK35"/>
+      <c r="AL35"/>
+      <c r="AM35"/>
+      <c r="AN35"/>
+      <c r="AO35"/>
+      <c r="AP35"/>
+      <c r="AQ35"/>
+      <c r="AR35"/>
+      <c r="AS35"/>
+      <c r="AT35"/>
+      <c r="AU35"/>
+      <c r="AV35"/>
+      <c r="AW35"/>
+      <c r="AX35"/>
+      <c r="AY35"/>
+      <c r="AZ35"/>
+      <c r="BA35"/>
+      <c r="BB35"/>
+      <c r="BC35"/>
+      <c r="BD35"/>
+      <c r="BE35"/>
+      <c r="BF35"/>
+      <c r="BG35"/>
+      <c r="BH35"/>
+      <c r="BI35"/>
+      <c r="BJ35"/>
+      <c r="BK35"/>
+      <c r="BL35"/>
+      <c r="BM35"/>
+      <c r="BN35"/>
+      <c r="BO35"/>
+      <c r="BP35"/>
+      <c r="BQ35"/>
+      <c r="BR35"/>
+      <c r="BS35"/>
+      <c r="BT35"/>
+      <c r="BU35"/>
+      <c r="BV35"/>
+      <c r="BW35"/>
+      <c r="BX35"/>
+      <c r="BY35"/>
+      <c r="BZ35"/>
+      <c r="CA35"/>
+      <c r="CB35"/>
+      <c r="CC35"/>
+      <c r="CD35"/>
+      <c r="CE35"/>
+      <c r="CF35"/>
+      <c r="CG35"/>
+      <c r="CH35"/>
+      <c r="CI35"/>
+      <c r="CJ35"/>
+      <c r="CK35"/>
+      <c r="CL35"/>
+      <c r="CM35"/>
+      <c r="CN35"/>
+      <c r="CO35"/>
+      <c r="CP35"/>
+      <c r="CQ35"/>
+      <c r="CR35"/>
+      <c r="CS35"/>
+      <c r="CT35"/>
+      <c r="CU35"/>
+      <c r="CV35"/>
+      <c r="CW35"/>
+      <c r="CX35"/>
+      <c r="CY35"/>
+      <c r="CZ35"/>
+      <c r="DA35"/>
+      <c r="DB35"/>
+      <c r="DC35"/>
+      <c r="DD35"/>
+      <c r="DE35"/>
+      <c r="DF35"/>
+      <c r="DG35"/>
+      <c r="DH35"/>
+      <c r="DI35"/>
+      <c r="DJ35"/>
+      <c r="DK35"/>
+      <c r="DL35"/>
+      <c r="DM35"/>
+      <c r="DN35"/>
+      <c r="DO35"/>
+      <c r="DP35"/>
+      <c r="DQ35"/>
+      <c r="DR35"/>
+      <c r="DS35"/>
+      <c r="DT35"/>
+      <c r="DU35"/>
+      <c r="DV35"/>
+      <c r="DW35"/>
+      <c r="DX35"/>
+      <c r="DY35"/>
+      <c r="DZ35"/>
+      <c r="EA35"/>
+      <c r="EB35"/>
+      <c r="EC35"/>
+      <c r="ED35"/>
+      <c r="EE35"/>
+      <c r="EF35"/>
+      <c r="EG35"/>
+      <c r="EH35"/>
+      <c r="EI35"/>
+      <c r="EJ35"/>
+      <c r="EK35"/>
+      <c r="EL35"/>
+      <c r="EM35"/>
+      <c r="EN35"/>
+      <c r="EO35"/>
+      <c r="EP35"/>
+      <c r="EQ35"/>
+      <c r="ER35"/>
+      <c r="ES35"/>
+      <c r="ET35"/>
+      <c r="EU35"/>
+      <c r="EV35"/>
+      <c r="EW35"/>
+      <c r="EX35"/>
+      <c r="EY35"/>
+      <c r="EZ35"/>
+      <c r="FA35"/>
+      <c r="FB35"/>
+      <c r="FC35"/>
+      <c r="FD35"/>
+      <c r="FE35"/>
+      <c r="FF35"/>
+      <c r="FG35"/>
+      <c r="FH35"/>
+      <c r="FI35"/>
+      <c r="FJ35"/>
+      <c r="FK35"/>
+      <c r="FL35"/>
+      <c r="FM35"/>
+      <c r="FN35"/>
+      <c r="FO35"/>
+      <c r="FP35"/>
+      <c r="FQ35"/>
+      <c r="FR35"/>
+      <c r="FS35"/>
+      <c r="FT35"/>
+      <c r="FU35"/>
+      <c r="FV35"/>
+      <c r="FW35"/>
+      <c r="FX35"/>
+      <c r="FY35"/>
+      <c r="FZ35"/>
+      <c r="GA35"/>
+      <c r="GB35"/>
+      <c r="GC35"/>
+      <c r="GD35"/>
+      <c r="GE35"/>
+      <c r="GF35"/>
+      <c r="GG35"/>
+      <c r="GH35"/>
+      <c r="GI35"/>
+      <c r="GJ35"/>
+      <c r="GK35"/>
+      <c r="GL35"/>
+      <c r="GM35"/>
+      <c r="GN35"/>
+      <c r="GO35"/>
+      <c r="GP35"/>
+      <c r="GQ35"/>
+      <c r="GR35"/>
+      <c r="GS35"/>
+      <c r="GT35"/>
+      <c r="GU35"/>
+      <c r="GV35"/>
+      <c r="GW35"/>
+      <c r="GX35"/>
+      <c r="GY35"/>
+      <c r="GZ35"/>
+      <c r="HA35"/>
+      <c r="HB35"/>
+      <c r="HC35"/>
+      <c r="HD35"/>
+      <c r="HE35"/>
+      <c r="HF35"/>
+      <c r="HG35"/>
+      <c r="HH35"/>
+      <c r="HI35"/>
+      <c r="HJ35"/>
+      <c r="HK35"/>
+      <c r="HL35"/>
+      <c r="HM35"/>
+      <c r="HN35"/>
+      <c r="HO35"/>
+      <c r="HP35"/>
+      <c r="HQ35"/>
+      <c r="HR35"/>
+      <c r="HS35"/>
+      <c r="HT35"/>
+      <c r="HU35"/>
+      <c r="HV35"/>
+      <c r="HW35"/>
+      <c r="HX35"/>
+      <c r="HY35"/>
+      <c r="HZ35"/>
+      <c r="IA35"/>
+      <c r="IB35"/>
+      <c r="IC35"/>
+      <c r="ID35"/>
+      <c r="IE35"/>
+      <c r="IF35"/>
+      <c r="IG35"/>
+      <c r="IH35"/>
+      <c r="II35"/>
+      <c r="IJ35"/>
+      <c r="IK35"/>
+      <c r="IL35"/>
+      <c r="IM35"/>
+      <c r="IN35"/>
+      <c r="IO35"/>
+      <c r="IP35"/>
+      <c r="IQ35"/>
+      <c r="IR35"/>
+      <c r="IS35"/>
+      <c r="IT35"/>
+      <c r="IU35"/>
+      <c r="IV35"/>
+    </row>
+    <row r="36" spans="1:256" ht="15" customHeight="1">
+      <c r="A36" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="88"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="42"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="42"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AJ36"/>
+      <c r="AK36"/>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+      <c r="AR36"/>
+      <c r="AS36"/>
+      <c r="AT36"/>
+      <c r="AU36"/>
+      <c r="AV36"/>
+      <c r="AW36"/>
+      <c r="AX36"/>
+      <c r="AY36"/>
+      <c r="AZ36"/>
+      <c r="BA36"/>
+      <c r="BB36"/>
+      <c r="BC36"/>
+      <c r="BD36"/>
+      <c r="BE36"/>
+      <c r="BF36"/>
+      <c r="BG36"/>
+      <c r="BH36"/>
+      <c r="BI36"/>
+      <c r="BJ36"/>
+      <c r="BK36"/>
+      <c r="BL36"/>
+      <c r="BM36"/>
+      <c r="BN36"/>
+      <c r="BO36"/>
+      <c r="BP36"/>
+      <c r="BQ36"/>
+      <c r="BR36"/>
+      <c r="BS36"/>
+      <c r="BT36"/>
+      <c r="BU36"/>
+      <c r="BV36"/>
+      <c r="BW36"/>
+      <c r="BX36"/>
+      <c r="BY36"/>
+      <c r="BZ36"/>
+      <c r="CA36"/>
+      <c r="CB36"/>
+      <c r="CC36"/>
+      <c r="CD36"/>
+      <c r="CE36"/>
+      <c r="CF36"/>
+      <c r="CG36"/>
+      <c r="CH36"/>
+      <c r="CI36"/>
+      <c r="CJ36"/>
+      <c r="CK36"/>
+      <c r="CL36"/>
+      <c r="CM36"/>
+      <c r="CN36"/>
+      <c r="CO36"/>
+      <c r="CP36"/>
+      <c r="CQ36"/>
+      <c r="CR36"/>
+      <c r="CS36"/>
+      <c r="CT36"/>
+      <c r="CU36"/>
+      <c r="CV36"/>
+      <c r="CW36"/>
+      <c r="CX36"/>
+      <c r="CY36"/>
+      <c r="CZ36"/>
+      <c r="DA36"/>
+      <c r="DB36"/>
+      <c r="DC36"/>
+      <c r="DD36"/>
+      <c r="DE36"/>
+      <c r="DF36"/>
+      <c r="DG36"/>
+      <c r="DH36"/>
+      <c r="DI36"/>
+      <c r="DJ36"/>
+      <c r="DK36"/>
+      <c r="DL36"/>
+      <c r="DM36"/>
+      <c r="DN36"/>
+      <c r="DO36"/>
+      <c r="DP36"/>
+      <c r="DQ36"/>
+      <c r="DR36"/>
+      <c r="DS36"/>
+      <c r="DT36"/>
+      <c r="DU36"/>
+      <c r="DV36"/>
+      <c r="DW36"/>
+      <c r="DX36"/>
+      <c r="DY36"/>
+      <c r="DZ36"/>
+      <c r="EA36"/>
+      <c r="EB36"/>
+      <c r="EC36"/>
+      <c r="ED36"/>
+      <c r="EE36"/>
+      <c r="EF36"/>
+      <c r="EG36"/>
+      <c r="EH36"/>
+      <c r="EI36"/>
+      <c r="EJ36"/>
+      <c r="EK36"/>
+      <c r="EL36"/>
+      <c r="EM36"/>
+      <c r="EN36"/>
+      <c r="EO36"/>
+      <c r="EP36"/>
+      <c r="EQ36"/>
+      <c r="ER36"/>
+      <c r="ES36"/>
+      <c r="ET36"/>
+      <c r="EU36"/>
+      <c r="EV36"/>
+      <c r="EW36"/>
+      <c r="EX36"/>
+      <c r="EY36"/>
+      <c r="EZ36"/>
+      <c r="FA36"/>
+      <c r="FB36"/>
+      <c r="FC36"/>
+      <c r="FD36"/>
+      <c r="FE36"/>
+      <c r="FF36"/>
+      <c r="FG36"/>
+      <c r="FH36"/>
+      <c r="FI36"/>
+      <c r="FJ36"/>
+      <c r="FK36"/>
+      <c r="FL36"/>
+      <c r="FM36"/>
+      <c r="FN36"/>
+      <c r="FO36"/>
+      <c r="FP36"/>
+      <c r="FQ36"/>
+      <c r="FR36"/>
+      <c r="FS36"/>
+      <c r="FT36"/>
+      <c r="FU36"/>
+      <c r="FV36"/>
+      <c r="FW36"/>
+      <c r="FX36"/>
+      <c r="FY36"/>
+      <c r="FZ36"/>
+      <c r="GA36"/>
+      <c r="GB36"/>
+      <c r="GC36"/>
+      <c r="GD36"/>
+      <c r="GE36"/>
+      <c r="GF36"/>
+      <c r="GG36"/>
+      <c r="GH36"/>
+      <c r="GI36"/>
+      <c r="GJ36"/>
+      <c r="GK36"/>
+      <c r="GL36"/>
+      <c r="GM36"/>
+      <c r="GN36"/>
+      <c r="GO36"/>
+      <c r="GP36"/>
+      <c r="GQ36"/>
+      <c r="GR36"/>
+      <c r="GS36"/>
+      <c r="GT36"/>
+      <c r="GU36"/>
+      <c r="GV36"/>
+      <c r="GW36"/>
+      <c r="GX36"/>
+      <c r="GY36"/>
+      <c r="GZ36"/>
+      <c r="HA36"/>
+      <c r="HB36"/>
+      <c r="HC36"/>
+      <c r="HD36"/>
+      <c r="HE36"/>
+      <c r="HF36"/>
+      <c r="HG36"/>
+      <c r="HH36"/>
+      <c r="HI36"/>
+      <c r="HJ36"/>
+      <c r="HK36"/>
+      <c r="HL36"/>
+      <c r="HM36"/>
+      <c r="HN36"/>
+      <c r="HO36"/>
+      <c r="HP36"/>
+      <c r="HQ36"/>
+      <c r="HR36"/>
+      <c r="HS36"/>
+      <c r="HT36"/>
+      <c r="HU36"/>
+      <c r="HV36"/>
+      <c r="HW36"/>
+      <c r="HX36"/>
+      <c r="HY36"/>
+      <c r="HZ36"/>
+      <c r="IA36"/>
+      <c r="IB36"/>
+      <c r="IC36"/>
+      <c r="ID36"/>
+      <c r="IE36"/>
+      <c r="IF36"/>
+      <c r="IG36"/>
+      <c r="IH36"/>
+      <c r="II36"/>
+      <c r="IJ36"/>
+      <c r="IK36"/>
+      <c r="IL36"/>
+      <c r="IM36"/>
+      <c r="IN36"/>
+      <c r="IO36"/>
+      <c r="IP36"/>
+      <c r="IQ36"/>
+      <c r="IR36"/>
+      <c r="IS36"/>
+      <c r="IT36"/>
+      <c r="IU36"/>
+      <c r="IV36"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A35:C35"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3415,11 +5189,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="83" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
+      <c r="A1" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -3431,10 +5205,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="19"/>
@@ -3444,10 +5218,10 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="44" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>57</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="7"/>
@@ -3458,10 +5232,10 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="44" t="s">
         <v>58</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>59</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="7"/>
@@ -3472,10 +5246,10 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="7"/>
@@ -3486,10 +5260,10 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="7"/>
@@ -3500,10 +5274,10 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="7"/>
@@ -3514,10 +5288,10 @@
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="7"/>
@@ -3528,10 +5302,10 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="34"/>
@@ -3542,10 +5316,10 @@
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="31"/>
@@ -3603,21 +5377,21 @@
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="52">
         <v>42715</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="55">
         <v>42714</v>
       </c>
       <c r="F2" s="56"/>
       <c r="G2" s="54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="57">
         <v>42714</v>
@@ -3625,21 +5399,21 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="16">
         <v>42715</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="52">
         <v>42349</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="60">
         <v>42715</v>
@@ -3647,21 +5421,21 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="55">
         <v>42714</v>
       </c>
       <c r="C4" s="62"/>
       <c r="D4" s="44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="10">
         <v>42349</v>
       </c>
       <c r="F4" s="53"/>
       <c r="G4" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H4" s="57">
         <v>42714</v>
@@ -3669,7 +5443,7 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="52">
         <v>42715</v>
@@ -3679,7 +5453,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="53"/>
       <c r="G5" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="57">
         <v>42714</v>
@@ -3687,7 +5461,7 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="16">
         <v>42715</v>
@@ -3701,33 +5475,33 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="65"/>
       <c r="C7" s="56"/>
       <c r="D7" s="66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" s="65"/>
       <c r="F7" s="56"/>
       <c r="G7" s="66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" s="67"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="23"/>
       <c r="D8" s="51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="23"/>
       <c r="G8" s="51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8" s="52">
         <v>42715</v>
@@ -3735,7 +5509,7 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -3745,7 +5519,7 @@
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
       <c r="G9" s="44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H9" s="23"/>
     </row>
@@ -3777,17 +5551,17 @@
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="23"/>
       <c r="D12" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="23"/>
       <c r="G12" s="51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H12" s="21"/>
     </row>
@@ -3796,12 +5570,12 @@
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
       <c r="D13" s="44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H13" s="23"/>
     </row>
@@ -3846,15 +5620,15 @@
       <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="92" t="s">
+      <c r="A18" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="99"/>
+      <c r="G18" s="99"/>
       <c r="H18" s="71"/>
     </row>
   </sheetData>
@@ -3895,7 +5669,7 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -3904,10 +5678,10 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="44" t="s">
         <v>89</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>90</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -3915,10 +5689,10 @@
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="44" t="s">
         <v>91</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>92</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -3934,28 +5708,28 @@
     <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="23"/>
       <c r="B6" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="44" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>94</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="23">
         <v>3</v>
@@ -3966,7 +5740,7 @@
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="25">
         <v>10</v>
@@ -3993,10 +5767,10 @@
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="A12" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="74" t="s">
         <v>99</v>
-      </c>
-      <c r="B12" s="74" t="s">
-        <v>100</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="23"/>
@@ -4004,7 +5778,7 @@
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -4035,7 +5809,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -4051,7 +5825,7 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -4060,7 +5834,7 @@
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -4069,7 +5843,7 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -4078,7 +5852,7 @@
     </row>
     <row r="6" spans="1:5" ht="45" customHeight="1">
       <c r="A6" s="78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -4094,7 +5868,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -4103,7 +5877,7 @@
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1">
       <c r="A9" s="77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -4112,7 +5886,7 @@
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="78" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>

</xml_diff>

<commit_message>
Actualizar de prospecto a actual en llamadas, citas y cotizaciones
</commit_message>
<xml_diff>
--- a/Scrum Febrero.xlsx
+++ b/Scrum Febrero.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="116">
   <si>
     <t>TOÑO</t>
   </si>
@@ -362,13 +362,19 @@
   </si>
   <si>
     <t>12/02/2017</t>
+  </si>
+  <si>
+    <t>Cotización - Revisar cuando se guarda que se limpien los campos</t>
+  </si>
+  <si>
+    <t>Indicador de llamadas - Revisar diseño de tabla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -379,9 +385,16 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -770,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -871,6 +884,11 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -899,8 +917,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2126,11 +2143,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -2225,11 +2242,11 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="19"/>
       <c r="E10" s="8"/>
     </row>
@@ -2310,20 +2327,20 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="87"/>
-      <c r="C21" s="88"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="93"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
-      <c r="A22" s="93" t="s">
+      <c r="A22" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="94"/>
-      <c r="C22" s="95"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="100"/>
       <c r="D22" s="31"/>
       <c r="E22" s="32"/>
     </row>
@@ -2359,11 +2376,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2505,7 +2522,7 @@
       <c r="B10" s="84">
         <v>42778</v>
       </c>
-      <c r="C10" s="101" t="s">
+      <c r="C10" s="90" t="s">
         <v>113</v>
       </c>
       <c r="D10" s="7"/>
@@ -2539,11 +2556,11 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="96"/>
-      <c r="C13" s="92"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -2649,11 +2666,11 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="86" t="s">
+      <c r="A23" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="87"/>
-      <c r="C23" s="88"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="93"/>
       <c r="D23" s="7"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
@@ -2661,11 +2678,11 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="93" t="s">
+      <c r="A24" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="94"/>
-      <c r="C24" s="95"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="31"/>
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
@@ -2689,10 +2706,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV36"/>
+  <dimension ref="A1:IV37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2704,11 +2721,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -3372,31 +3389,283 @@
       <c r="IV11" s="75"/>
     </row>
     <row r="12" spans="1:256" ht="15" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="10">
+      <c r="A12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="13">
         <v>42785</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="14">
+        <v>42785</v>
+      </c>
       <c r="D12" s="34"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
       <c r="H12" s="35"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="75"/>
+      <c r="O12" s="75"/>
+      <c r="P12" s="75"/>
+      <c r="Q12" s="75"/>
+      <c r="R12" s="75"/>
+      <c r="S12" s="75"/>
+      <c r="T12" s="75"/>
+      <c r="U12" s="75"/>
+      <c r="V12" s="75"/>
+      <c r="W12" s="75"/>
+      <c r="X12" s="75"/>
+      <c r="Y12" s="75"/>
+      <c r="Z12" s="75"/>
+      <c r="AA12" s="75"/>
+      <c r="AB12" s="75"/>
+      <c r="AC12" s="75"/>
+      <c r="AD12" s="75"/>
+      <c r="AE12" s="75"/>
+      <c r="AF12" s="75"/>
+      <c r="AG12" s="75"/>
+      <c r="AH12" s="75"/>
+      <c r="AI12" s="75"/>
+      <c r="AJ12" s="75"/>
+      <c r="AK12" s="75"/>
+      <c r="AL12" s="75"/>
+      <c r="AM12" s="75"/>
+      <c r="AN12" s="75"/>
+      <c r="AO12" s="75"/>
+      <c r="AP12" s="75"/>
+      <c r="AQ12" s="75"/>
+      <c r="AR12" s="75"/>
+      <c r="AS12" s="75"/>
+      <c r="AT12" s="75"/>
+      <c r="AU12" s="75"/>
+      <c r="AV12" s="75"/>
+      <c r="AW12" s="75"/>
+      <c r="AX12" s="75"/>
+      <c r="AY12" s="75"/>
+      <c r="AZ12" s="75"/>
+      <c r="BA12" s="75"/>
+      <c r="BB12" s="75"/>
+      <c r="BC12" s="75"/>
+      <c r="BD12" s="75"/>
+      <c r="BE12" s="75"/>
+      <c r="BF12" s="75"/>
+      <c r="BG12" s="75"/>
+      <c r="BH12" s="75"/>
+      <c r="BI12" s="75"/>
+      <c r="BJ12" s="75"/>
+      <c r="BK12" s="75"/>
+      <c r="BL12" s="75"/>
+      <c r="BM12" s="75"/>
+      <c r="BN12" s="75"/>
+      <c r="BO12" s="75"/>
+      <c r="BP12" s="75"/>
+      <c r="BQ12" s="75"/>
+      <c r="BR12" s="75"/>
+      <c r="BS12" s="75"/>
+      <c r="BT12" s="75"/>
+      <c r="BU12" s="75"/>
+      <c r="BV12" s="75"/>
+      <c r="BW12" s="75"/>
+      <c r="BX12" s="75"/>
+      <c r="BY12" s="75"/>
+      <c r="BZ12" s="75"/>
+      <c r="CA12" s="75"/>
+      <c r="CB12" s="75"/>
+      <c r="CC12" s="75"/>
+      <c r="CD12" s="75"/>
+      <c r="CE12" s="75"/>
+      <c r="CF12" s="75"/>
+      <c r="CG12" s="75"/>
+      <c r="CH12" s="75"/>
+      <c r="CI12" s="75"/>
+      <c r="CJ12" s="75"/>
+      <c r="CK12" s="75"/>
+      <c r="CL12" s="75"/>
+      <c r="CM12" s="75"/>
+      <c r="CN12" s="75"/>
+      <c r="CO12" s="75"/>
+      <c r="CP12" s="75"/>
+      <c r="CQ12" s="75"/>
+      <c r="CR12" s="75"/>
+      <c r="CS12" s="75"/>
+      <c r="CT12" s="75"/>
+      <c r="CU12" s="75"/>
+      <c r="CV12" s="75"/>
+      <c r="CW12" s="75"/>
+      <c r="CX12" s="75"/>
+      <c r="CY12" s="75"/>
+      <c r="CZ12" s="75"/>
+      <c r="DA12" s="75"/>
+      <c r="DB12" s="75"/>
+      <c r="DC12" s="75"/>
+      <c r="DD12" s="75"/>
+      <c r="DE12" s="75"/>
+      <c r="DF12" s="75"/>
+      <c r="DG12" s="75"/>
+      <c r="DH12" s="75"/>
+      <c r="DI12" s="75"/>
+      <c r="DJ12" s="75"/>
+      <c r="DK12" s="75"/>
+      <c r="DL12" s="75"/>
+      <c r="DM12" s="75"/>
+      <c r="DN12" s="75"/>
+      <c r="DO12" s="75"/>
+      <c r="DP12" s="75"/>
+      <c r="DQ12" s="75"/>
+      <c r="DR12" s="75"/>
+      <c r="DS12" s="75"/>
+      <c r="DT12" s="75"/>
+      <c r="DU12" s="75"/>
+      <c r="DV12" s="75"/>
+      <c r="DW12" s="75"/>
+      <c r="DX12" s="75"/>
+      <c r="DY12" s="75"/>
+      <c r="DZ12" s="75"/>
+      <c r="EA12" s="75"/>
+      <c r="EB12" s="75"/>
+      <c r="EC12" s="75"/>
+      <c r="ED12" s="75"/>
+      <c r="EE12" s="75"/>
+      <c r="EF12" s="75"/>
+      <c r="EG12" s="75"/>
+      <c r="EH12" s="75"/>
+      <c r="EI12" s="75"/>
+      <c r="EJ12" s="75"/>
+      <c r="EK12" s="75"/>
+      <c r="EL12" s="75"/>
+      <c r="EM12" s="75"/>
+      <c r="EN12" s="75"/>
+      <c r="EO12" s="75"/>
+      <c r="EP12" s="75"/>
+      <c r="EQ12" s="75"/>
+      <c r="ER12" s="75"/>
+      <c r="ES12" s="75"/>
+      <c r="ET12" s="75"/>
+      <c r="EU12" s="75"/>
+      <c r="EV12" s="75"/>
+      <c r="EW12" s="75"/>
+      <c r="EX12" s="75"/>
+      <c r="EY12" s="75"/>
+      <c r="EZ12" s="75"/>
+      <c r="FA12" s="75"/>
+      <c r="FB12" s="75"/>
+      <c r="FC12" s="75"/>
+      <c r="FD12" s="75"/>
+      <c r="FE12" s="75"/>
+      <c r="FF12" s="75"/>
+      <c r="FG12" s="75"/>
+      <c r="FH12" s="75"/>
+      <c r="FI12" s="75"/>
+      <c r="FJ12" s="75"/>
+      <c r="FK12" s="75"/>
+      <c r="FL12" s="75"/>
+      <c r="FM12" s="75"/>
+      <c r="FN12" s="75"/>
+      <c r="FO12" s="75"/>
+      <c r="FP12" s="75"/>
+      <c r="FQ12" s="75"/>
+      <c r="FR12" s="75"/>
+      <c r="FS12" s="75"/>
+      <c r="FT12" s="75"/>
+      <c r="FU12" s="75"/>
+      <c r="FV12" s="75"/>
+      <c r="FW12" s="75"/>
+      <c r="FX12" s="75"/>
+      <c r="FY12" s="75"/>
+      <c r="FZ12" s="75"/>
+      <c r="GA12" s="75"/>
+      <c r="GB12" s="75"/>
+      <c r="GC12" s="75"/>
+      <c r="GD12" s="75"/>
+      <c r="GE12" s="75"/>
+      <c r="GF12" s="75"/>
+      <c r="GG12" s="75"/>
+      <c r="GH12" s="75"/>
+      <c r="GI12" s="75"/>
+      <c r="GJ12" s="75"/>
+      <c r="GK12" s="75"/>
+      <c r="GL12" s="75"/>
+      <c r="GM12" s="75"/>
+      <c r="GN12" s="75"/>
+      <c r="GO12" s="75"/>
+      <c r="GP12" s="75"/>
+      <c r="GQ12" s="75"/>
+      <c r="GR12" s="75"/>
+      <c r="GS12" s="75"/>
+      <c r="GT12" s="75"/>
+      <c r="GU12" s="75"/>
+      <c r="GV12" s="75"/>
+      <c r="GW12" s="75"/>
+      <c r="GX12" s="75"/>
+      <c r="GY12" s="75"/>
+      <c r="GZ12" s="75"/>
+      <c r="HA12" s="75"/>
+      <c r="HB12" s="75"/>
+      <c r="HC12" s="75"/>
+      <c r="HD12" s="75"/>
+      <c r="HE12" s="75"/>
+      <c r="HF12" s="75"/>
+      <c r="HG12" s="75"/>
+      <c r="HH12" s="75"/>
+      <c r="HI12" s="75"/>
+      <c r="HJ12" s="75"/>
+      <c r="HK12" s="75"/>
+      <c r="HL12" s="75"/>
+      <c r="HM12" s="75"/>
+      <c r="HN12" s="75"/>
+      <c r="HO12" s="75"/>
+      <c r="HP12" s="75"/>
+      <c r="HQ12" s="75"/>
+      <c r="HR12" s="75"/>
+      <c r="HS12" s="75"/>
+      <c r="HT12" s="75"/>
+      <c r="HU12" s="75"/>
+      <c r="HV12" s="75"/>
+      <c r="HW12" s="75"/>
+      <c r="HX12" s="75"/>
+      <c r="HY12" s="75"/>
+      <c r="HZ12" s="75"/>
+      <c r="IA12" s="75"/>
+      <c r="IB12" s="75"/>
+      <c r="IC12" s="75"/>
+      <c r="ID12" s="75"/>
+      <c r="IE12" s="75"/>
+      <c r="IF12" s="75"/>
+      <c r="IG12" s="75"/>
+      <c r="IH12" s="75"/>
+      <c r="II12" s="75"/>
+      <c r="IJ12" s="75"/>
+      <c r="IK12" s="75"/>
+      <c r="IL12" s="75"/>
+      <c r="IM12" s="75"/>
+      <c r="IN12" s="75"/>
+      <c r="IO12" s="75"/>
+      <c r="IP12" s="75"/>
+      <c r="IQ12" s="75"/>
+      <c r="IR12" s="75"/>
+      <c r="IS12" s="75"/>
+      <c r="IT12" s="75"/>
+      <c r="IU12" s="75"/>
+      <c r="IV12" s="75"/>
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1">
-      <c r="A13" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="10">
+      <c r="A13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="13">
         <v>42785</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="14">
+        <v>42785</v>
+      </c>
       <c r="D13" s="34"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
       <c r="H13" s="35"/>
       <c r="I13" s="75"/>
       <c r="J13" s="75"/>
@@ -3649,279 +3918,279 @@
     </row>
     <row r="14" spans="1:256" ht="15" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B14" s="10">
         <v>42785</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="75"/>
-      <c r="O14" s="75"/>
-      <c r="P14" s="75"/>
-      <c r="Q14" s="75"/>
-      <c r="R14" s="75"/>
-      <c r="S14" s="75"/>
-      <c r="T14" s="75"/>
-      <c r="U14" s="75"/>
-      <c r="V14" s="75"/>
-      <c r="W14" s="75"/>
-      <c r="X14" s="75"/>
-      <c r="Y14" s="75"/>
-      <c r="Z14" s="75"/>
-      <c r="AA14" s="75"/>
-      <c r="AB14" s="75"/>
-      <c r="AC14" s="75"/>
-      <c r="AD14" s="75"/>
-      <c r="AE14" s="75"/>
-      <c r="AF14" s="75"/>
-      <c r="AG14" s="75"/>
-      <c r="AH14" s="75"/>
-      <c r="AI14" s="75"/>
-      <c r="AJ14" s="75"/>
-      <c r="AK14" s="75"/>
-      <c r="AL14" s="75"/>
-      <c r="AM14" s="75"/>
-      <c r="AN14" s="75"/>
-      <c r="AO14" s="75"/>
-      <c r="AP14" s="75"/>
-      <c r="AQ14" s="75"/>
-      <c r="AR14" s="75"/>
-      <c r="AS14" s="75"/>
-      <c r="AT14" s="75"/>
-      <c r="AU14" s="75"/>
-      <c r="AV14" s="75"/>
-      <c r="AW14" s="75"/>
-      <c r="AX14" s="75"/>
-      <c r="AY14" s="75"/>
-      <c r="AZ14" s="75"/>
-      <c r="BA14" s="75"/>
-      <c r="BB14" s="75"/>
-      <c r="BC14" s="75"/>
-      <c r="BD14" s="75"/>
-      <c r="BE14" s="75"/>
-      <c r="BF14" s="75"/>
-      <c r="BG14" s="75"/>
-      <c r="BH14" s="75"/>
-      <c r="BI14" s="75"/>
-      <c r="BJ14" s="75"/>
-      <c r="BK14" s="75"/>
-      <c r="BL14" s="75"/>
-      <c r="BM14" s="75"/>
-      <c r="BN14" s="75"/>
-      <c r="BO14" s="75"/>
-      <c r="BP14" s="75"/>
-      <c r="BQ14" s="75"/>
-      <c r="BR14" s="75"/>
-      <c r="BS14" s="75"/>
-      <c r="BT14" s="75"/>
-      <c r="BU14" s="75"/>
-      <c r="BV14" s="75"/>
-      <c r="BW14" s="75"/>
-      <c r="BX14" s="75"/>
-      <c r="BY14" s="75"/>
-      <c r="BZ14" s="75"/>
-      <c r="CA14" s="75"/>
-      <c r="CB14" s="75"/>
-      <c r="CC14" s="75"/>
-      <c r="CD14" s="75"/>
-      <c r="CE14" s="75"/>
-      <c r="CF14" s="75"/>
-      <c r="CG14" s="75"/>
-      <c r="CH14" s="75"/>
-      <c r="CI14" s="75"/>
-      <c r="CJ14" s="75"/>
-      <c r="CK14" s="75"/>
-      <c r="CL14" s="75"/>
-      <c r="CM14" s="75"/>
-      <c r="CN14" s="75"/>
-      <c r="CO14" s="75"/>
-      <c r="CP14" s="75"/>
-      <c r="CQ14" s="75"/>
-      <c r="CR14" s="75"/>
-      <c r="CS14" s="75"/>
-      <c r="CT14" s="75"/>
-      <c r="CU14" s="75"/>
-      <c r="CV14" s="75"/>
-      <c r="CW14" s="75"/>
-      <c r="CX14" s="75"/>
-      <c r="CY14" s="75"/>
-      <c r="CZ14" s="75"/>
-      <c r="DA14" s="75"/>
-      <c r="DB14" s="75"/>
-      <c r="DC14" s="75"/>
-      <c r="DD14" s="75"/>
-      <c r="DE14" s="75"/>
-      <c r="DF14" s="75"/>
-      <c r="DG14" s="75"/>
-      <c r="DH14" s="75"/>
-      <c r="DI14" s="75"/>
-      <c r="DJ14" s="75"/>
-      <c r="DK14" s="75"/>
-      <c r="DL14" s="75"/>
-      <c r="DM14" s="75"/>
-      <c r="DN14" s="75"/>
-      <c r="DO14" s="75"/>
-      <c r="DP14" s="75"/>
-      <c r="DQ14" s="75"/>
-      <c r="DR14" s="75"/>
-      <c r="DS14" s="75"/>
-      <c r="DT14" s="75"/>
-      <c r="DU14" s="75"/>
-      <c r="DV14" s="75"/>
-      <c r="DW14" s="75"/>
-      <c r="DX14" s="75"/>
-      <c r="DY14" s="75"/>
-      <c r="DZ14" s="75"/>
-      <c r="EA14" s="75"/>
-      <c r="EB14" s="75"/>
-      <c r="EC14" s="75"/>
-      <c r="ED14" s="75"/>
-      <c r="EE14" s="75"/>
-      <c r="EF14" s="75"/>
-      <c r="EG14" s="75"/>
-      <c r="EH14" s="75"/>
-      <c r="EI14" s="75"/>
-      <c r="EJ14" s="75"/>
-      <c r="EK14" s="75"/>
-      <c r="EL14" s="75"/>
-      <c r="EM14" s="75"/>
-      <c r="EN14" s="75"/>
-      <c r="EO14" s="75"/>
-      <c r="EP14" s="75"/>
-      <c r="EQ14" s="75"/>
-      <c r="ER14" s="75"/>
-      <c r="ES14" s="75"/>
-      <c r="ET14" s="75"/>
-      <c r="EU14" s="75"/>
-      <c r="EV14" s="75"/>
-      <c r="EW14" s="75"/>
-      <c r="EX14" s="75"/>
-      <c r="EY14" s="75"/>
-      <c r="EZ14" s="75"/>
-      <c r="FA14" s="75"/>
-      <c r="FB14" s="75"/>
-      <c r="FC14" s="75"/>
-      <c r="FD14" s="75"/>
-      <c r="FE14" s="75"/>
-      <c r="FF14" s="75"/>
-      <c r="FG14" s="75"/>
-      <c r="FH14" s="75"/>
-      <c r="FI14" s="75"/>
-      <c r="FJ14" s="75"/>
-      <c r="FK14" s="75"/>
-      <c r="FL14" s="75"/>
-      <c r="FM14" s="75"/>
-      <c r="FN14" s="75"/>
-      <c r="FO14" s="75"/>
-      <c r="FP14" s="75"/>
-      <c r="FQ14" s="75"/>
-      <c r="FR14" s="75"/>
-      <c r="FS14" s="75"/>
-      <c r="FT14" s="75"/>
-      <c r="FU14" s="75"/>
-      <c r="FV14" s="75"/>
-      <c r="FW14" s="75"/>
-      <c r="FX14" s="75"/>
-      <c r="FY14" s="75"/>
-      <c r="FZ14" s="75"/>
-      <c r="GA14" s="75"/>
-      <c r="GB14" s="75"/>
-      <c r="GC14" s="75"/>
-      <c r="GD14" s="75"/>
-      <c r="GE14" s="75"/>
-      <c r="GF14" s="75"/>
-      <c r="GG14" s="75"/>
-      <c r="GH14" s="75"/>
-      <c r="GI14" s="75"/>
-      <c r="GJ14" s="75"/>
-      <c r="GK14" s="75"/>
-      <c r="GL14" s="75"/>
-      <c r="GM14" s="75"/>
-      <c r="GN14" s="75"/>
-      <c r="GO14" s="75"/>
-      <c r="GP14" s="75"/>
-      <c r="GQ14" s="75"/>
-      <c r="GR14" s="75"/>
-      <c r="GS14" s="75"/>
-      <c r="GT14" s="75"/>
-      <c r="GU14" s="75"/>
-      <c r="GV14" s="75"/>
-      <c r="GW14" s="75"/>
-      <c r="GX14" s="75"/>
-      <c r="GY14" s="75"/>
-      <c r="GZ14" s="75"/>
-      <c r="HA14" s="75"/>
-      <c r="HB14" s="75"/>
-      <c r="HC14" s="75"/>
-      <c r="HD14" s="75"/>
-      <c r="HE14" s="75"/>
-      <c r="HF14" s="75"/>
-      <c r="HG14" s="75"/>
-      <c r="HH14" s="75"/>
-      <c r="HI14" s="75"/>
-      <c r="HJ14" s="75"/>
-      <c r="HK14" s="75"/>
-      <c r="HL14" s="75"/>
-      <c r="HM14" s="75"/>
-      <c r="HN14" s="75"/>
-      <c r="HO14" s="75"/>
-      <c r="HP14" s="75"/>
-      <c r="HQ14" s="75"/>
-      <c r="HR14" s="75"/>
-      <c r="HS14" s="75"/>
-      <c r="HT14" s="75"/>
-      <c r="HU14" s="75"/>
-      <c r="HV14" s="75"/>
-      <c r="HW14" s="75"/>
-      <c r="HX14" s="75"/>
-      <c r="HY14" s="75"/>
-      <c r="HZ14" s="75"/>
-      <c r="IA14" s="75"/>
-      <c r="IB14" s="75"/>
-      <c r="IC14" s="75"/>
-      <c r="ID14" s="75"/>
-      <c r="IE14" s="75"/>
-      <c r="IF14" s="75"/>
-      <c r="IG14" s="75"/>
-      <c r="IH14" s="75"/>
-      <c r="II14" s="75"/>
-      <c r="IJ14" s="75"/>
-      <c r="IK14" s="75"/>
-      <c r="IL14" s="75"/>
-      <c r="IM14" s="75"/>
-      <c r="IN14" s="75"/>
-      <c r="IO14" s="75"/>
-      <c r="IP14" s="75"/>
-      <c r="IQ14" s="75"/>
-      <c r="IR14" s="75"/>
-      <c r="IS14" s="75"/>
-      <c r="IT14" s="75"/>
-      <c r="IU14" s="75"/>
-      <c r="IV14" s="75"/>
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B15" s="10">
         <v>42785</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
       <c r="H15" s="35"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75"/>
+      <c r="L15" s="75"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="75"/>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="75"/>
+      <c r="S15" s="75"/>
+      <c r="T15" s="75"/>
+      <c r="U15" s="75"/>
+      <c r="V15" s="75"/>
+      <c r="W15" s="75"/>
+      <c r="X15" s="75"/>
+      <c r="Y15" s="75"/>
+      <c r="Z15" s="75"/>
+      <c r="AA15" s="75"/>
+      <c r="AB15" s="75"/>
+      <c r="AC15" s="75"/>
+      <c r="AD15" s="75"/>
+      <c r="AE15" s="75"/>
+      <c r="AF15" s="75"/>
+      <c r="AG15" s="75"/>
+      <c r="AH15" s="75"/>
+      <c r="AI15" s="75"/>
+      <c r="AJ15" s="75"/>
+      <c r="AK15" s="75"/>
+      <c r="AL15" s="75"/>
+      <c r="AM15" s="75"/>
+      <c r="AN15" s="75"/>
+      <c r="AO15" s="75"/>
+      <c r="AP15" s="75"/>
+      <c r="AQ15" s="75"/>
+      <c r="AR15" s="75"/>
+      <c r="AS15" s="75"/>
+      <c r="AT15" s="75"/>
+      <c r="AU15" s="75"/>
+      <c r="AV15" s="75"/>
+      <c r="AW15" s="75"/>
+      <c r="AX15" s="75"/>
+      <c r="AY15" s="75"/>
+      <c r="AZ15" s="75"/>
+      <c r="BA15" s="75"/>
+      <c r="BB15" s="75"/>
+      <c r="BC15" s="75"/>
+      <c r="BD15" s="75"/>
+      <c r="BE15" s="75"/>
+      <c r="BF15" s="75"/>
+      <c r="BG15" s="75"/>
+      <c r="BH15" s="75"/>
+      <c r="BI15" s="75"/>
+      <c r="BJ15" s="75"/>
+      <c r="BK15" s="75"/>
+      <c r="BL15" s="75"/>
+      <c r="BM15" s="75"/>
+      <c r="BN15" s="75"/>
+      <c r="BO15" s="75"/>
+      <c r="BP15" s="75"/>
+      <c r="BQ15" s="75"/>
+      <c r="BR15" s="75"/>
+      <c r="BS15" s="75"/>
+      <c r="BT15" s="75"/>
+      <c r="BU15" s="75"/>
+      <c r="BV15" s="75"/>
+      <c r="BW15" s="75"/>
+      <c r="BX15" s="75"/>
+      <c r="BY15" s="75"/>
+      <c r="BZ15" s="75"/>
+      <c r="CA15" s="75"/>
+      <c r="CB15" s="75"/>
+      <c r="CC15" s="75"/>
+      <c r="CD15" s="75"/>
+      <c r="CE15" s="75"/>
+      <c r="CF15" s="75"/>
+      <c r="CG15" s="75"/>
+      <c r="CH15" s="75"/>
+      <c r="CI15" s="75"/>
+      <c r="CJ15" s="75"/>
+      <c r="CK15" s="75"/>
+      <c r="CL15" s="75"/>
+      <c r="CM15" s="75"/>
+      <c r="CN15" s="75"/>
+      <c r="CO15" s="75"/>
+      <c r="CP15" s="75"/>
+      <c r="CQ15" s="75"/>
+      <c r="CR15" s="75"/>
+      <c r="CS15" s="75"/>
+      <c r="CT15" s="75"/>
+      <c r="CU15" s="75"/>
+      <c r="CV15" s="75"/>
+      <c r="CW15" s="75"/>
+      <c r="CX15" s="75"/>
+      <c r="CY15" s="75"/>
+      <c r="CZ15" s="75"/>
+      <c r="DA15" s="75"/>
+      <c r="DB15" s="75"/>
+      <c r="DC15" s="75"/>
+      <c r="DD15" s="75"/>
+      <c r="DE15" s="75"/>
+      <c r="DF15" s="75"/>
+      <c r="DG15" s="75"/>
+      <c r="DH15" s="75"/>
+      <c r="DI15" s="75"/>
+      <c r="DJ15" s="75"/>
+      <c r="DK15" s="75"/>
+      <c r="DL15" s="75"/>
+      <c r="DM15" s="75"/>
+      <c r="DN15" s="75"/>
+      <c r="DO15" s="75"/>
+      <c r="DP15" s="75"/>
+      <c r="DQ15" s="75"/>
+      <c r="DR15" s="75"/>
+      <c r="DS15" s="75"/>
+      <c r="DT15" s="75"/>
+      <c r="DU15" s="75"/>
+      <c r="DV15" s="75"/>
+      <c r="DW15" s="75"/>
+      <c r="DX15" s="75"/>
+      <c r="DY15" s="75"/>
+      <c r="DZ15" s="75"/>
+      <c r="EA15" s="75"/>
+      <c r="EB15" s="75"/>
+      <c r="EC15" s="75"/>
+      <c r="ED15" s="75"/>
+      <c r="EE15" s="75"/>
+      <c r="EF15" s="75"/>
+      <c r="EG15" s="75"/>
+      <c r="EH15" s="75"/>
+      <c r="EI15" s="75"/>
+      <c r="EJ15" s="75"/>
+      <c r="EK15" s="75"/>
+      <c r="EL15" s="75"/>
+      <c r="EM15" s="75"/>
+      <c r="EN15" s="75"/>
+      <c r="EO15" s="75"/>
+      <c r="EP15" s="75"/>
+      <c r="EQ15" s="75"/>
+      <c r="ER15" s="75"/>
+      <c r="ES15" s="75"/>
+      <c r="ET15" s="75"/>
+      <c r="EU15" s="75"/>
+      <c r="EV15" s="75"/>
+      <c r="EW15" s="75"/>
+      <c r="EX15" s="75"/>
+      <c r="EY15" s="75"/>
+      <c r="EZ15" s="75"/>
+      <c r="FA15" s="75"/>
+      <c r="FB15" s="75"/>
+      <c r="FC15" s="75"/>
+      <c r="FD15" s="75"/>
+      <c r="FE15" s="75"/>
+      <c r="FF15" s="75"/>
+      <c r="FG15" s="75"/>
+      <c r="FH15" s="75"/>
+      <c r="FI15" s="75"/>
+      <c r="FJ15" s="75"/>
+      <c r="FK15" s="75"/>
+      <c r="FL15" s="75"/>
+      <c r="FM15" s="75"/>
+      <c r="FN15" s="75"/>
+      <c r="FO15" s="75"/>
+      <c r="FP15" s="75"/>
+      <c r="FQ15" s="75"/>
+      <c r="FR15" s="75"/>
+      <c r="FS15" s="75"/>
+      <c r="FT15" s="75"/>
+      <c r="FU15" s="75"/>
+      <c r="FV15" s="75"/>
+      <c r="FW15" s="75"/>
+      <c r="FX15" s="75"/>
+      <c r="FY15" s="75"/>
+      <c r="FZ15" s="75"/>
+      <c r="GA15" s="75"/>
+      <c r="GB15" s="75"/>
+      <c r="GC15" s="75"/>
+      <c r="GD15" s="75"/>
+      <c r="GE15" s="75"/>
+      <c r="GF15" s="75"/>
+      <c r="GG15" s="75"/>
+      <c r="GH15" s="75"/>
+      <c r="GI15" s="75"/>
+      <c r="GJ15" s="75"/>
+      <c r="GK15" s="75"/>
+      <c r="GL15" s="75"/>
+      <c r="GM15" s="75"/>
+      <c r="GN15" s="75"/>
+      <c r="GO15" s="75"/>
+      <c r="GP15" s="75"/>
+      <c r="GQ15" s="75"/>
+      <c r="GR15" s="75"/>
+      <c r="GS15" s="75"/>
+      <c r="GT15" s="75"/>
+      <c r="GU15" s="75"/>
+      <c r="GV15" s="75"/>
+      <c r="GW15" s="75"/>
+      <c r="GX15" s="75"/>
+      <c r="GY15" s="75"/>
+      <c r="GZ15" s="75"/>
+      <c r="HA15" s="75"/>
+      <c r="HB15" s="75"/>
+      <c r="HC15" s="75"/>
+      <c r="HD15" s="75"/>
+      <c r="HE15" s="75"/>
+      <c r="HF15" s="75"/>
+      <c r="HG15" s="75"/>
+      <c r="HH15" s="75"/>
+      <c r="HI15" s="75"/>
+      <c r="HJ15" s="75"/>
+      <c r="HK15" s="75"/>
+      <c r="HL15" s="75"/>
+      <c r="HM15" s="75"/>
+      <c r="HN15" s="75"/>
+      <c r="HO15" s="75"/>
+      <c r="HP15" s="75"/>
+      <c r="HQ15" s="75"/>
+      <c r="HR15" s="75"/>
+      <c r="HS15" s="75"/>
+      <c r="HT15" s="75"/>
+      <c r="HU15" s="75"/>
+      <c r="HV15" s="75"/>
+      <c r="HW15" s="75"/>
+      <c r="HX15" s="75"/>
+      <c r="HY15" s="75"/>
+      <c r="HZ15" s="75"/>
+      <c r="IA15" s="75"/>
+      <c r="IB15" s="75"/>
+      <c r="IC15" s="75"/>
+      <c r="ID15" s="75"/>
+      <c r="IE15" s="75"/>
+      <c r="IF15" s="75"/>
+      <c r="IG15" s="75"/>
+      <c r="IH15" s="75"/>
+      <c r="II15" s="75"/>
+      <c r="IJ15" s="75"/>
+      <c r="IK15" s="75"/>
+      <c r="IL15" s="75"/>
+      <c r="IM15" s="75"/>
+      <c r="IN15" s="75"/>
+      <c r="IO15" s="75"/>
+      <c r="IP15" s="75"/>
+      <c r="IQ15" s="75"/>
+      <c r="IR15" s="75"/>
+      <c r="IS15" s="75"/>
+      <c r="IT15" s="75"/>
+      <c r="IU15" s="75"/>
+      <c r="IV15" s="75"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
       <c r="A16" s="15"/>
@@ -3934,11 +4203,11 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:256" ht="15" customHeight="1">
-      <c r="A17" s="97" t="s">
+      <c r="A17" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="92"/>
-      <c r="C17" s="92"/>
+      <c r="B17" s="97"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
@@ -3946,7 +4215,7 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:256" ht="15" customHeight="1">
-      <c r="A18" s="100" t="s">
+      <c r="A18" s="89" t="s">
         <v>111</v>
       </c>
       <c r="B18" s="21"/>
@@ -4550,16 +4819,264 @@
       <c r="IV26" s="75"/>
     </row>
     <row r="27" spans="1:256" ht="15" customHeight="1">
-      <c r="A27" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="24"/>
+      <c r="A27" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="86"/>
+      <c r="C27" s="87"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
       <c r="H27" s="35"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="75"/>
+      <c r="O27" s="75"/>
+      <c r="P27" s="75"/>
+      <c r="Q27" s="75"/>
+      <c r="R27" s="75"/>
+      <c r="S27" s="75"/>
+      <c r="T27" s="75"/>
+      <c r="U27" s="75"/>
+      <c r="V27" s="75"/>
+      <c r="W27" s="75"/>
+      <c r="X27" s="75"/>
+      <c r="Y27" s="75"/>
+      <c r="Z27" s="75"/>
+      <c r="AA27" s="75"/>
+      <c r="AB27" s="75"/>
+      <c r="AC27" s="75"/>
+      <c r="AD27" s="75"/>
+      <c r="AE27" s="75"/>
+      <c r="AF27" s="75"/>
+      <c r="AG27" s="75"/>
+      <c r="AH27" s="75"/>
+      <c r="AI27" s="75"/>
+      <c r="AJ27" s="75"/>
+      <c r="AK27" s="75"/>
+      <c r="AL27" s="75"/>
+      <c r="AM27" s="75"/>
+      <c r="AN27" s="75"/>
+      <c r="AO27" s="75"/>
+      <c r="AP27" s="75"/>
+      <c r="AQ27" s="75"/>
+      <c r="AR27" s="75"/>
+      <c r="AS27" s="75"/>
+      <c r="AT27" s="75"/>
+      <c r="AU27" s="75"/>
+      <c r="AV27" s="75"/>
+      <c r="AW27" s="75"/>
+      <c r="AX27" s="75"/>
+      <c r="AY27" s="75"/>
+      <c r="AZ27" s="75"/>
+      <c r="BA27" s="75"/>
+      <c r="BB27" s="75"/>
+      <c r="BC27" s="75"/>
+      <c r="BD27" s="75"/>
+      <c r="BE27" s="75"/>
+      <c r="BF27" s="75"/>
+      <c r="BG27" s="75"/>
+      <c r="BH27" s="75"/>
+      <c r="BI27" s="75"/>
+      <c r="BJ27" s="75"/>
+      <c r="BK27" s="75"/>
+      <c r="BL27" s="75"/>
+      <c r="BM27" s="75"/>
+      <c r="BN27" s="75"/>
+      <c r="BO27" s="75"/>
+      <c r="BP27" s="75"/>
+      <c r="BQ27" s="75"/>
+      <c r="BR27" s="75"/>
+      <c r="BS27" s="75"/>
+      <c r="BT27" s="75"/>
+      <c r="BU27" s="75"/>
+      <c r="BV27" s="75"/>
+      <c r="BW27" s="75"/>
+      <c r="BX27" s="75"/>
+      <c r="BY27" s="75"/>
+      <c r="BZ27" s="75"/>
+      <c r="CA27" s="75"/>
+      <c r="CB27" s="75"/>
+      <c r="CC27" s="75"/>
+      <c r="CD27" s="75"/>
+      <c r="CE27" s="75"/>
+      <c r="CF27" s="75"/>
+      <c r="CG27" s="75"/>
+      <c r="CH27" s="75"/>
+      <c r="CI27" s="75"/>
+      <c r="CJ27" s="75"/>
+      <c r="CK27" s="75"/>
+      <c r="CL27" s="75"/>
+      <c r="CM27" s="75"/>
+      <c r="CN27" s="75"/>
+      <c r="CO27" s="75"/>
+      <c r="CP27" s="75"/>
+      <c r="CQ27" s="75"/>
+      <c r="CR27" s="75"/>
+      <c r="CS27" s="75"/>
+      <c r="CT27" s="75"/>
+      <c r="CU27" s="75"/>
+      <c r="CV27" s="75"/>
+      <c r="CW27" s="75"/>
+      <c r="CX27" s="75"/>
+      <c r="CY27" s="75"/>
+      <c r="CZ27" s="75"/>
+      <c r="DA27" s="75"/>
+      <c r="DB27" s="75"/>
+      <c r="DC27" s="75"/>
+      <c r="DD27" s="75"/>
+      <c r="DE27" s="75"/>
+      <c r="DF27" s="75"/>
+      <c r="DG27" s="75"/>
+      <c r="DH27" s="75"/>
+      <c r="DI27" s="75"/>
+      <c r="DJ27" s="75"/>
+      <c r="DK27" s="75"/>
+      <c r="DL27" s="75"/>
+      <c r="DM27" s="75"/>
+      <c r="DN27" s="75"/>
+      <c r="DO27" s="75"/>
+      <c r="DP27" s="75"/>
+      <c r="DQ27" s="75"/>
+      <c r="DR27" s="75"/>
+      <c r="DS27" s="75"/>
+      <c r="DT27" s="75"/>
+      <c r="DU27" s="75"/>
+      <c r="DV27" s="75"/>
+      <c r="DW27" s="75"/>
+      <c r="DX27" s="75"/>
+      <c r="DY27" s="75"/>
+      <c r="DZ27" s="75"/>
+      <c r="EA27" s="75"/>
+      <c r="EB27" s="75"/>
+      <c r="EC27" s="75"/>
+      <c r="ED27" s="75"/>
+      <c r="EE27" s="75"/>
+      <c r="EF27" s="75"/>
+      <c r="EG27" s="75"/>
+      <c r="EH27" s="75"/>
+      <c r="EI27" s="75"/>
+      <c r="EJ27" s="75"/>
+      <c r="EK27" s="75"/>
+      <c r="EL27" s="75"/>
+      <c r="EM27" s="75"/>
+      <c r="EN27" s="75"/>
+      <c r="EO27" s="75"/>
+      <c r="EP27" s="75"/>
+      <c r="EQ27" s="75"/>
+      <c r="ER27" s="75"/>
+      <c r="ES27" s="75"/>
+      <c r="ET27" s="75"/>
+      <c r="EU27" s="75"/>
+      <c r="EV27" s="75"/>
+      <c r="EW27" s="75"/>
+      <c r="EX27" s="75"/>
+      <c r="EY27" s="75"/>
+      <c r="EZ27" s="75"/>
+      <c r="FA27" s="75"/>
+      <c r="FB27" s="75"/>
+      <c r="FC27" s="75"/>
+      <c r="FD27" s="75"/>
+      <c r="FE27" s="75"/>
+      <c r="FF27" s="75"/>
+      <c r="FG27" s="75"/>
+      <c r="FH27" s="75"/>
+      <c r="FI27" s="75"/>
+      <c r="FJ27" s="75"/>
+      <c r="FK27" s="75"/>
+      <c r="FL27" s="75"/>
+      <c r="FM27" s="75"/>
+      <c r="FN27" s="75"/>
+      <c r="FO27" s="75"/>
+      <c r="FP27" s="75"/>
+      <c r="FQ27" s="75"/>
+      <c r="FR27" s="75"/>
+      <c r="FS27" s="75"/>
+      <c r="FT27" s="75"/>
+      <c r="FU27" s="75"/>
+      <c r="FV27" s="75"/>
+      <c r="FW27" s="75"/>
+      <c r="FX27" s="75"/>
+      <c r="FY27" s="75"/>
+      <c r="FZ27" s="75"/>
+      <c r="GA27" s="75"/>
+      <c r="GB27" s="75"/>
+      <c r="GC27" s="75"/>
+      <c r="GD27" s="75"/>
+      <c r="GE27" s="75"/>
+      <c r="GF27" s="75"/>
+      <c r="GG27" s="75"/>
+      <c r="GH27" s="75"/>
+      <c r="GI27" s="75"/>
+      <c r="GJ27" s="75"/>
+      <c r="GK27" s="75"/>
+      <c r="GL27" s="75"/>
+      <c r="GM27" s="75"/>
+      <c r="GN27" s="75"/>
+      <c r="GO27" s="75"/>
+      <c r="GP27" s="75"/>
+      <c r="GQ27" s="75"/>
+      <c r="GR27" s="75"/>
+      <c r="GS27" s="75"/>
+      <c r="GT27" s="75"/>
+      <c r="GU27" s="75"/>
+      <c r="GV27" s="75"/>
+      <c r="GW27" s="75"/>
+      <c r="GX27" s="75"/>
+      <c r="GY27" s="75"/>
+      <c r="GZ27" s="75"/>
+      <c r="HA27" s="75"/>
+      <c r="HB27" s="75"/>
+      <c r="HC27" s="75"/>
+      <c r="HD27" s="75"/>
+      <c r="HE27" s="75"/>
+      <c r="HF27" s="75"/>
+      <c r="HG27" s="75"/>
+      <c r="HH27" s="75"/>
+      <c r="HI27" s="75"/>
+      <c r="HJ27" s="75"/>
+      <c r="HK27" s="75"/>
+      <c r="HL27" s="75"/>
+      <c r="HM27" s="75"/>
+      <c r="HN27" s="75"/>
+      <c r="HO27" s="75"/>
+      <c r="HP27" s="75"/>
+      <c r="HQ27" s="75"/>
+      <c r="HR27" s="75"/>
+      <c r="HS27" s="75"/>
+      <c r="HT27" s="75"/>
+      <c r="HU27" s="75"/>
+      <c r="HV27" s="75"/>
+      <c r="HW27" s="75"/>
+      <c r="HX27" s="75"/>
+      <c r="HY27" s="75"/>
+      <c r="HZ27" s="75"/>
+      <c r="IA27" s="75"/>
+      <c r="IB27" s="75"/>
+      <c r="IC27" s="75"/>
+      <c r="ID27" s="75"/>
+      <c r="IE27" s="75"/>
+      <c r="IF27" s="75"/>
+      <c r="IG27" s="75"/>
+      <c r="IH27" s="75"/>
+      <c r="II27" s="75"/>
+      <c r="IJ27" s="75"/>
+      <c r="IK27" s="75"/>
+      <c r="IL27" s="75"/>
+      <c r="IM27" s="75"/>
+      <c r="IN27" s="75"/>
+      <c r="IO27" s="75"/>
+      <c r="IP27" s="75"/>
+      <c r="IQ27" s="75"/>
+      <c r="IR27" s="75"/>
+      <c r="IS27" s="75"/>
+      <c r="IT27" s="75"/>
+      <c r="IU27" s="75"/>
+      <c r="IV27" s="75"/>
     </row>
     <row r="28" spans="1:256" ht="15" customHeight="1">
       <c r="A28" s="9" t="s">
@@ -4598,41 +5115,291 @@
       <c r="H30" s="35"/>
     </row>
     <row r="31" spans="1:256" ht="15" customHeight="1">
-      <c r="A31" s="15"/>
+      <c r="A31" s="105" t="s">
+        <v>114</v>
+      </c>
       <c r="B31" s="25"/>
       <c r="C31" s="26"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="8"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="88"/>
+      <c r="F31" s="88"/>
+      <c r="G31" s="88"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="75"/>
+      <c r="M31" s="75"/>
+      <c r="N31" s="75"/>
+      <c r="O31" s="75"/>
+      <c r="P31" s="75"/>
+      <c r="Q31" s="75"/>
+      <c r="R31" s="75"/>
+      <c r="S31" s="75"/>
+      <c r="T31" s="75"/>
+      <c r="U31" s="75"/>
+      <c r="V31" s="75"/>
+      <c r="W31" s="75"/>
+      <c r="X31" s="75"/>
+      <c r="Y31" s="75"/>
+      <c r="Z31" s="75"/>
+      <c r="AA31" s="75"/>
+      <c r="AB31" s="75"/>
+      <c r="AC31" s="75"/>
+      <c r="AD31" s="75"/>
+      <c r="AE31" s="75"/>
+      <c r="AF31" s="75"/>
+      <c r="AG31" s="75"/>
+      <c r="AH31" s="75"/>
+      <c r="AI31" s="75"/>
+      <c r="AJ31" s="75"/>
+      <c r="AK31" s="75"/>
+      <c r="AL31" s="75"/>
+      <c r="AM31" s="75"/>
+      <c r="AN31" s="75"/>
+      <c r="AO31" s="75"/>
+      <c r="AP31" s="75"/>
+      <c r="AQ31" s="75"/>
+      <c r="AR31" s="75"/>
+      <c r="AS31" s="75"/>
+      <c r="AT31" s="75"/>
+      <c r="AU31" s="75"/>
+      <c r="AV31" s="75"/>
+      <c r="AW31" s="75"/>
+      <c r="AX31" s="75"/>
+      <c r="AY31" s="75"/>
+      <c r="AZ31" s="75"/>
+      <c r="BA31" s="75"/>
+      <c r="BB31" s="75"/>
+      <c r="BC31" s="75"/>
+      <c r="BD31" s="75"/>
+      <c r="BE31" s="75"/>
+      <c r="BF31" s="75"/>
+      <c r="BG31" s="75"/>
+      <c r="BH31" s="75"/>
+      <c r="BI31" s="75"/>
+      <c r="BJ31" s="75"/>
+      <c r="BK31" s="75"/>
+      <c r="BL31" s="75"/>
+      <c r="BM31" s="75"/>
+      <c r="BN31" s="75"/>
+      <c r="BO31" s="75"/>
+      <c r="BP31" s="75"/>
+      <c r="BQ31" s="75"/>
+      <c r="BR31" s="75"/>
+      <c r="BS31" s="75"/>
+      <c r="BT31" s="75"/>
+      <c r="BU31" s="75"/>
+      <c r="BV31" s="75"/>
+      <c r="BW31" s="75"/>
+      <c r="BX31" s="75"/>
+      <c r="BY31" s="75"/>
+      <c r="BZ31" s="75"/>
+      <c r="CA31" s="75"/>
+      <c r="CB31" s="75"/>
+      <c r="CC31" s="75"/>
+      <c r="CD31" s="75"/>
+      <c r="CE31" s="75"/>
+      <c r="CF31" s="75"/>
+      <c r="CG31" s="75"/>
+      <c r="CH31" s="75"/>
+      <c r="CI31" s="75"/>
+      <c r="CJ31" s="75"/>
+      <c r="CK31" s="75"/>
+      <c r="CL31" s="75"/>
+      <c r="CM31" s="75"/>
+      <c r="CN31" s="75"/>
+      <c r="CO31" s="75"/>
+      <c r="CP31" s="75"/>
+      <c r="CQ31" s="75"/>
+      <c r="CR31" s="75"/>
+      <c r="CS31" s="75"/>
+      <c r="CT31" s="75"/>
+      <c r="CU31" s="75"/>
+      <c r="CV31" s="75"/>
+      <c r="CW31" s="75"/>
+      <c r="CX31" s="75"/>
+      <c r="CY31" s="75"/>
+      <c r="CZ31" s="75"/>
+      <c r="DA31" s="75"/>
+      <c r="DB31" s="75"/>
+      <c r="DC31" s="75"/>
+      <c r="DD31" s="75"/>
+      <c r="DE31" s="75"/>
+      <c r="DF31" s="75"/>
+      <c r="DG31" s="75"/>
+      <c r="DH31" s="75"/>
+      <c r="DI31" s="75"/>
+      <c r="DJ31" s="75"/>
+      <c r="DK31" s="75"/>
+      <c r="DL31" s="75"/>
+      <c r="DM31" s="75"/>
+      <c r="DN31" s="75"/>
+      <c r="DO31" s="75"/>
+      <c r="DP31" s="75"/>
+      <c r="DQ31" s="75"/>
+      <c r="DR31" s="75"/>
+      <c r="DS31" s="75"/>
+      <c r="DT31" s="75"/>
+      <c r="DU31" s="75"/>
+      <c r="DV31" s="75"/>
+      <c r="DW31" s="75"/>
+      <c r="DX31" s="75"/>
+      <c r="DY31" s="75"/>
+      <c r="DZ31" s="75"/>
+      <c r="EA31" s="75"/>
+      <c r="EB31" s="75"/>
+      <c r="EC31" s="75"/>
+      <c r="ED31" s="75"/>
+      <c r="EE31" s="75"/>
+      <c r="EF31" s="75"/>
+      <c r="EG31" s="75"/>
+      <c r="EH31" s="75"/>
+      <c r="EI31" s="75"/>
+      <c r="EJ31" s="75"/>
+      <c r="EK31" s="75"/>
+      <c r="EL31" s="75"/>
+      <c r="EM31" s="75"/>
+      <c r="EN31" s="75"/>
+      <c r="EO31" s="75"/>
+      <c r="EP31" s="75"/>
+      <c r="EQ31" s="75"/>
+      <c r="ER31" s="75"/>
+      <c r="ES31" s="75"/>
+      <c r="ET31" s="75"/>
+      <c r="EU31" s="75"/>
+      <c r="EV31" s="75"/>
+      <c r="EW31" s="75"/>
+      <c r="EX31" s="75"/>
+      <c r="EY31" s="75"/>
+      <c r="EZ31" s="75"/>
+      <c r="FA31" s="75"/>
+      <c r="FB31" s="75"/>
+      <c r="FC31" s="75"/>
+      <c r="FD31" s="75"/>
+      <c r="FE31" s="75"/>
+      <c r="FF31" s="75"/>
+      <c r="FG31" s="75"/>
+      <c r="FH31" s="75"/>
+      <c r="FI31" s="75"/>
+      <c r="FJ31" s="75"/>
+      <c r="FK31" s="75"/>
+      <c r="FL31" s="75"/>
+      <c r="FM31" s="75"/>
+      <c r="FN31" s="75"/>
+      <c r="FO31" s="75"/>
+      <c r="FP31" s="75"/>
+      <c r="FQ31" s="75"/>
+      <c r="FR31" s="75"/>
+      <c r="FS31" s="75"/>
+      <c r="FT31" s="75"/>
+      <c r="FU31" s="75"/>
+      <c r="FV31" s="75"/>
+      <c r="FW31" s="75"/>
+      <c r="FX31" s="75"/>
+      <c r="FY31" s="75"/>
+      <c r="FZ31" s="75"/>
+      <c r="GA31" s="75"/>
+      <c r="GB31" s="75"/>
+      <c r="GC31" s="75"/>
+      <c r="GD31" s="75"/>
+      <c r="GE31" s="75"/>
+      <c r="GF31" s="75"/>
+      <c r="GG31" s="75"/>
+      <c r="GH31" s="75"/>
+      <c r="GI31" s="75"/>
+      <c r="GJ31" s="75"/>
+      <c r="GK31" s="75"/>
+      <c r="GL31" s="75"/>
+      <c r="GM31" s="75"/>
+      <c r="GN31" s="75"/>
+      <c r="GO31" s="75"/>
+      <c r="GP31" s="75"/>
+      <c r="GQ31" s="75"/>
+      <c r="GR31" s="75"/>
+      <c r="GS31" s="75"/>
+      <c r="GT31" s="75"/>
+      <c r="GU31" s="75"/>
+      <c r="GV31" s="75"/>
+      <c r="GW31" s="75"/>
+      <c r="GX31" s="75"/>
+      <c r="GY31" s="75"/>
+      <c r="GZ31" s="75"/>
+      <c r="HA31" s="75"/>
+      <c r="HB31" s="75"/>
+      <c r="HC31" s="75"/>
+      <c r="HD31" s="75"/>
+      <c r="HE31" s="75"/>
+      <c r="HF31" s="75"/>
+      <c r="HG31" s="75"/>
+      <c r="HH31" s="75"/>
+      <c r="HI31" s="75"/>
+      <c r="HJ31" s="75"/>
+      <c r="HK31" s="75"/>
+      <c r="HL31" s="75"/>
+      <c r="HM31" s="75"/>
+      <c r="HN31" s="75"/>
+      <c r="HO31" s="75"/>
+      <c r="HP31" s="75"/>
+      <c r="HQ31" s="75"/>
+      <c r="HR31" s="75"/>
+      <c r="HS31" s="75"/>
+      <c r="HT31" s="75"/>
+      <c r="HU31" s="75"/>
+      <c r="HV31" s="75"/>
+      <c r="HW31" s="75"/>
+      <c r="HX31" s="75"/>
+      <c r="HY31" s="75"/>
+      <c r="HZ31" s="75"/>
+      <c r="IA31" s="75"/>
+      <c r="IB31" s="75"/>
+      <c r="IC31" s="75"/>
+      <c r="ID31" s="75"/>
+      <c r="IE31" s="75"/>
+      <c r="IF31" s="75"/>
+      <c r="IG31" s="75"/>
+      <c r="IH31" s="75"/>
+      <c r="II31" s="75"/>
+      <c r="IJ31" s="75"/>
+      <c r="IK31" s="75"/>
+      <c r="IL31" s="75"/>
+      <c r="IM31" s="75"/>
+      <c r="IN31" s="75"/>
+      <c r="IO31" s="75"/>
+      <c r="IP31" s="75"/>
+      <c r="IQ31" s="75"/>
+      <c r="IR31" s="75"/>
+      <c r="IS31" s="75"/>
+      <c r="IT31" s="75"/>
+      <c r="IU31" s="75"/>
+      <c r="IV31" s="75"/>
     </row>
     <row r="32" spans="1:256" ht="15" customHeight="1">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="15"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:256" ht="15" customHeight="1">
+      <c r="A33" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="35"/>
-    </row>
-    <row r="33" spans="1:256" ht="15" customHeight="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="34"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
       <c r="H33" s="35"/>
     </row>
     <row r="34" spans="1:256" ht="15" customHeight="1">
-      <c r="A34" s="30"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="34"/>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
@@ -4640,276 +5407,26 @@
       <c r="H34" s="35"/>
     </row>
     <row r="35" spans="1:256" ht="15" customHeight="1">
-      <c r="A35" s="86" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="87"/>
-      <c r="C35" s="88"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="34"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
       <c r="H35" s="35"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
-      <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35"/>
-      <c r="AQ35"/>
-      <c r="AR35"/>
-      <c r="AS35"/>
-      <c r="AT35"/>
-      <c r="AU35"/>
-      <c r="AV35"/>
-      <c r="AW35"/>
-      <c r="AX35"/>
-      <c r="AY35"/>
-      <c r="AZ35"/>
-      <c r="BA35"/>
-      <c r="BB35"/>
-      <c r="BC35"/>
-      <c r="BD35"/>
-      <c r="BE35"/>
-      <c r="BF35"/>
-      <c r="BG35"/>
-      <c r="BH35"/>
-      <c r="BI35"/>
-      <c r="BJ35"/>
-      <c r="BK35"/>
-      <c r="BL35"/>
-      <c r="BM35"/>
-      <c r="BN35"/>
-      <c r="BO35"/>
-      <c r="BP35"/>
-      <c r="BQ35"/>
-      <c r="BR35"/>
-      <c r="BS35"/>
-      <c r="BT35"/>
-      <c r="BU35"/>
-      <c r="BV35"/>
-      <c r="BW35"/>
-      <c r="BX35"/>
-      <c r="BY35"/>
-      <c r="BZ35"/>
-      <c r="CA35"/>
-      <c r="CB35"/>
-      <c r="CC35"/>
-      <c r="CD35"/>
-      <c r="CE35"/>
-      <c r="CF35"/>
-      <c r="CG35"/>
-      <c r="CH35"/>
-      <c r="CI35"/>
-      <c r="CJ35"/>
-      <c r="CK35"/>
-      <c r="CL35"/>
-      <c r="CM35"/>
-      <c r="CN35"/>
-      <c r="CO35"/>
-      <c r="CP35"/>
-      <c r="CQ35"/>
-      <c r="CR35"/>
-      <c r="CS35"/>
-      <c r="CT35"/>
-      <c r="CU35"/>
-      <c r="CV35"/>
-      <c r="CW35"/>
-      <c r="CX35"/>
-      <c r="CY35"/>
-      <c r="CZ35"/>
-      <c r="DA35"/>
-      <c r="DB35"/>
-      <c r="DC35"/>
-      <c r="DD35"/>
-      <c r="DE35"/>
-      <c r="DF35"/>
-      <c r="DG35"/>
-      <c r="DH35"/>
-      <c r="DI35"/>
-      <c r="DJ35"/>
-      <c r="DK35"/>
-      <c r="DL35"/>
-      <c r="DM35"/>
-      <c r="DN35"/>
-      <c r="DO35"/>
-      <c r="DP35"/>
-      <c r="DQ35"/>
-      <c r="DR35"/>
-      <c r="DS35"/>
-      <c r="DT35"/>
-      <c r="DU35"/>
-      <c r="DV35"/>
-      <c r="DW35"/>
-      <c r="DX35"/>
-      <c r="DY35"/>
-      <c r="DZ35"/>
-      <c r="EA35"/>
-      <c r="EB35"/>
-      <c r="EC35"/>
-      <c r="ED35"/>
-      <c r="EE35"/>
-      <c r="EF35"/>
-      <c r="EG35"/>
-      <c r="EH35"/>
-      <c r="EI35"/>
-      <c r="EJ35"/>
-      <c r="EK35"/>
-      <c r="EL35"/>
-      <c r="EM35"/>
-      <c r="EN35"/>
-      <c r="EO35"/>
-      <c r="EP35"/>
-      <c r="EQ35"/>
-      <c r="ER35"/>
-      <c r="ES35"/>
-      <c r="ET35"/>
-      <c r="EU35"/>
-      <c r="EV35"/>
-      <c r="EW35"/>
-      <c r="EX35"/>
-      <c r="EY35"/>
-      <c r="EZ35"/>
-      <c r="FA35"/>
-      <c r="FB35"/>
-      <c r="FC35"/>
-      <c r="FD35"/>
-      <c r="FE35"/>
-      <c r="FF35"/>
-      <c r="FG35"/>
-      <c r="FH35"/>
-      <c r="FI35"/>
-      <c r="FJ35"/>
-      <c r="FK35"/>
-      <c r="FL35"/>
-      <c r="FM35"/>
-      <c r="FN35"/>
-      <c r="FO35"/>
-      <c r="FP35"/>
-      <c r="FQ35"/>
-      <c r="FR35"/>
-      <c r="FS35"/>
-      <c r="FT35"/>
-      <c r="FU35"/>
-      <c r="FV35"/>
-      <c r="FW35"/>
-      <c r="FX35"/>
-      <c r="FY35"/>
-      <c r="FZ35"/>
-      <c r="GA35"/>
-      <c r="GB35"/>
-      <c r="GC35"/>
-      <c r="GD35"/>
-      <c r="GE35"/>
-      <c r="GF35"/>
-      <c r="GG35"/>
-      <c r="GH35"/>
-      <c r="GI35"/>
-      <c r="GJ35"/>
-      <c r="GK35"/>
-      <c r="GL35"/>
-      <c r="GM35"/>
-      <c r="GN35"/>
-      <c r="GO35"/>
-      <c r="GP35"/>
-      <c r="GQ35"/>
-      <c r="GR35"/>
-      <c r="GS35"/>
-      <c r="GT35"/>
-      <c r="GU35"/>
-      <c r="GV35"/>
-      <c r="GW35"/>
-      <c r="GX35"/>
-      <c r="GY35"/>
-      <c r="GZ35"/>
-      <c r="HA35"/>
-      <c r="HB35"/>
-      <c r="HC35"/>
-      <c r="HD35"/>
-      <c r="HE35"/>
-      <c r="HF35"/>
-      <c r="HG35"/>
-      <c r="HH35"/>
-      <c r="HI35"/>
-      <c r="HJ35"/>
-      <c r="HK35"/>
-      <c r="HL35"/>
-      <c r="HM35"/>
-      <c r="HN35"/>
-      <c r="HO35"/>
-      <c r="HP35"/>
-      <c r="HQ35"/>
-      <c r="HR35"/>
-      <c r="HS35"/>
-      <c r="HT35"/>
-      <c r="HU35"/>
-      <c r="HV35"/>
-      <c r="HW35"/>
-      <c r="HX35"/>
-      <c r="HY35"/>
-      <c r="HZ35"/>
-      <c r="IA35"/>
-      <c r="IB35"/>
-      <c r="IC35"/>
-      <c r="ID35"/>
-      <c r="IE35"/>
-      <c r="IF35"/>
-      <c r="IG35"/>
-      <c r="IH35"/>
-      <c r="II35"/>
-      <c r="IJ35"/>
-      <c r="IK35"/>
-      <c r="IL35"/>
-      <c r="IM35"/>
-      <c r="IN35"/>
-      <c r="IO35"/>
-      <c r="IP35"/>
-      <c r="IQ35"/>
-      <c r="IR35"/>
-      <c r="IS35"/>
-      <c r="IT35"/>
-      <c r="IU35"/>
-      <c r="IV35"/>
     </row>
     <row r="36" spans="1:256" ht="15" customHeight="1">
-      <c r="A36" s="93" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36" s="94"/>
-      <c r="C36" s="95"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="42"/>
+      <c r="A36" s="91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="92"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="35"/>
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>
@@ -5159,12 +5676,272 @@
       <c r="IU36"/>
       <c r="IV36"/>
     </row>
+    <row r="37" spans="1:256" ht="15" customHeight="1">
+      <c r="A37" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="99"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="42"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37"/>
+      <c r="AC37"/>
+      <c r="AD37"/>
+      <c r="AE37"/>
+      <c r="AF37"/>
+      <c r="AG37"/>
+      <c r="AH37"/>
+      <c r="AI37"/>
+      <c r="AJ37"/>
+      <c r="AK37"/>
+      <c r="AL37"/>
+      <c r="AM37"/>
+      <c r="AN37"/>
+      <c r="AO37"/>
+      <c r="AP37"/>
+      <c r="AQ37"/>
+      <c r="AR37"/>
+      <c r="AS37"/>
+      <c r="AT37"/>
+      <c r="AU37"/>
+      <c r="AV37"/>
+      <c r="AW37"/>
+      <c r="AX37"/>
+      <c r="AY37"/>
+      <c r="AZ37"/>
+      <c r="BA37"/>
+      <c r="BB37"/>
+      <c r="BC37"/>
+      <c r="BD37"/>
+      <c r="BE37"/>
+      <c r="BF37"/>
+      <c r="BG37"/>
+      <c r="BH37"/>
+      <c r="BI37"/>
+      <c r="BJ37"/>
+      <c r="BK37"/>
+      <c r="BL37"/>
+      <c r="BM37"/>
+      <c r="BN37"/>
+      <c r="BO37"/>
+      <c r="BP37"/>
+      <c r="BQ37"/>
+      <c r="BR37"/>
+      <c r="BS37"/>
+      <c r="BT37"/>
+      <c r="BU37"/>
+      <c r="BV37"/>
+      <c r="BW37"/>
+      <c r="BX37"/>
+      <c r="BY37"/>
+      <c r="BZ37"/>
+      <c r="CA37"/>
+      <c r="CB37"/>
+      <c r="CC37"/>
+      <c r="CD37"/>
+      <c r="CE37"/>
+      <c r="CF37"/>
+      <c r="CG37"/>
+      <c r="CH37"/>
+      <c r="CI37"/>
+      <c r="CJ37"/>
+      <c r="CK37"/>
+      <c r="CL37"/>
+      <c r="CM37"/>
+      <c r="CN37"/>
+      <c r="CO37"/>
+      <c r="CP37"/>
+      <c r="CQ37"/>
+      <c r="CR37"/>
+      <c r="CS37"/>
+      <c r="CT37"/>
+      <c r="CU37"/>
+      <c r="CV37"/>
+      <c r="CW37"/>
+      <c r="CX37"/>
+      <c r="CY37"/>
+      <c r="CZ37"/>
+      <c r="DA37"/>
+      <c r="DB37"/>
+      <c r="DC37"/>
+      <c r="DD37"/>
+      <c r="DE37"/>
+      <c r="DF37"/>
+      <c r="DG37"/>
+      <c r="DH37"/>
+      <c r="DI37"/>
+      <c r="DJ37"/>
+      <c r="DK37"/>
+      <c r="DL37"/>
+      <c r="DM37"/>
+      <c r="DN37"/>
+      <c r="DO37"/>
+      <c r="DP37"/>
+      <c r="DQ37"/>
+      <c r="DR37"/>
+      <c r="DS37"/>
+      <c r="DT37"/>
+      <c r="DU37"/>
+      <c r="DV37"/>
+      <c r="DW37"/>
+      <c r="DX37"/>
+      <c r="DY37"/>
+      <c r="DZ37"/>
+      <c r="EA37"/>
+      <c r="EB37"/>
+      <c r="EC37"/>
+      <c r="ED37"/>
+      <c r="EE37"/>
+      <c r="EF37"/>
+      <c r="EG37"/>
+      <c r="EH37"/>
+      <c r="EI37"/>
+      <c r="EJ37"/>
+      <c r="EK37"/>
+      <c r="EL37"/>
+      <c r="EM37"/>
+      <c r="EN37"/>
+      <c r="EO37"/>
+      <c r="EP37"/>
+      <c r="EQ37"/>
+      <c r="ER37"/>
+      <c r="ES37"/>
+      <c r="ET37"/>
+      <c r="EU37"/>
+      <c r="EV37"/>
+      <c r="EW37"/>
+      <c r="EX37"/>
+      <c r="EY37"/>
+      <c r="EZ37"/>
+      <c r="FA37"/>
+      <c r="FB37"/>
+      <c r="FC37"/>
+      <c r="FD37"/>
+      <c r="FE37"/>
+      <c r="FF37"/>
+      <c r="FG37"/>
+      <c r="FH37"/>
+      <c r="FI37"/>
+      <c r="FJ37"/>
+      <c r="FK37"/>
+      <c r="FL37"/>
+      <c r="FM37"/>
+      <c r="FN37"/>
+      <c r="FO37"/>
+      <c r="FP37"/>
+      <c r="FQ37"/>
+      <c r="FR37"/>
+      <c r="FS37"/>
+      <c r="FT37"/>
+      <c r="FU37"/>
+      <c r="FV37"/>
+      <c r="FW37"/>
+      <c r="FX37"/>
+      <c r="FY37"/>
+      <c r="FZ37"/>
+      <c r="GA37"/>
+      <c r="GB37"/>
+      <c r="GC37"/>
+      <c r="GD37"/>
+      <c r="GE37"/>
+      <c r="GF37"/>
+      <c r="GG37"/>
+      <c r="GH37"/>
+      <c r="GI37"/>
+      <c r="GJ37"/>
+      <c r="GK37"/>
+      <c r="GL37"/>
+      <c r="GM37"/>
+      <c r="GN37"/>
+      <c r="GO37"/>
+      <c r="GP37"/>
+      <c r="GQ37"/>
+      <c r="GR37"/>
+      <c r="GS37"/>
+      <c r="GT37"/>
+      <c r="GU37"/>
+      <c r="GV37"/>
+      <c r="GW37"/>
+      <c r="GX37"/>
+      <c r="GY37"/>
+      <c r="GZ37"/>
+      <c r="HA37"/>
+      <c r="HB37"/>
+      <c r="HC37"/>
+      <c r="HD37"/>
+      <c r="HE37"/>
+      <c r="HF37"/>
+      <c r="HG37"/>
+      <c r="HH37"/>
+      <c r="HI37"/>
+      <c r="HJ37"/>
+      <c r="HK37"/>
+      <c r="HL37"/>
+      <c r="HM37"/>
+      <c r="HN37"/>
+      <c r="HO37"/>
+      <c r="HP37"/>
+      <c r="HQ37"/>
+      <c r="HR37"/>
+      <c r="HS37"/>
+      <c r="HT37"/>
+      <c r="HU37"/>
+      <c r="HV37"/>
+      <c r="HW37"/>
+      <c r="HX37"/>
+      <c r="HY37"/>
+      <c r="HZ37"/>
+      <c r="IA37"/>
+      <c r="IB37"/>
+      <c r="IC37"/>
+      <c r="ID37"/>
+      <c r="IE37"/>
+      <c r="IF37"/>
+      <c r="IG37"/>
+      <c r="IH37"/>
+      <c r="II37"/>
+      <c r="IJ37"/>
+      <c r="IK37"/>
+      <c r="IL37"/>
+      <c r="IM37"/>
+      <c r="IN37"/>
+      <c r="IO37"/>
+      <c r="IP37"/>
+      <c r="IQ37"/>
+      <c r="IR37"/>
+      <c r="IS37"/>
+      <c r="IT37"/>
+      <c r="IU37"/>
+      <c r="IV37"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:C36"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5189,11 +5966,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -5620,15 +6397,15 @@
       <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="98" t="s">
+      <c r="A18" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="99"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="104"/>
       <c r="H18" s="71"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Indicadores - Agregar overflow, Cotización - Revisar cuando se guarda que se limpien los campos, Actualizar actividades
</commit_message>
<xml_diff>
--- a/Scrum Febrero.xlsx
+++ b/Scrum Febrero.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="130">
   <si>
     <t>TOÑO</t>
   </si>
@@ -398,6 +398,21 @@
   </si>
   <si>
     <t>Login - Que mande a esa pantalla si finaliza la sesión</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servidor - Modificar configuración para correr SP y crear SP </t>
+  </si>
+  <si>
+    <t>Servidor - Conexión remota SSH para reiniciar tomcat</t>
+  </si>
+  <si>
+    <t>Servidor - Que se realicen los queries</t>
+  </si>
+  <si>
+    <t>Base de datos - Tablas para sección de logística y cobranza en perfil</t>
+  </si>
+  <si>
+    <t>Cotizaciones - Cambiar vista inicial de contacto a inactivos (como cuando se recarga)</t>
   </si>
 </sst>
 </file>
@@ -856,7 +871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -977,11 +992,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -990,6 +1004,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -998,13 +1017,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1014,6 +1026,15 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2227,7 +2248,7 @@
   <dimension ref="A1:IV19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2239,11 +2260,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -2265,7 +2286,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="10">
-        <v>42799</v>
+        <v>42806</v>
       </c>
       <c r="C3" s="89"/>
       <c r="D3" s="7"/>
@@ -2276,7 +2297,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="10">
-        <v>42799</v>
+        <v>42806</v>
       </c>
       <c r="C4" s="89"/>
       <c r="D4" s="7"/>
@@ -2287,7 +2308,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="10">
-        <v>42799</v>
+        <v>42806</v>
       </c>
       <c r="C5" s="89"/>
       <c r="D5" s="7"/>
@@ -2298,7 +2319,7 @@
         <v>124</v>
       </c>
       <c r="B6" s="10">
-        <v>42799</v>
+        <v>42806</v>
       </c>
       <c r="C6" s="89"/>
       <c r="D6" s="7"/>
@@ -2312,11 +2333,11 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="105" t="s">
+      <c r="A8" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="106"/>
-      <c r="C8" s="106"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
       <c r="D8" s="19"/>
       <c r="E8" s="8"/>
     </row>
@@ -2386,20 +2407,20 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="100" t="s">
+      <c r="A18" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="101"/>
-      <c r="C18" s="102"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="110"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="107" t="s">
+      <c r="A19" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="108"/>
-      <c r="C19" s="109"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="113"/>
       <c r="D19" s="30"/>
       <c r="E19" s="31"/>
     </row>
@@ -2552,7 +2573,7 @@
   <dimension ref="A1:IV17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2564,11 +2585,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2596,7 +2617,7 @@
         <v>122</v>
       </c>
       <c r="B3" s="10">
-        <v>42799</v>
+        <v>42806</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="7"/>
@@ -2610,7 +2631,7 @@
         <v>121</v>
       </c>
       <c r="B4" s="10">
-        <v>42799</v>
+        <v>42778</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="7"/>
@@ -2642,7 +2663,9 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="20"/>
+      <c r="A7" s="122" t="s">
+        <v>128</v>
+      </c>
       <c r="B7" s="10"/>
       <c r="C7" s="22"/>
       <c r="D7" s="7"/>
@@ -2770,10 +2793,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV33"/>
+  <dimension ref="A1:IV37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2785,11 +2808,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2865,7 +2888,9 @@
       <c r="B6" s="13">
         <v>42799</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="14">
+        <v>42798</v>
+      </c>
       <c r="D6" s="33"/>
       <c r="E6" s="96"/>
       <c r="F6" s="96"/>
@@ -2873,21 +2898,31 @@
       <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
+      <c r="A7" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="13">
+        <v>42799</v>
+      </c>
+      <c r="C7" s="14">
+        <v>42798</v>
+      </c>
       <c r="D7" s="33"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
       <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="A8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
+      <c r="A8" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="13">
+        <v>42799</v>
+      </c>
+      <c r="C8" s="14">
+        <v>42798</v>
+      </c>
       <c r="D8" s="33"/>
       <c r="E8" s="96"/>
       <c r="F8" s="96"/>
@@ -2895,33 +2930,37 @@
       <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="13">
+        <v>42806</v>
+      </c>
+      <c r="C9" s="14">
+        <v>42805</v>
+      </c>
       <c r="D9" s="33"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="96"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
       <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="120" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="121">
+        <v>42806</v>
+      </c>
+      <c r="C10" s="14"/>
       <c r="D10" s="33"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
       <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
-      <c r="A11" s="9" t="s">
-        <v>41</v>
-      </c>
+      <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="33"/>
@@ -2931,8 +2970,8 @@
       <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>123</v>
+      <c r="A12" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
@@ -2944,7 +2983,7 @@
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
@@ -2955,78 +2994,78 @@
       <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="8"/>
+      <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="34"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="34"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1">
+      <c r="A18" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="83" t="s">
+      <c r="B18" s="107"/>
+      <c r="C18" s="107"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1">
+      <c r="A19" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:256" ht="15" customHeight="1">
-      <c r="A17" s="9" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1">
+      <c r="A20" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="34"/>
-    </row>
-    <row r="18" spans="1:256" ht="15" customHeight="1">
-      <c r="A18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="94"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="34"/>
-    </row>
-    <row r="19" spans="1:256" ht="15" customHeight="1">
-      <c r="A19" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="93"/>
-      <c r="C19" s="94"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="34"/>
-    </row>
-    <row r="20" spans="1:256" ht="15" customHeight="1">
-      <c r="A20" s="79" t="s">
-        <v>109</v>
       </c>
       <c r="B20" s="93"/>
       <c r="C20" s="94"/>
@@ -3036,21 +3075,21 @@
       <c r="G20" s="96"/>
       <c r="H20" s="34"/>
     </row>
-    <row r="21" spans="1:256" ht="15" customHeight="1">
-      <c r="A21" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="94"/>
+    <row r="21" spans="1:8" ht="15" customHeight="1">
+      <c r="A21" s="120" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="100"/>
+      <c r="C21" s="101"/>
       <c r="D21" s="33"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="96"/>
-      <c r="G21" s="96"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
       <c r="H21" s="34"/>
     </row>
-    <row r="22" spans="1:256" ht="15" customHeight="1">
-      <c r="A22" s="12" t="s">
-        <v>114</v>
+    <row r="22" spans="1:8" ht="15" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="B22" s="93"/>
       <c r="C22" s="94"/>
@@ -3060,9 +3099,9 @@
       <c r="G22" s="96"/>
       <c r="H22" s="34"/>
     </row>
-    <row r="23" spans="1:256" ht="15" customHeight="1">
+    <row r="23" spans="1:8" ht="15" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B23" s="93"/>
       <c r="C23" s="94"/>
@@ -3072,9 +3111,9 @@
       <c r="G23" s="96"/>
       <c r="H23" s="34"/>
     </row>
-    <row r="24" spans="1:256" ht="15" customHeight="1">
-      <c r="A24" s="9" t="s">
-        <v>47</v>
+    <row r="24" spans="1:8" ht="15" customHeight="1">
+      <c r="A24" s="79" t="s">
+        <v>109</v>
       </c>
       <c r="B24" s="93"/>
       <c r="C24" s="94"/>
@@ -3084,9 +3123,9 @@
       <c r="G24" s="96"/>
       <c r="H24" s="34"/>
     </row>
-    <row r="25" spans="1:256" ht="15" customHeight="1">
-      <c r="A25" s="9" t="s">
-        <v>48</v>
+    <row r="25" spans="1:8" ht="15" customHeight="1">
+      <c r="A25" s="79" t="s">
+        <v>50</v>
       </c>
       <c r="B25" s="93"/>
       <c r="C25" s="94"/>
@@ -3096,596 +3135,644 @@
       <c r="G25" s="96"/>
       <c r="H25" s="34"/>
     </row>
-    <row r="26" spans="1:256" ht="15" customHeight="1">
-      <c r="A26" s="84" t="s">
-        <v>119</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
+    <row r="26" spans="1:8" ht="15" customHeight="1">
+      <c r="A26" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="93"/>
+      <c r="C26" s="94"/>
       <c r="D26" s="33"/>
       <c r="E26" s="96"/>
       <c r="F26" s="96"/>
       <c r="G26" s="96"/>
       <c r="H26" s="34"/>
     </row>
-    <row r="27" spans="1:256" ht="15" customHeight="1">
-      <c r="A27" s="84"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
+    <row r="27" spans="1:8" ht="15" customHeight="1">
+      <c r="A27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="93"/>
+      <c r="C27" s="94"/>
       <c r="D27" s="33"/>
       <c r="E27" s="96"/>
       <c r="F27" s="96"/>
       <c r="G27" s="96"/>
       <c r="H27" s="34"/>
     </row>
-    <row r="28" spans="1:256" ht="15" customHeight="1">
-      <c r="A28" s="15"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:256" ht="15" customHeight="1">
-      <c r="A29" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="96"/>
+    <row r="28" spans="1:8" ht="15" customHeight="1">
+      <c r="A28" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="93"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="96"/>
+      <c r="G28" s="96"/>
+      <c r="H28" s="34"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1">
+      <c r="A29" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="93"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="96"/>
       <c r="F29" s="96"/>
       <c r="G29" s="96"/>
       <c r="H29" s="34"/>
     </row>
-    <row r="30" spans="1:256" ht="15" customHeight="1">
-      <c r="A30" s="28"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
+    <row r="30" spans="1:8" ht="15" customHeight="1">
+      <c r="A30" s="84" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="33"/>
       <c r="E30" s="96"/>
       <c r="F30" s="96"/>
       <c r="G30" s="96"/>
       <c r="H30" s="34"/>
     </row>
-    <row r="31" spans="1:256" ht="15" customHeight="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="93"/>
-      <c r="C31" s="94"/>
+    <row r="31" spans="1:8" ht="15" customHeight="1">
+      <c r="A31" s="84"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="33"/>
       <c r="E31" s="96"/>
       <c r="F31" s="96"/>
       <c r="G31" s="96"/>
       <c r="H31" s="34"/>
     </row>
-    <row r="32" spans="1:256" ht="15" customHeight="1">
-      <c r="A32" s="100" t="s">
+    <row r="32" spans="1:8" ht="15" customHeight="1">
+      <c r="A32" s="15"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:256" ht="15" customHeight="1">
+      <c r="A33" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="96"/>
+      <c r="F33" s="96"/>
+      <c r="G33" s="96"/>
+      <c r="H33" s="34"/>
+    </row>
+    <row r="34" spans="1:256" ht="15" customHeight="1">
+      <c r="A34" s="28"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="96"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="34"/>
+    </row>
+    <row r="35" spans="1:256" ht="15" customHeight="1">
+      <c r="A35" s="29"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="34"/>
+    </row>
+    <row r="36" spans="1:256" ht="15" customHeight="1">
+      <c r="A36" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="101"/>
-      <c r="C32" s="102"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="96"/>
-      <c r="F32" s="96"/>
-      <c r="G32" s="96"/>
-      <c r="H32" s="34"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
-      <c r="AC32"/>
-      <c r="AD32"/>
-      <c r="AE32"/>
-      <c r="AF32"/>
-      <c r="AG32"/>
-      <c r="AH32"/>
-      <c r="AI32"/>
-      <c r="AJ32"/>
-      <c r="AK32"/>
-      <c r="AL32"/>
-      <c r="AM32"/>
-      <c r="AN32"/>
-      <c r="AO32"/>
-      <c r="AP32"/>
-      <c r="AQ32"/>
-      <c r="AR32"/>
-      <c r="AS32"/>
-      <c r="AT32"/>
-      <c r="AU32"/>
-      <c r="AV32"/>
-      <c r="AW32"/>
-      <c r="AX32"/>
-      <c r="AY32"/>
-      <c r="AZ32"/>
-      <c r="BA32"/>
-      <c r="BB32"/>
-      <c r="BC32"/>
-      <c r="BD32"/>
-      <c r="BE32"/>
-      <c r="BF32"/>
-      <c r="BG32"/>
-      <c r="BH32"/>
-      <c r="BI32"/>
-      <c r="BJ32"/>
-      <c r="BK32"/>
-      <c r="BL32"/>
-      <c r="BM32"/>
-      <c r="BN32"/>
-      <c r="BO32"/>
-      <c r="BP32"/>
-      <c r="BQ32"/>
-      <c r="BR32"/>
-      <c r="BS32"/>
-      <c r="BT32"/>
-      <c r="BU32"/>
-      <c r="BV32"/>
-      <c r="BW32"/>
-      <c r="BX32"/>
-      <c r="BY32"/>
-      <c r="BZ32"/>
-      <c r="CA32"/>
-      <c r="CB32"/>
-      <c r="CC32"/>
-      <c r="CD32"/>
-      <c r="CE32"/>
-      <c r="CF32"/>
-      <c r="CG32"/>
-      <c r="CH32"/>
-      <c r="CI32"/>
-      <c r="CJ32"/>
-      <c r="CK32"/>
-      <c r="CL32"/>
-      <c r="CM32"/>
-      <c r="CN32"/>
-      <c r="CO32"/>
-      <c r="CP32"/>
-      <c r="CQ32"/>
-      <c r="CR32"/>
-      <c r="CS32"/>
-      <c r="CT32"/>
-      <c r="CU32"/>
-      <c r="CV32"/>
-      <c r="CW32"/>
-      <c r="CX32"/>
-      <c r="CY32"/>
-      <c r="CZ32"/>
-      <c r="DA32"/>
-      <c r="DB32"/>
-      <c r="DC32"/>
-      <c r="DD32"/>
-      <c r="DE32"/>
-      <c r="DF32"/>
-      <c r="DG32"/>
-      <c r="DH32"/>
-      <c r="DI32"/>
-      <c r="DJ32"/>
-      <c r="DK32"/>
-      <c r="DL32"/>
-      <c r="DM32"/>
-      <c r="DN32"/>
-      <c r="DO32"/>
-      <c r="DP32"/>
-      <c r="DQ32"/>
-      <c r="DR32"/>
-      <c r="DS32"/>
-      <c r="DT32"/>
-      <c r="DU32"/>
-      <c r="DV32"/>
-      <c r="DW32"/>
-      <c r="DX32"/>
-      <c r="DY32"/>
-      <c r="DZ32"/>
-      <c r="EA32"/>
-      <c r="EB32"/>
-      <c r="EC32"/>
-      <c r="ED32"/>
-      <c r="EE32"/>
-      <c r="EF32"/>
-      <c r="EG32"/>
-      <c r="EH32"/>
-      <c r="EI32"/>
-      <c r="EJ32"/>
-      <c r="EK32"/>
-      <c r="EL32"/>
-      <c r="EM32"/>
-      <c r="EN32"/>
-      <c r="EO32"/>
-      <c r="EP32"/>
-      <c r="EQ32"/>
-      <c r="ER32"/>
-      <c r="ES32"/>
-      <c r="ET32"/>
-      <c r="EU32"/>
-      <c r="EV32"/>
-      <c r="EW32"/>
-      <c r="EX32"/>
-      <c r="EY32"/>
-      <c r="EZ32"/>
-      <c r="FA32"/>
-      <c r="FB32"/>
-      <c r="FC32"/>
-      <c r="FD32"/>
-      <c r="FE32"/>
-      <c r="FF32"/>
-      <c r="FG32"/>
-      <c r="FH32"/>
-      <c r="FI32"/>
-      <c r="FJ32"/>
-      <c r="FK32"/>
-      <c r="FL32"/>
-      <c r="FM32"/>
-      <c r="FN32"/>
-      <c r="FO32"/>
-      <c r="FP32"/>
-      <c r="FQ32"/>
-      <c r="FR32"/>
-      <c r="FS32"/>
-      <c r="FT32"/>
-      <c r="FU32"/>
-      <c r="FV32"/>
-      <c r="FW32"/>
-      <c r="FX32"/>
-      <c r="FY32"/>
-      <c r="FZ32"/>
-      <c r="GA32"/>
-      <c r="GB32"/>
-      <c r="GC32"/>
-      <c r="GD32"/>
-      <c r="GE32"/>
-      <c r="GF32"/>
-      <c r="GG32"/>
-      <c r="GH32"/>
-      <c r="GI32"/>
-      <c r="GJ32"/>
-      <c r="GK32"/>
-      <c r="GL32"/>
-      <c r="GM32"/>
-      <c r="GN32"/>
-      <c r="GO32"/>
-      <c r="GP32"/>
-      <c r="GQ32"/>
-      <c r="GR32"/>
-      <c r="GS32"/>
-      <c r="GT32"/>
-      <c r="GU32"/>
-      <c r="GV32"/>
-      <c r="GW32"/>
-      <c r="GX32"/>
-      <c r="GY32"/>
-      <c r="GZ32"/>
-      <c r="HA32"/>
-      <c r="HB32"/>
-      <c r="HC32"/>
-      <c r="HD32"/>
-      <c r="HE32"/>
-      <c r="HF32"/>
-      <c r="HG32"/>
-      <c r="HH32"/>
-      <c r="HI32"/>
-      <c r="HJ32"/>
-      <c r="HK32"/>
-      <c r="HL32"/>
-      <c r="HM32"/>
-      <c r="HN32"/>
-      <c r="HO32"/>
-      <c r="HP32"/>
-      <c r="HQ32"/>
-      <c r="HR32"/>
-      <c r="HS32"/>
-      <c r="HT32"/>
-      <c r="HU32"/>
-      <c r="HV32"/>
-      <c r="HW32"/>
-      <c r="HX32"/>
-      <c r="HY32"/>
-      <c r="HZ32"/>
-      <c r="IA32"/>
-      <c r="IB32"/>
-      <c r="IC32"/>
-      <c r="ID32"/>
-      <c r="IE32"/>
-      <c r="IF32"/>
-      <c r="IG32"/>
-      <c r="IH32"/>
-      <c r="II32"/>
-      <c r="IJ32"/>
-      <c r="IK32"/>
-      <c r="IL32"/>
-      <c r="IM32"/>
-      <c r="IN32"/>
-      <c r="IO32"/>
-      <c r="IP32"/>
-      <c r="IQ32"/>
-      <c r="IR32"/>
-      <c r="IS32"/>
-      <c r="IT32"/>
-      <c r="IU32"/>
-      <c r="IV32"/>
-    </row>
-    <row r="33" spans="1:256" ht="15" customHeight="1">
-      <c r="A33" s="107" t="s">
+      <c r="B36" s="109"/>
+      <c r="C36" s="110"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="96"/>
+      <c r="H36" s="34"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AJ36"/>
+      <c r="AK36"/>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+      <c r="AR36"/>
+      <c r="AS36"/>
+      <c r="AT36"/>
+      <c r="AU36"/>
+      <c r="AV36"/>
+      <c r="AW36"/>
+      <c r="AX36"/>
+      <c r="AY36"/>
+      <c r="AZ36"/>
+      <c r="BA36"/>
+      <c r="BB36"/>
+      <c r="BC36"/>
+      <c r="BD36"/>
+      <c r="BE36"/>
+      <c r="BF36"/>
+      <c r="BG36"/>
+      <c r="BH36"/>
+      <c r="BI36"/>
+      <c r="BJ36"/>
+      <c r="BK36"/>
+      <c r="BL36"/>
+      <c r="BM36"/>
+      <c r="BN36"/>
+      <c r="BO36"/>
+      <c r="BP36"/>
+      <c r="BQ36"/>
+      <c r="BR36"/>
+      <c r="BS36"/>
+      <c r="BT36"/>
+      <c r="BU36"/>
+      <c r="BV36"/>
+      <c r="BW36"/>
+      <c r="BX36"/>
+      <c r="BY36"/>
+      <c r="BZ36"/>
+      <c r="CA36"/>
+      <c r="CB36"/>
+      <c r="CC36"/>
+      <c r="CD36"/>
+      <c r="CE36"/>
+      <c r="CF36"/>
+      <c r="CG36"/>
+      <c r="CH36"/>
+      <c r="CI36"/>
+      <c r="CJ36"/>
+      <c r="CK36"/>
+      <c r="CL36"/>
+      <c r="CM36"/>
+      <c r="CN36"/>
+      <c r="CO36"/>
+      <c r="CP36"/>
+      <c r="CQ36"/>
+      <c r="CR36"/>
+      <c r="CS36"/>
+      <c r="CT36"/>
+      <c r="CU36"/>
+      <c r="CV36"/>
+      <c r="CW36"/>
+      <c r="CX36"/>
+      <c r="CY36"/>
+      <c r="CZ36"/>
+      <c r="DA36"/>
+      <c r="DB36"/>
+      <c r="DC36"/>
+      <c r="DD36"/>
+      <c r="DE36"/>
+      <c r="DF36"/>
+      <c r="DG36"/>
+      <c r="DH36"/>
+      <c r="DI36"/>
+      <c r="DJ36"/>
+      <c r="DK36"/>
+      <c r="DL36"/>
+      <c r="DM36"/>
+      <c r="DN36"/>
+      <c r="DO36"/>
+      <c r="DP36"/>
+      <c r="DQ36"/>
+      <c r="DR36"/>
+      <c r="DS36"/>
+      <c r="DT36"/>
+      <c r="DU36"/>
+      <c r="DV36"/>
+      <c r="DW36"/>
+      <c r="DX36"/>
+      <c r="DY36"/>
+      <c r="DZ36"/>
+      <c r="EA36"/>
+      <c r="EB36"/>
+      <c r="EC36"/>
+      <c r="ED36"/>
+      <c r="EE36"/>
+      <c r="EF36"/>
+      <c r="EG36"/>
+      <c r="EH36"/>
+      <c r="EI36"/>
+      <c r="EJ36"/>
+      <c r="EK36"/>
+      <c r="EL36"/>
+      <c r="EM36"/>
+      <c r="EN36"/>
+      <c r="EO36"/>
+      <c r="EP36"/>
+      <c r="EQ36"/>
+      <c r="ER36"/>
+      <c r="ES36"/>
+      <c r="ET36"/>
+      <c r="EU36"/>
+      <c r="EV36"/>
+      <c r="EW36"/>
+      <c r="EX36"/>
+      <c r="EY36"/>
+      <c r="EZ36"/>
+      <c r="FA36"/>
+      <c r="FB36"/>
+      <c r="FC36"/>
+      <c r="FD36"/>
+      <c r="FE36"/>
+      <c r="FF36"/>
+      <c r="FG36"/>
+      <c r="FH36"/>
+      <c r="FI36"/>
+      <c r="FJ36"/>
+      <c r="FK36"/>
+      <c r="FL36"/>
+      <c r="FM36"/>
+      <c r="FN36"/>
+      <c r="FO36"/>
+      <c r="FP36"/>
+      <c r="FQ36"/>
+      <c r="FR36"/>
+      <c r="FS36"/>
+      <c r="FT36"/>
+      <c r="FU36"/>
+      <c r="FV36"/>
+      <c r="FW36"/>
+      <c r="FX36"/>
+      <c r="FY36"/>
+      <c r="FZ36"/>
+      <c r="GA36"/>
+      <c r="GB36"/>
+      <c r="GC36"/>
+      <c r="GD36"/>
+      <c r="GE36"/>
+      <c r="GF36"/>
+      <c r="GG36"/>
+      <c r="GH36"/>
+      <c r="GI36"/>
+      <c r="GJ36"/>
+      <c r="GK36"/>
+      <c r="GL36"/>
+      <c r="GM36"/>
+      <c r="GN36"/>
+      <c r="GO36"/>
+      <c r="GP36"/>
+      <c r="GQ36"/>
+      <c r="GR36"/>
+      <c r="GS36"/>
+      <c r="GT36"/>
+      <c r="GU36"/>
+      <c r="GV36"/>
+      <c r="GW36"/>
+      <c r="GX36"/>
+      <c r="GY36"/>
+      <c r="GZ36"/>
+      <c r="HA36"/>
+      <c r="HB36"/>
+      <c r="HC36"/>
+      <c r="HD36"/>
+      <c r="HE36"/>
+      <c r="HF36"/>
+      <c r="HG36"/>
+      <c r="HH36"/>
+      <c r="HI36"/>
+      <c r="HJ36"/>
+      <c r="HK36"/>
+      <c r="HL36"/>
+      <c r="HM36"/>
+      <c r="HN36"/>
+      <c r="HO36"/>
+      <c r="HP36"/>
+      <c r="HQ36"/>
+      <c r="HR36"/>
+      <c r="HS36"/>
+      <c r="HT36"/>
+      <c r="HU36"/>
+      <c r="HV36"/>
+      <c r="HW36"/>
+      <c r="HX36"/>
+      <c r="HY36"/>
+      <c r="HZ36"/>
+      <c r="IA36"/>
+      <c r="IB36"/>
+      <c r="IC36"/>
+      <c r="ID36"/>
+      <c r="IE36"/>
+      <c r="IF36"/>
+      <c r="IG36"/>
+      <c r="IH36"/>
+      <c r="II36"/>
+      <c r="IJ36"/>
+      <c r="IK36"/>
+      <c r="IL36"/>
+      <c r="IM36"/>
+      <c r="IN36"/>
+      <c r="IO36"/>
+      <c r="IP36"/>
+      <c r="IQ36"/>
+      <c r="IR36"/>
+      <c r="IS36"/>
+      <c r="IT36"/>
+      <c r="IU36"/>
+      <c r="IV36"/>
+    </row>
+    <row r="37" spans="1:256" ht="15" customHeight="1">
+      <c r="A37" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="108"/>
-      <c r="C33" s="109"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="40"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
-      <c r="AE33"/>
-      <c r="AF33"/>
-      <c r="AG33"/>
-      <c r="AH33"/>
-      <c r="AI33"/>
-      <c r="AJ33"/>
-      <c r="AK33"/>
-      <c r="AL33"/>
-      <c r="AM33"/>
-      <c r="AN33"/>
-      <c r="AO33"/>
-      <c r="AP33"/>
-      <c r="AQ33"/>
-      <c r="AR33"/>
-      <c r="AS33"/>
-      <c r="AT33"/>
-      <c r="AU33"/>
-      <c r="AV33"/>
-      <c r="AW33"/>
-      <c r="AX33"/>
-      <c r="AY33"/>
-      <c r="AZ33"/>
-      <c r="BA33"/>
-      <c r="BB33"/>
-      <c r="BC33"/>
-      <c r="BD33"/>
-      <c r="BE33"/>
-      <c r="BF33"/>
-      <c r="BG33"/>
-      <c r="BH33"/>
-      <c r="BI33"/>
-      <c r="BJ33"/>
-      <c r="BK33"/>
-      <c r="BL33"/>
-      <c r="BM33"/>
-      <c r="BN33"/>
-      <c r="BO33"/>
-      <c r="BP33"/>
-      <c r="BQ33"/>
-      <c r="BR33"/>
-      <c r="BS33"/>
-      <c r="BT33"/>
-      <c r="BU33"/>
-      <c r="BV33"/>
-      <c r="BW33"/>
-      <c r="BX33"/>
-      <c r="BY33"/>
-      <c r="BZ33"/>
-      <c r="CA33"/>
-      <c r="CB33"/>
-      <c r="CC33"/>
-      <c r="CD33"/>
-      <c r="CE33"/>
-      <c r="CF33"/>
-      <c r="CG33"/>
-      <c r="CH33"/>
-      <c r="CI33"/>
-      <c r="CJ33"/>
-      <c r="CK33"/>
-      <c r="CL33"/>
-      <c r="CM33"/>
-      <c r="CN33"/>
-      <c r="CO33"/>
-      <c r="CP33"/>
-      <c r="CQ33"/>
-      <c r="CR33"/>
-      <c r="CS33"/>
-      <c r="CT33"/>
-      <c r="CU33"/>
-      <c r="CV33"/>
-      <c r="CW33"/>
-      <c r="CX33"/>
-      <c r="CY33"/>
-      <c r="CZ33"/>
-      <c r="DA33"/>
-      <c r="DB33"/>
-      <c r="DC33"/>
-      <c r="DD33"/>
-      <c r="DE33"/>
-      <c r="DF33"/>
-      <c r="DG33"/>
-      <c r="DH33"/>
-      <c r="DI33"/>
-      <c r="DJ33"/>
-      <c r="DK33"/>
-      <c r="DL33"/>
-      <c r="DM33"/>
-      <c r="DN33"/>
-      <c r="DO33"/>
-      <c r="DP33"/>
-      <c r="DQ33"/>
-      <c r="DR33"/>
-      <c r="DS33"/>
-      <c r="DT33"/>
-      <c r="DU33"/>
-      <c r="DV33"/>
-      <c r="DW33"/>
-      <c r="DX33"/>
-      <c r="DY33"/>
-      <c r="DZ33"/>
-      <c r="EA33"/>
-      <c r="EB33"/>
-      <c r="EC33"/>
-      <c r="ED33"/>
-      <c r="EE33"/>
-      <c r="EF33"/>
-      <c r="EG33"/>
-      <c r="EH33"/>
-      <c r="EI33"/>
-      <c r="EJ33"/>
-      <c r="EK33"/>
-      <c r="EL33"/>
-      <c r="EM33"/>
-      <c r="EN33"/>
-      <c r="EO33"/>
-      <c r="EP33"/>
-      <c r="EQ33"/>
-      <c r="ER33"/>
-      <c r="ES33"/>
-      <c r="ET33"/>
-      <c r="EU33"/>
-      <c r="EV33"/>
-      <c r="EW33"/>
-      <c r="EX33"/>
-      <c r="EY33"/>
-      <c r="EZ33"/>
-      <c r="FA33"/>
-      <c r="FB33"/>
-      <c r="FC33"/>
-      <c r="FD33"/>
-      <c r="FE33"/>
-      <c r="FF33"/>
-      <c r="FG33"/>
-      <c r="FH33"/>
-      <c r="FI33"/>
-      <c r="FJ33"/>
-      <c r="FK33"/>
-      <c r="FL33"/>
-      <c r="FM33"/>
-      <c r="FN33"/>
-      <c r="FO33"/>
-      <c r="FP33"/>
-      <c r="FQ33"/>
-      <c r="FR33"/>
-      <c r="FS33"/>
-      <c r="FT33"/>
-      <c r="FU33"/>
-      <c r="FV33"/>
-      <c r="FW33"/>
-      <c r="FX33"/>
-      <c r="FY33"/>
-      <c r="FZ33"/>
-      <c r="GA33"/>
-      <c r="GB33"/>
-      <c r="GC33"/>
-      <c r="GD33"/>
-      <c r="GE33"/>
-      <c r="GF33"/>
-      <c r="GG33"/>
-      <c r="GH33"/>
-      <c r="GI33"/>
-      <c r="GJ33"/>
-      <c r="GK33"/>
-      <c r="GL33"/>
-      <c r="GM33"/>
-      <c r="GN33"/>
-      <c r="GO33"/>
-      <c r="GP33"/>
-      <c r="GQ33"/>
-      <c r="GR33"/>
-      <c r="GS33"/>
-      <c r="GT33"/>
-      <c r="GU33"/>
-      <c r="GV33"/>
-      <c r="GW33"/>
-      <c r="GX33"/>
-      <c r="GY33"/>
-      <c r="GZ33"/>
-      <c r="HA33"/>
-      <c r="HB33"/>
-      <c r="HC33"/>
-      <c r="HD33"/>
-      <c r="HE33"/>
-      <c r="HF33"/>
-      <c r="HG33"/>
-      <c r="HH33"/>
-      <c r="HI33"/>
-      <c r="HJ33"/>
-      <c r="HK33"/>
-      <c r="HL33"/>
-      <c r="HM33"/>
-      <c r="HN33"/>
-      <c r="HO33"/>
-      <c r="HP33"/>
-      <c r="HQ33"/>
-      <c r="HR33"/>
-      <c r="HS33"/>
-      <c r="HT33"/>
-      <c r="HU33"/>
-      <c r="HV33"/>
-      <c r="HW33"/>
-      <c r="HX33"/>
-      <c r="HY33"/>
-      <c r="HZ33"/>
-      <c r="IA33"/>
-      <c r="IB33"/>
-      <c r="IC33"/>
-      <c r="ID33"/>
-      <c r="IE33"/>
-      <c r="IF33"/>
-      <c r="IG33"/>
-      <c r="IH33"/>
-      <c r="II33"/>
-      <c r="IJ33"/>
-      <c r="IK33"/>
-      <c r="IL33"/>
-      <c r="IM33"/>
-      <c r="IN33"/>
-      <c r="IO33"/>
-      <c r="IP33"/>
-      <c r="IQ33"/>
-      <c r="IR33"/>
-      <c r="IS33"/>
-      <c r="IT33"/>
-      <c r="IU33"/>
-      <c r="IV33"/>
+      <c r="B37" s="112"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="40"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37"/>
+      <c r="AC37"/>
+      <c r="AD37"/>
+      <c r="AE37"/>
+      <c r="AF37"/>
+      <c r="AG37"/>
+      <c r="AH37"/>
+      <c r="AI37"/>
+      <c r="AJ37"/>
+      <c r="AK37"/>
+      <c r="AL37"/>
+      <c r="AM37"/>
+      <c r="AN37"/>
+      <c r="AO37"/>
+      <c r="AP37"/>
+      <c r="AQ37"/>
+      <c r="AR37"/>
+      <c r="AS37"/>
+      <c r="AT37"/>
+      <c r="AU37"/>
+      <c r="AV37"/>
+      <c r="AW37"/>
+      <c r="AX37"/>
+      <c r="AY37"/>
+      <c r="AZ37"/>
+      <c r="BA37"/>
+      <c r="BB37"/>
+      <c r="BC37"/>
+      <c r="BD37"/>
+      <c r="BE37"/>
+      <c r="BF37"/>
+      <c r="BG37"/>
+      <c r="BH37"/>
+      <c r="BI37"/>
+      <c r="BJ37"/>
+      <c r="BK37"/>
+      <c r="BL37"/>
+      <c r="BM37"/>
+      <c r="BN37"/>
+      <c r="BO37"/>
+      <c r="BP37"/>
+      <c r="BQ37"/>
+      <c r="BR37"/>
+      <c r="BS37"/>
+      <c r="BT37"/>
+      <c r="BU37"/>
+      <c r="BV37"/>
+      <c r="BW37"/>
+      <c r="BX37"/>
+      <c r="BY37"/>
+      <c r="BZ37"/>
+      <c r="CA37"/>
+      <c r="CB37"/>
+      <c r="CC37"/>
+      <c r="CD37"/>
+      <c r="CE37"/>
+      <c r="CF37"/>
+      <c r="CG37"/>
+      <c r="CH37"/>
+      <c r="CI37"/>
+      <c r="CJ37"/>
+      <c r="CK37"/>
+      <c r="CL37"/>
+      <c r="CM37"/>
+      <c r="CN37"/>
+      <c r="CO37"/>
+      <c r="CP37"/>
+      <c r="CQ37"/>
+      <c r="CR37"/>
+      <c r="CS37"/>
+      <c r="CT37"/>
+      <c r="CU37"/>
+      <c r="CV37"/>
+      <c r="CW37"/>
+      <c r="CX37"/>
+      <c r="CY37"/>
+      <c r="CZ37"/>
+      <c r="DA37"/>
+      <c r="DB37"/>
+      <c r="DC37"/>
+      <c r="DD37"/>
+      <c r="DE37"/>
+      <c r="DF37"/>
+      <c r="DG37"/>
+      <c r="DH37"/>
+      <c r="DI37"/>
+      <c r="DJ37"/>
+      <c r="DK37"/>
+      <c r="DL37"/>
+      <c r="DM37"/>
+      <c r="DN37"/>
+      <c r="DO37"/>
+      <c r="DP37"/>
+      <c r="DQ37"/>
+      <c r="DR37"/>
+      <c r="DS37"/>
+      <c r="DT37"/>
+      <c r="DU37"/>
+      <c r="DV37"/>
+      <c r="DW37"/>
+      <c r="DX37"/>
+      <c r="DY37"/>
+      <c r="DZ37"/>
+      <c r="EA37"/>
+      <c r="EB37"/>
+      <c r="EC37"/>
+      <c r="ED37"/>
+      <c r="EE37"/>
+      <c r="EF37"/>
+      <c r="EG37"/>
+      <c r="EH37"/>
+      <c r="EI37"/>
+      <c r="EJ37"/>
+      <c r="EK37"/>
+      <c r="EL37"/>
+      <c r="EM37"/>
+      <c r="EN37"/>
+      <c r="EO37"/>
+      <c r="EP37"/>
+      <c r="EQ37"/>
+      <c r="ER37"/>
+      <c r="ES37"/>
+      <c r="ET37"/>
+      <c r="EU37"/>
+      <c r="EV37"/>
+      <c r="EW37"/>
+      <c r="EX37"/>
+      <c r="EY37"/>
+      <c r="EZ37"/>
+      <c r="FA37"/>
+      <c r="FB37"/>
+      <c r="FC37"/>
+      <c r="FD37"/>
+      <c r="FE37"/>
+      <c r="FF37"/>
+      <c r="FG37"/>
+      <c r="FH37"/>
+      <c r="FI37"/>
+      <c r="FJ37"/>
+      <c r="FK37"/>
+      <c r="FL37"/>
+      <c r="FM37"/>
+      <c r="FN37"/>
+      <c r="FO37"/>
+      <c r="FP37"/>
+      <c r="FQ37"/>
+      <c r="FR37"/>
+      <c r="FS37"/>
+      <c r="FT37"/>
+      <c r="FU37"/>
+      <c r="FV37"/>
+      <c r="FW37"/>
+      <c r="FX37"/>
+      <c r="FY37"/>
+      <c r="FZ37"/>
+      <c r="GA37"/>
+      <c r="GB37"/>
+      <c r="GC37"/>
+      <c r="GD37"/>
+      <c r="GE37"/>
+      <c r="GF37"/>
+      <c r="GG37"/>
+      <c r="GH37"/>
+      <c r="GI37"/>
+      <c r="GJ37"/>
+      <c r="GK37"/>
+      <c r="GL37"/>
+      <c r="GM37"/>
+      <c r="GN37"/>
+      <c r="GO37"/>
+      <c r="GP37"/>
+      <c r="GQ37"/>
+      <c r="GR37"/>
+      <c r="GS37"/>
+      <c r="GT37"/>
+      <c r="GU37"/>
+      <c r="GV37"/>
+      <c r="GW37"/>
+      <c r="GX37"/>
+      <c r="GY37"/>
+      <c r="GZ37"/>
+      <c r="HA37"/>
+      <c r="HB37"/>
+      <c r="HC37"/>
+      <c r="HD37"/>
+      <c r="HE37"/>
+      <c r="HF37"/>
+      <c r="HG37"/>
+      <c r="HH37"/>
+      <c r="HI37"/>
+      <c r="HJ37"/>
+      <c r="HK37"/>
+      <c r="HL37"/>
+      <c r="HM37"/>
+      <c r="HN37"/>
+      <c r="HO37"/>
+      <c r="HP37"/>
+      <c r="HQ37"/>
+      <c r="HR37"/>
+      <c r="HS37"/>
+      <c r="HT37"/>
+      <c r="HU37"/>
+      <c r="HV37"/>
+      <c r="HW37"/>
+      <c r="HX37"/>
+      <c r="HY37"/>
+      <c r="HZ37"/>
+      <c r="IA37"/>
+      <c r="IB37"/>
+      <c r="IC37"/>
+      <c r="ID37"/>
+      <c r="IE37"/>
+      <c r="IF37"/>
+      <c r="IG37"/>
+      <c r="IH37"/>
+      <c r="II37"/>
+      <c r="IJ37"/>
+      <c r="IK37"/>
+      <c r="IL37"/>
+      <c r="IM37"/>
+      <c r="IN37"/>
+      <c r="IO37"/>
+      <c r="IP37"/>
+      <c r="IQ37"/>
+      <c r="IR37"/>
+      <c r="IS37"/>
+      <c r="IT37"/>
+      <c r="IU37"/>
+      <c r="IV37"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3712,11 +3799,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -4040,7 +4127,7 @@
       <c r="A7" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="113">
+      <c r="B7" s="103">
         <v>42792</v>
       </c>
       <c r="C7" s="89">
@@ -4308,9 +4395,9 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1">
-      <c r="A9" s="107"/>
-      <c r="B9" s="108"/>
-      <c r="C9" s="109"/>
+      <c r="A9" s="111"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="113"/>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
     </row>
@@ -4344,11 +4431,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -5054,9 +5141,9 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
-      <c r="A15" s="114"/>
-      <c r="B15" s="115"/>
-      <c r="C15" s="116"/>
+      <c r="A15" s="115"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5088,11 +5175,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -6558,9 +6645,9 @@
       <c r="IV15" s="73"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
-      <c r="A16" s="107"/>
-      <c r="B16" s="108"/>
-      <c r="C16" s="109"/>
+      <c r="A16" s="111"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="113"/>
       <c r="D16" s="38"/>
       <c r="E16" s="39"/>
       <c r="F16" s="39"/>
@@ -6843,11 +6930,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -7274,15 +7361,15 @@
       <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="111" t="s">
+      <c r="A18" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="112"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="119"/>
       <c r="H18" s="69"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización en actividades, correcciones menores a envío de correos, agregar nuevos estilos, corregir transacciones para servidor
</commit_message>
<xml_diff>
--- a/Scrum Febrero.xlsx
+++ b/Scrum Febrero.xlsx
@@ -7,23 +7,24 @@
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="10905"/>
   </bookViews>
   <sheets>
-    <sheet name="Actividades Marzo - Toño" sheetId="8" r:id="rId1"/>
-    <sheet name="Actividades Marzo - Mario" sheetId="9" r:id="rId2"/>
-    <sheet name="Actividades Marzo - Rosa" sheetId="10" r:id="rId3"/>
-    <sheet name="Actividades Febrero - Toño" sheetId="1" r:id="rId4"/>
-    <sheet name="Actividades Febrero - Mario" sheetId="2" r:id="rId5"/>
-    <sheet name="Actividades Febrero - Rosa" sheetId="3" r:id="rId6"/>
-    <sheet name="Nuevos módulos" sheetId="4" r:id="rId7"/>
-    <sheet name="Actividades Enero" sheetId="5" r:id="rId8"/>
-    <sheet name="Catálogo" sheetId="6" r:id="rId9"/>
-    <sheet name="Correo catálogos" sheetId="7" r:id="rId10"/>
+    <sheet name="Actividades Abril - Todos" sheetId="11" r:id="rId1"/>
+    <sheet name="Actividades Marzo - Toño" sheetId="8" r:id="rId2"/>
+    <sheet name="Actividades Marzo - Mario" sheetId="9" r:id="rId3"/>
+    <sheet name="Actividades Marzo - Rosa" sheetId="10" r:id="rId4"/>
+    <sheet name="Actividades Febrero - Toño" sheetId="1" r:id="rId5"/>
+    <sheet name="Actividades Febrero - Mario" sheetId="2" r:id="rId6"/>
+    <sheet name="Actividades Febrero - Rosa" sheetId="3" r:id="rId7"/>
+    <sheet name="Nuevos módulos" sheetId="4" r:id="rId8"/>
+    <sheet name="Actividades Enero" sheetId="5" r:id="rId9"/>
+    <sheet name="Catálogo" sheetId="6" r:id="rId10"/>
+    <sheet name="Correo catálogos" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="138">
   <si>
     <t>TOÑO</t>
   </si>
@@ -413,6 +414,30 @@
   </si>
   <si>
     <t>Cotizaciones - Cambiar vista inicial de contacto a inactivos (como cuando se recarga)</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Toño</t>
+  </si>
+  <si>
+    <t>No hay acceso al servidor</t>
+  </si>
+  <si>
+    <t>Formato de diagnóstico - Subir archivos renombrados y guardar en base de datos</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Rosa</t>
+  </si>
+  <si>
+    <t>Perfil del cliente - Carga de datos</t>
+  </si>
+  <si>
+    <t>Perfil del cliente - Inserción en base de datos</t>
   </si>
 </sst>
 </file>
@@ -490,7 +515,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -867,11 +892,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -996,6 +1032,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1032,9 +1073,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2245,26 +2286,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV19"/>
+  <dimension ref="A1:IV25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="59.85546875" style="73" customWidth="1"/>
+    <col min="1" max="1" width="80.5703125" style="73" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="73" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="73" customWidth="1"/>
     <col min="4" max="256" width="8.85546875" style="73" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="104" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
+      <c r="A1" s="109" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -2275,161 +2316,229 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
+      <c r="C2" s="89" t="s">
+        <v>130</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B3" s="10">
-        <v>42806</v>
-      </c>
-      <c r="C3" s="89"/>
+        <v>42834</v>
+      </c>
+      <c r="C3" s="125" t="s">
+        <v>131</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="9" t="s">
-        <v>8</v>
+      <c r="A4" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="B4" s="10">
-        <v>42806</v>
-      </c>
-      <c r="C4" s="89"/>
+        <v>42834</v>
+      </c>
+      <c r="C4" s="125" t="s">
+        <v>134</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="9" t="s">
-        <v>12</v>
+    <row r="5" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="40" t="s">
+        <v>128</v>
       </c>
       <c r="B5" s="10">
-        <v>42806</v>
-      </c>
-      <c r="C5" s="89"/>
+        <v>42834</v>
+      </c>
+      <c r="C5" s="125" t="s">
+        <v>135</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="84" t="s">
-        <v>124</v>
+    <row r="6" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="127" t="s">
+        <v>136</v>
       </c>
       <c r="B6" s="10">
-        <v>42806</v>
-      </c>
-      <c r="C6" s="89"/>
+        <v>42834</v>
+      </c>
+      <c r="C6" s="125" t="s">
+        <v>135</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
+    <row r="7" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="84" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="10">
+        <v>42834</v>
+      </c>
+      <c r="C7" s="89"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="106" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="19"/>
+    <row r="8" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A8" s="105" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="10">
+        <v>42834</v>
+      </c>
+      <c r="C8" s="89"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
+    <row r="9" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="93"/>
-      <c r="C10" s="94"/>
+    <row r="10" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
+    <row r="11" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="111" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="112"/>
+      <c r="C11" s="112"/>
       <c r="D11" s="19"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="21"/>
+    <row r="12" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="10"/>
       <c r="C12" s="22"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="126" t="s">
+        <v>132</v>
+      </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A14" s="29"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="7"/>
+    <row r="14" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="105" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="126" t="s">
+        <v>132</v>
+      </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="94"/>
+    <row r="15" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A15" s="86"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A16" s="29"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="94"/>
+    <row r="16" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="9"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="108"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A17" s="29"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="7"/>
+    <row r="17" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A17" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="108" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="110"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="111" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="107"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A20" s="29"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A21" s="29"/>
+      <c r="B21" s="107"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A22" s="29"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A23" s="29"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A24" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="114"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A25" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="112"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2447,6 +2556,157 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
+    <col min="1" max="1" width="37" style="70" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="70" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="70" customWidth="1"/>
+    <col min="5" max="5" width="54.85546875" style="70" customWidth="1"/>
+    <col min="6" max="256" width="8.85546875" style="70" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1">
+      <c r="A2" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="23"/>
+      <c r="B6" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="23">
+        <v>3</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1">
+      <c r="A9" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="24">
+        <v>10</v>
+      </c>
+      <c r="C9" s="24">
+        <v>12</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="71"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="71"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <cols>
     <col min="1" max="1" width="119.85546875" style="73" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="73" customWidth="1"/>
     <col min="3" max="256" width="8.85546875" style="73" customWidth="1"/>
@@ -2570,10 +2830,208 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="59.85546875" style="73" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="4" max="256" width="8.85546875" style="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="109" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="89"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10">
+        <v>42820</v>
+      </c>
+      <c r="C3" s="89"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10">
+        <v>42820</v>
+      </c>
+      <c r="C4" s="89">
+        <v>42819</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10">
+        <v>42820</v>
+      </c>
+      <c r="C5" s="89"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="13">
+        <v>42820</v>
+      </c>
+      <c r="C6" s="89">
+        <v>42819</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="111" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="112"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="29"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A14" s="29"/>
+      <c r="B14" s="93"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A15" s="29"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A16" s="29"/>
+      <c r="B16" s="93"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A17" s="29"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A18" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="114"/>
+      <c r="C18" s="115"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A19" s="116" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="117"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2585,11 +3043,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2617,7 +3075,7 @@
         <v>122</v>
       </c>
       <c r="B3" s="10">
-        <v>42806</v>
+        <v>42820</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="7"/>
@@ -2631,7 +3089,7 @@
         <v>121</v>
       </c>
       <c r="B4" s="10">
-        <v>42778</v>
+        <v>42820</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="7"/>
@@ -2663,7 +3121,7 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="106" t="s">
         <v>128</v>
       </c>
       <c r="B7" s="10"/>
@@ -2766,18 +3224,23 @@
       </c>
       <c r="B16" s="93"/>
       <c r="C16" s="94"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="1:3" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="D16" s="7"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="97" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="98"/>
       <c r="C17" s="99"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2791,12 +3254,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV37"/>
+  <dimension ref="A1:IV39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A18" sqref="A17:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2808,11 +3271,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2840,7 +3303,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="10">
-        <v>42792</v>
+        <v>42820</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="33"/>
@@ -2946,13 +3409,15 @@
       <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="121">
-        <v>42806</v>
-      </c>
-      <c r="C10" s="14"/>
+      <c r="B10" s="13">
+        <v>42820</v>
+      </c>
+      <c r="C10" s="14">
+        <v>42819</v>
+      </c>
       <c r="D10" s="33"/>
       <c r="E10" s="102"/>
       <c r="F10" s="102"/>
@@ -2970,32 +3435,28 @@
       <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="33"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96"/>
+      <c r="E12" s="104"/>
+      <c r="F12" s="104"/>
+      <c r="G12" s="104"/>
       <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="A13" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="A13" s="9"/>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="33"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="96"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="104"/>
       <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
@@ -3006,8 +3467,8 @@
       <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="12" t="s">
-        <v>123</v>
+      <c r="A15" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
@@ -3018,8 +3479,8 @@
       <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="12" t="s">
-        <v>44</v>
+      <c r="A16" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
@@ -3030,33 +3491,33 @@
       <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="8"/>
+      <c r="A17" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="114" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="107"/>
-      <c r="C18" s="107"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="8"/>
+      <c r="A18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1">
-      <c r="A19" s="83" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="7"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
@@ -3064,32 +3525,32 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1">
-      <c r="A20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="93"/>
-      <c r="C20" s="94"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="34"/>
+      <c r="A20" s="119" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="112"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1">
-      <c r="A21" s="120" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="100"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="34"/>
+      <c r="A21" s="83" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B22" s="93"/>
       <c r="C22" s="94"/>
@@ -3100,20 +3561,20 @@
       <c r="H22" s="34"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="94"/>
+      <c r="A23" s="105" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="100"/>
+      <c r="C23" s="101"/>
       <c r="D23" s="33"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
       <c r="H23" s="34"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="79" t="s">
-        <v>109</v>
+      <c r="A24" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="B24" s="93"/>
       <c r="C24" s="94"/>
@@ -3124,8 +3585,8 @@
       <c r="H24" s="34"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="79" t="s">
-        <v>50</v>
+      <c r="A25" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="B25" s="93"/>
       <c r="C25" s="94"/>
@@ -3136,8 +3597,8 @@
       <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="12" t="s">
-        <v>114</v>
+      <c r="A26" s="79" t="s">
+        <v>109</v>
       </c>
       <c r="B26" s="93"/>
       <c r="C26" s="94"/>
@@ -3148,8 +3609,8 @@
       <c r="H26" s="34"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="9" t="s">
-        <v>46</v>
+      <c r="A27" s="79" t="s">
+        <v>50</v>
       </c>
       <c r="B27" s="93"/>
       <c r="C27" s="94"/>
@@ -3160,8 +3621,8 @@
       <c r="H27" s="34"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1">
-      <c r="A28" s="9" t="s">
-        <v>47</v>
+      <c r="A28" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="B28" s="93"/>
       <c r="C28" s="94"/>
@@ -3173,7 +3634,7 @@
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B29" s="93"/>
       <c r="C29" s="94"/>
@@ -3184,11 +3645,11 @@
       <c r="H29" s="34"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30" s="84" t="s">
-        <v>119</v>
-      </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="93"/>
+      <c r="C30" s="94"/>
       <c r="D30" s="33"/>
       <c r="E30" s="96"/>
       <c r="F30" s="96"/>
@@ -3196,9 +3657,11 @@
       <c r="H30" s="34"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1">
-      <c r="A31" s="84"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="93"/>
+      <c r="C31" s="94"/>
       <c r="D31" s="33"/>
       <c r="E31" s="96"/>
       <c r="F31" s="96"/>
@@ -3206,573 +3669,595 @@
       <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1">
-      <c r="A32" s="15"/>
+      <c r="A32" s="84" t="s">
+        <v>119</v>
+      </c>
       <c r="B32" s="24"/>
       <c r="C32" s="25"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="8"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="34"/>
     </row>
     <row r="33" spans="1:256" ht="15" customHeight="1">
-      <c r="A33" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="96"/>
+      <c r="A33" s="84"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="96"/>
       <c r="F33" s="96"/>
       <c r="G33" s="96"/>
       <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:256" ht="15" customHeight="1">
-      <c r="A34" s="28"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="96"/>
-      <c r="F34" s="96"/>
-      <c r="G34" s="96"/>
-      <c r="H34" s="34"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:256" ht="15" customHeight="1">
-      <c r="A35" s="29"/>
-      <c r="B35" s="93"/>
-      <c r="C35" s="94"/>
-      <c r="D35" s="33"/>
+      <c r="A35" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="96"/>
       <c r="E35" s="96"/>
       <c r="F35" s="96"/>
       <c r="G35" s="96"/>
       <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:256" ht="15" customHeight="1">
-      <c r="A36" s="108" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="109"/>
-      <c r="C36" s="110"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="33"/>
       <c r="E36" s="96"/>
       <c r="F36" s="96"/>
       <c r="G36" s="96"/>
       <c r="H36" s="34"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-      <c r="X36"/>
-      <c r="Y36"/>
-      <c r="Z36"/>
-      <c r="AA36"/>
-      <c r="AB36"/>
-      <c r="AC36"/>
-      <c r="AD36"/>
-      <c r="AE36"/>
-      <c r="AF36"/>
-      <c r="AG36"/>
-      <c r="AH36"/>
-      <c r="AI36"/>
-      <c r="AJ36"/>
-      <c r="AK36"/>
-      <c r="AL36"/>
-      <c r="AM36"/>
-      <c r="AN36"/>
-      <c r="AO36"/>
-      <c r="AP36"/>
-      <c r="AQ36"/>
-      <c r="AR36"/>
-      <c r="AS36"/>
-      <c r="AT36"/>
-      <c r="AU36"/>
-      <c r="AV36"/>
-      <c r="AW36"/>
-      <c r="AX36"/>
-      <c r="AY36"/>
-      <c r="AZ36"/>
-      <c r="BA36"/>
-      <c r="BB36"/>
-      <c r="BC36"/>
-      <c r="BD36"/>
-      <c r="BE36"/>
-      <c r="BF36"/>
-      <c r="BG36"/>
-      <c r="BH36"/>
-      <c r="BI36"/>
-      <c r="BJ36"/>
-      <c r="BK36"/>
-      <c r="BL36"/>
-      <c r="BM36"/>
-      <c r="BN36"/>
-      <c r="BO36"/>
-      <c r="BP36"/>
-      <c r="BQ36"/>
-      <c r="BR36"/>
-      <c r="BS36"/>
-      <c r="BT36"/>
-      <c r="BU36"/>
-      <c r="BV36"/>
-      <c r="BW36"/>
-      <c r="BX36"/>
-      <c r="BY36"/>
-      <c r="BZ36"/>
-      <c r="CA36"/>
-      <c r="CB36"/>
-      <c r="CC36"/>
-      <c r="CD36"/>
-      <c r="CE36"/>
-      <c r="CF36"/>
-      <c r="CG36"/>
-      <c r="CH36"/>
-      <c r="CI36"/>
-      <c r="CJ36"/>
-      <c r="CK36"/>
-      <c r="CL36"/>
-      <c r="CM36"/>
-      <c r="CN36"/>
-      <c r="CO36"/>
-      <c r="CP36"/>
-      <c r="CQ36"/>
-      <c r="CR36"/>
-      <c r="CS36"/>
-      <c r="CT36"/>
-      <c r="CU36"/>
-      <c r="CV36"/>
-      <c r="CW36"/>
-      <c r="CX36"/>
-      <c r="CY36"/>
-      <c r="CZ36"/>
-      <c r="DA36"/>
-      <c r="DB36"/>
-      <c r="DC36"/>
-      <c r="DD36"/>
-      <c r="DE36"/>
-      <c r="DF36"/>
-      <c r="DG36"/>
-      <c r="DH36"/>
-      <c r="DI36"/>
-      <c r="DJ36"/>
-      <c r="DK36"/>
-      <c r="DL36"/>
-      <c r="DM36"/>
-      <c r="DN36"/>
-      <c r="DO36"/>
-      <c r="DP36"/>
-      <c r="DQ36"/>
-      <c r="DR36"/>
-      <c r="DS36"/>
-      <c r="DT36"/>
-      <c r="DU36"/>
-      <c r="DV36"/>
-      <c r="DW36"/>
-      <c r="DX36"/>
-      <c r="DY36"/>
-      <c r="DZ36"/>
-      <c r="EA36"/>
-      <c r="EB36"/>
-      <c r="EC36"/>
-      <c r="ED36"/>
-      <c r="EE36"/>
-      <c r="EF36"/>
-      <c r="EG36"/>
-      <c r="EH36"/>
-      <c r="EI36"/>
-      <c r="EJ36"/>
-      <c r="EK36"/>
-      <c r="EL36"/>
-      <c r="EM36"/>
-      <c r="EN36"/>
-      <c r="EO36"/>
-      <c r="EP36"/>
-      <c r="EQ36"/>
-      <c r="ER36"/>
-      <c r="ES36"/>
-      <c r="ET36"/>
-      <c r="EU36"/>
-      <c r="EV36"/>
-      <c r="EW36"/>
-      <c r="EX36"/>
-      <c r="EY36"/>
-      <c r="EZ36"/>
-      <c r="FA36"/>
-      <c r="FB36"/>
-      <c r="FC36"/>
-      <c r="FD36"/>
-      <c r="FE36"/>
-      <c r="FF36"/>
-      <c r="FG36"/>
-      <c r="FH36"/>
-      <c r="FI36"/>
-      <c r="FJ36"/>
-      <c r="FK36"/>
-      <c r="FL36"/>
-      <c r="FM36"/>
-      <c r="FN36"/>
-      <c r="FO36"/>
-      <c r="FP36"/>
-      <c r="FQ36"/>
-      <c r="FR36"/>
-      <c r="FS36"/>
-      <c r="FT36"/>
-      <c r="FU36"/>
-      <c r="FV36"/>
-      <c r="FW36"/>
-      <c r="FX36"/>
-      <c r="FY36"/>
-      <c r="FZ36"/>
-      <c r="GA36"/>
-      <c r="GB36"/>
-      <c r="GC36"/>
-      <c r="GD36"/>
-      <c r="GE36"/>
-      <c r="GF36"/>
-      <c r="GG36"/>
-      <c r="GH36"/>
-      <c r="GI36"/>
-      <c r="GJ36"/>
-      <c r="GK36"/>
-      <c r="GL36"/>
-      <c r="GM36"/>
-      <c r="GN36"/>
-      <c r="GO36"/>
-      <c r="GP36"/>
-      <c r="GQ36"/>
-      <c r="GR36"/>
-      <c r="GS36"/>
-      <c r="GT36"/>
-      <c r="GU36"/>
-      <c r="GV36"/>
-      <c r="GW36"/>
-      <c r="GX36"/>
-      <c r="GY36"/>
-      <c r="GZ36"/>
-      <c r="HA36"/>
-      <c r="HB36"/>
-      <c r="HC36"/>
-      <c r="HD36"/>
-      <c r="HE36"/>
-      <c r="HF36"/>
-      <c r="HG36"/>
-      <c r="HH36"/>
-      <c r="HI36"/>
-      <c r="HJ36"/>
-      <c r="HK36"/>
-      <c r="HL36"/>
-      <c r="HM36"/>
-      <c r="HN36"/>
-      <c r="HO36"/>
-      <c r="HP36"/>
-      <c r="HQ36"/>
-      <c r="HR36"/>
-      <c r="HS36"/>
-      <c r="HT36"/>
-      <c r="HU36"/>
-      <c r="HV36"/>
-      <c r="HW36"/>
-      <c r="HX36"/>
-      <c r="HY36"/>
-      <c r="HZ36"/>
-      <c r="IA36"/>
-      <c r="IB36"/>
-      <c r="IC36"/>
-      <c r="ID36"/>
-      <c r="IE36"/>
-      <c r="IF36"/>
-      <c r="IG36"/>
-      <c r="IH36"/>
-      <c r="II36"/>
-      <c r="IJ36"/>
-      <c r="IK36"/>
-      <c r="IL36"/>
-      <c r="IM36"/>
-      <c r="IN36"/>
-      <c r="IO36"/>
-      <c r="IP36"/>
-      <c r="IQ36"/>
-      <c r="IR36"/>
-      <c r="IS36"/>
-      <c r="IT36"/>
-      <c r="IU36"/>
-      <c r="IV36"/>
     </row>
     <row r="37" spans="1:256" ht="15" customHeight="1">
-      <c r="A37" s="111" t="s">
+      <c r="A37" s="29"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="96"/>
+      <c r="F37" s="96"/>
+      <c r="G37" s="96"/>
+      <c r="H37" s="34"/>
+    </row>
+    <row r="38" spans="1:256" ht="15" customHeight="1">
+      <c r="A38" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="114"/>
+      <c r="C38" s="115"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="96"/>
+      <c r="G38" s="96"/>
+      <c r="H38" s="34"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+      <c r="Z38"/>
+      <c r="AA38"/>
+      <c r="AB38"/>
+      <c r="AC38"/>
+      <c r="AD38"/>
+      <c r="AE38"/>
+      <c r="AF38"/>
+      <c r="AG38"/>
+      <c r="AH38"/>
+      <c r="AI38"/>
+      <c r="AJ38"/>
+      <c r="AK38"/>
+      <c r="AL38"/>
+      <c r="AM38"/>
+      <c r="AN38"/>
+      <c r="AO38"/>
+      <c r="AP38"/>
+      <c r="AQ38"/>
+      <c r="AR38"/>
+      <c r="AS38"/>
+      <c r="AT38"/>
+      <c r="AU38"/>
+      <c r="AV38"/>
+      <c r="AW38"/>
+      <c r="AX38"/>
+      <c r="AY38"/>
+      <c r="AZ38"/>
+      <c r="BA38"/>
+      <c r="BB38"/>
+      <c r="BC38"/>
+      <c r="BD38"/>
+      <c r="BE38"/>
+      <c r="BF38"/>
+      <c r="BG38"/>
+      <c r="BH38"/>
+      <c r="BI38"/>
+      <c r="BJ38"/>
+      <c r="BK38"/>
+      <c r="BL38"/>
+      <c r="BM38"/>
+      <c r="BN38"/>
+      <c r="BO38"/>
+      <c r="BP38"/>
+      <c r="BQ38"/>
+      <c r="BR38"/>
+      <c r="BS38"/>
+      <c r="BT38"/>
+      <c r="BU38"/>
+      <c r="BV38"/>
+      <c r="BW38"/>
+      <c r="BX38"/>
+      <c r="BY38"/>
+      <c r="BZ38"/>
+      <c r="CA38"/>
+      <c r="CB38"/>
+      <c r="CC38"/>
+      <c r="CD38"/>
+      <c r="CE38"/>
+      <c r="CF38"/>
+      <c r="CG38"/>
+      <c r="CH38"/>
+      <c r="CI38"/>
+      <c r="CJ38"/>
+      <c r="CK38"/>
+      <c r="CL38"/>
+      <c r="CM38"/>
+      <c r="CN38"/>
+      <c r="CO38"/>
+      <c r="CP38"/>
+      <c r="CQ38"/>
+      <c r="CR38"/>
+      <c r="CS38"/>
+      <c r="CT38"/>
+      <c r="CU38"/>
+      <c r="CV38"/>
+      <c r="CW38"/>
+      <c r="CX38"/>
+      <c r="CY38"/>
+      <c r="CZ38"/>
+      <c r="DA38"/>
+      <c r="DB38"/>
+      <c r="DC38"/>
+      <c r="DD38"/>
+      <c r="DE38"/>
+      <c r="DF38"/>
+      <c r="DG38"/>
+      <c r="DH38"/>
+      <c r="DI38"/>
+      <c r="DJ38"/>
+      <c r="DK38"/>
+      <c r="DL38"/>
+      <c r="DM38"/>
+      <c r="DN38"/>
+      <c r="DO38"/>
+      <c r="DP38"/>
+      <c r="DQ38"/>
+      <c r="DR38"/>
+      <c r="DS38"/>
+      <c r="DT38"/>
+      <c r="DU38"/>
+      <c r="DV38"/>
+      <c r="DW38"/>
+      <c r="DX38"/>
+      <c r="DY38"/>
+      <c r="DZ38"/>
+      <c r="EA38"/>
+      <c r="EB38"/>
+      <c r="EC38"/>
+      <c r="ED38"/>
+      <c r="EE38"/>
+      <c r="EF38"/>
+      <c r="EG38"/>
+      <c r="EH38"/>
+      <c r="EI38"/>
+      <c r="EJ38"/>
+      <c r="EK38"/>
+      <c r="EL38"/>
+      <c r="EM38"/>
+      <c r="EN38"/>
+      <c r="EO38"/>
+      <c r="EP38"/>
+      <c r="EQ38"/>
+      <c r="ER38"/>
+      <c r="ES38"/>
+      <c r="ET38"/>
+      <c r="EU38"/>
+      <c r="EV38"/>
+      <c r="EW38"/>
+      <c r="EX38"/>
+      <c r="EY38"/>
+      <c r="EZ38"/>
+      <c r="FA38"/>
+      <c r="FB38"/>
+      <c r="FC38"/>
+      <c r="FD38"/>
+      <c r="FE38"/>
+      <c r="FF38"/>
+      <c r="FG38"/>
+      <c r="FH38"/>
+      <c r="FI38"/>
+      <c r="FJ38"/>
+      <c r="FK38"/>
+      <c r="FL38"/>
+      <c r="FM38"/>
+      <c r="FN38"/>
+      <c r="FO38"/>
+      <c r="FP38"/>
+      <c r="FQ38"/>
+      <c r="FR38"/>
+      <c r="FS38"/>
+      <c r="FT38"/>
+      <c r="FU38"/>
+      <c r="FV38"/>
+      <c r="FW38"/>
+      <c r="FX38"/>
+      <c r="FY38"/>
+      <c r="FZ38"/>
+      <c r="GA38"/>
+      <c r="GB38"/>
+      <c r="GC38"/>
+      <c r="GD38"/>
+      <c r="GE38"/>
+      <c r="GF38"/>
+      <c r="GG38"/>
+      <c r="GH38"/>
+      <c r="GI38"/>
+      <c r="GJ38"/>
+      <c r="GK38"/>
+      <c r="GL38"/>
+      <c r="GM38"/>
+      <c r="GN38"/>
+      <c r="GO38"/>
+      <c r="GP38"/>
+      <c r="GQ38"/>
+      <c r="GR38"/>
+      <c r="GS38"/>
+      <c r="GT38"/>
+      <c r="GU38"/>
+      <c r="GV38"/>
+      <c r="GW38"/>
+      <c r="GX38"/>
+      <c r="GY38"/>
+      <c r="GZ38"/>
+      <c r="HA38"/>
+      <c r="HB38"/>
+      <c r="HC38"/>
+      <c r="HD38"/>
+      <c r="HE38"/>
+      <c r="HF38"/>
+      <c r="HG38"/>
+      <c r="HH38"/>
+      <c r="HI38"/>
+      <c r="HJ38"/>
+      <c r="HK38"/>
+      <c r="HL38"/>
+      <c r="HM38"/>
+      <c r="HN38"/>
+      <c r="HO38"/>
+      <c r="HP38"/>
+      <c r="HQ38"/>
+      <c r="HR38"/>
+      <c r="HS38"/>
+      <c r="HT38"/>
+      <c r="HU38"/>
+      <c r="HV38"/>
+      <c r="HW38"/>
+      <c r="HX38"/>
+      <c r="HY38"/>
+      <c r="HZ38"/>
+      <c r="IA38"/>
+      <c r="IB38"/>
+      <c r="IC38"/>
+      <c r="ID38"/>
+      <c r="IE38"/>
+      <c r="IF38"/>
+      <c r="IG38"/>
+      <c r="IH38"/>
+      <c r="II38"/>
+      <c r="IJ38"/>
+      <c r="IK38"/>
+      <c r="IL38"/>
+      <c r="IM38"/>
+      <c r="IN38"/>
+      <c r="IO38"/>
+      <c r="IP38"/>
+      <c r="IQ38"/>
+      <c r="IR38"/>
+      <c r="IS38"/>
+      <c r="IT38"/>
+      <c r="IU38"/>
+      <c r="IV38"/>
+    </row>
+    <row r="39" spans="1:256" ht="15" customHeight="1">
+      <c r="A39" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="112"/>
-      <c r="C37" s="113"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="40"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-      <c r="N37"/>
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
-      <c r="Y37"/>
-      <c r="Z37"/>
-      <c r="AA37"/>
-      <c r="AB37"/>
-      <c r="AC37"/>
-      <c r="AD37"/>
-      <c r="AE37"/>
-      <c r="AF37"/>
-      <c r="AG37"/>
-      <c r="AH37"/>
-      <c r="AI37"/>
-      <c r="AJ37"/>
-      <c r="AK37"/>
-      <c r="AL37"/>
-      <c r="AM37"/>
-      <c r="AN37"/>
-      <c r="AO37"/>
-      <c r="AP37"/>
-      <c r="AQ37"/>
-      <c r="AR37"/>
-      <c r="AS37"/>
-      <c r="AT37"/>
-      <c r="AU37"/>
-      <c r="AV37"/>
-      <c r="AW37"/>
-      <c r="AX37"/>
-      <c r="AY37"/>
-      <c r="AZ37"/>
-      <c r="BA37"/>
-      <c r="BB37"/>
-      <c r="BC37"/>
-      <c r="BD37"/>
-      <c r="BE37"/>
-      <c r="BF37"/>
-      <c r="BG37"/>
-      <c r="BH37"/>
-      <c r="BI37"/>
-      <c r="BJ37"/>
-      <c r="BK37"/>
-      <c r="BL37"/>
-      <c r="BM37"/>
-      <c r="BN37"/>
-      <c r="BO37"/>
-      <c r="BP37"/>
-      <c r="BQ37"/>
-      <c r="BR37"/>
-      <c r="BS37"/>
-      <c r="BT37"/>
-      <c r="BU37"/>
-      <c r="BV37"/>
-      <c r="BW37"/>
-      <c r="BX37"/>
-      <c r="BY37"/>
-      <c r="BZ37"/>
-      <c r="CA37"/>
-      <c r="CB37"/>
-      <c r="CC37"/>
-      <c r="CD37"/>
-      <c r="CE37"/>
-      <c r="CF37"/>
-      <c r="CG37"/>
-      <c r="CH37"/>
-      <c r="CI37"/>
-      <c r="CJ37"/>
-      <c r="CK37"/>
-      <c r="CL37"/>
-      <c r="CM37"/>
-      <c r="CN37"/>
-      <c r="CO37"/>
-      <c r="CP37"/>
-      <c r="CQ37"/>
-      <c r="CR37"/>
-      <c r="CS37"/>
-      <c r="CT37"/>
-      <c r="CU37"/>
-      <c r="CV37"/>
-      <c r="CW37"/>
-      <c r="CX37"/>
-      <c r="CY37"/>
-      <c r="CZ37"/>
-      <c r="DA37"/>
-      <c r="DB37"/>
-      <c r="DC37"/>
-      <c r="DD37"/>
-      <c r="DE37"/>
-      <c r="DF37"/>
-      <c r="DG37"/>
-      <c r="DH37"/>
-      <c r="DI37"/>
-      <c r="DJ37"/>
-      <c r="DK37"/>
-      <c r="DL37"/>
-      <c r="DM37"/>
-      <c r="DN37"/>
-      <c r="DO37"/>
-      <c r="DP37"/>
-      <c r="DQ37"/>
-      <c r="DR37"/>
-      <c r="DS37"/>
-      <c r="DT37"/>
-      <c r="DU37"/>
-      <c r="DV37"/>
-      <c r="DW37"/>
-      <c r="DX37"/>
-      <c r="DY37"/>
-      <c r="DZ37"/>
-      <c r="EA37"/>
-      <c r="EB37"/>
-      <c r="EC37"/>
-      <c r="ED37"/>
-      <c r="EE37"/>
-      <c r="EF37"/>
-      <c r="EG37"/>
-      <c r="EH37"/>
-      <c r="EI37"/>
-      <c r="EJ37"/>
-      <c r="EK37"/>
-      <c r="EL37"/>
-      <c r="EM37"/>
-      <c r="EN37"/>
-      <c r="EO37"/>
-      <c r="EP37"/>
-      <c r="EQ37"/>
-      <c r="ER37"/>
-      <c r="ES37"/>
-      <c r="ET37"/>
-      <c r="EU37"/>
-      <c r="EV37"/>
-      <c r="EW37"/>
-      <c r="EX37"/>
-      <c r="EY37"/>
-      <c r="EZ37"/>
-      <c r="FA37"/>
-      <c r="FB37"/>
-      <c r="FC37"/>
-      <c r="FD37"/>
-      <c r="FE37"/>
-      <c r="FF37"/>
-      <c r="FG37"/>
-      <c r="FH37"/>
-      <c r="FI37"/>
-      <c r="FJ37"/>
-      <c r="FK37"/>
-      <c r="FL37"/>
-      <c r="FM37"/>
-      <c r="FN37"/>
-      <c r="FO37"/>
-      <c r="FP37"/>
-      <c r="FQ37"/>
-      <c r="FR37"/>
-      <c r="FS37"/>
-      <c r="FT37"/>
-      <c r="FU37"/>
-      <c r="FV37"/>
-      <c r="FW37"/>
-      <c r="FX37"/>
-      <c r="FY37"/>
-      <c r="FZ37"/>
-      <c r="GA37"/>
-      <c r="GB37"/>
-      <c r="GC37"/>
-      <c r="GD37"/>
-      <c r="GE37"/>
-      <c r="GF37"/>
-      <c r="GG37"/>
-      <c r="GH37"/>
-      <c r="GI37"/>
-      <c r="GJ37"/>
-      <c r="GK37"/>
-      <c r="GL37"/>
-      <c r="GM37"/>
-      <c r="GN37"/>
-      <c r="GO37"/>
-      <c r="GP37"/>
-      <c r="GQ37"/>
-      <c r="GR37"/>
-      <c r="GS37"/>
-      <c r="GT37"/>
-      <c r="GU37"/>
-      <c r="GV37"/>
-      <c r="GW37"/>
-      <c r="GX37"/>
-      <c r="GY37"/>
-      <c r="GZ37"/>
-      <c r="HA37"/>
-      <c r="HB37"/>
-      <c r="HC37"/>
-      <c r="HD37"/>
-      <c r="HE37"/>
-      <c r="HF37"/>
-      <c r="HG37"/>
-      <c r="HH37"/>
-      <c r="HI37"/>
-      <c r="HJ37"/>
-      <c r="HK37"/>
-      <c r="HL37"/>
-      <c r="HM37"/>
-      <c r="HN37"/>
-      <c r="HO37"/>
-      <c r="HP37"/>
-      <c r="HQ37"/>
-      <c r="HR37"/>
-      <c r="HS37"/>
-      <c r="HT37"/>
-      <c r="HU37"/>
-      <c r="HV37"/>
-      <c r="HW37"/>
-      <c r="HX37"/>
-      <c r="HY37"/>
-      <c r="HZ37"/>
-      <c r="IA37"/>
-      <c r="IB37"/>
-      <c r="IC37"/>
-      <c r="ID37"/>
-      <c r="IE37"/>
-      <c r="IF37"/>
-      <c r="IG37"/>
-      <c r="IH37"/>
-      <c r="II37"/>
-      <c r="IJ37"/>
-      <c r="IK37"/>
-      <c r="IL37"/>
-      <c r="IM37"/>
-      <c r="IN37"/>
-      <c r="IO37"/>
-      <c r="IP37"/>
-      <c r="IQ37"/>
-      <c r="IR37"/>
-      <c r="IS37"/>
-      <c r="IT37"/>
-      <c r="IU37"/>
-      <c r="IV37"/>
+      <c r="B39" s="117"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="40"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+      <c r="Z39"/>
+      <c r="AA39"/>
+      <c r="AB39"/>
+      <c r="AC39"/>
+      <c r="AD39"/>
+      <c r="AE39"/>
+      <c r="AF39"/>
+      <c r="AG39"/>
+      <c r="AH39"/>
+      <c r="AI39"/>
+      <c r="AJ39"/>
+      <c r="AK39"/>
+      <c r="AL39"/>
+      <c r="AM39"/>
+      <c r="AN39"/>
+      <c r="AO39"/>
+      <c r="AP39"/>
+      <c r="AQ39"/>
+      <c r="AR39"/>
+      <c r="AS39"/>
+      <c r="AT39"/>
+      <c r="AU39"/>
+      <c r="AV39"/>
+      <c r="AW39"/>
+      <c r="AX39"/>
+      <c r="AY39"/>
+      <c r="AZ39"/>
+      <c r="BA39"/>
+      <c r="BB39"/>
+      <c r="BC39"/>
+      <c r="BD39"/>
+      <c r="BE39"/>
+      <c r="BF39"/>
+      <c r="BG39"/>
+      <c r="BH39"/>
+      <c r="BI39"/>
+      <c r="BJ39"/>
+      <c r="BK39"/>
+      <c r="BL39"/>
+      <c r="BM39"/>
+      <c r="BN39"/>
+      <c r="BO39"/>
+      <c r="BP39"/>
+      <c r="BQ39"/>
+      <c r="BR39"/>
+      <c r="BS39"/>
+      <c r="BT39"/>
+      <c r="BU39"/>
+      <c r="BV39"/>
+      <c r="BW39"/>
+      <c r="BX39"/>
+      <c r="BY39"/>
+      <c r="BZ39"/>
+      <c r="CA39"/>
+      <c r="CB39"/>
+      <c r="CC39"/>
+      <c r="CD39"/>
+      <c r="CE39"/>
+      <c r="CF39"/>
+      <c r="CG39"/>
+      <c r="CH39"/>
+      <c r="CI39"/>
+      <c r="CJ39"/>
+      <c r="CK39"/>
+      <c r="CL39"/>
+      <c r="CM39"/>
+      <c r="CN39"/>
+      <c r="CO39"/>
+      <c r="CP39"/>
+      <c r="CQ39"/>
+      <c r="CR39"/>
+      <c r="CS39"/>
+      <c r="CT39"/>
+      <c r="CU39"/>
+      <c r="CV39"/>
+      <c r="CW39"/>
+      <c r="CX39"/>
+      <c r="CY39"/>
+      <c r="CZ39"/>
+      <c r="DA39"/>
+      <c r="DB39"/>
+      <c r="DC39"/>
+      <c r="DD39"/>
+      <c r="DE39"/>
+      <c r="DF39"/>
+      <c r="DG39"/>
+      <c r="DH39"/>
+      <c r="DI39"/>
+      <c r="DJ39"/>
+      <c r="DK39"/>
+      <c r="DL39"/>
+      <c r="DM39"/>
+      <c r="DN39"/>
+      <c r="DO39"/>
+      <c r="DP39"/>
+      <c r="DQ39"/>
+      <c r="DR39"/>
+      <c r="DS39"/>
+      <c r="DT39"/>
+      <c r="DU39"/>
+      <c r="DV39"/>
+      <c r="DW39"/>
+      <c r="DX39"/>
+      <c r="DY39"/>
+      <c r="DZ39"/>
+      <c r="EA39"/>
+      <c r="EB39"/>
+      <c r="EC39"/>
+      <c r="ED39"/>
+      <c r="EE39"/>
+      <c r="EF39"/>
+      <c r="EG39"/>
+      <c r="EH39"/>
+      <c r="EI39"/>
+      <c r="EJ39"/>
+      <c r="EK39"/>
+      <c r="EL39"/>
+      <c r="EM39"/>
+      <c r="EN39"/>
+      <c r="EO39"/>
+      <c r="EP39"/>
+      <c r="EQ39"/>
+      <c r="ER39"/>
+      <c r="ES39"/>
+      <c r="ET39"/>
+      <c r="EU39"/>
+      <c r="EV39"/>
+      <c r="EW39"/>
+      <c r="EX39"/>
+      <c r="EY39"/>
+      <c r="EZ39"/>
+      <c r="FA39"/>
+      <c r="FB39"/>
+      <c r="FC39"/>
+      <c r="FD39"/>
+      <c r="FE39"/>
+      <c r="FF39"/>
+      <c r="FG39"/>
+      <c r="FH39"/>
+      <c r="FI39"/>
+      <c r="FJ39"/>
+      <c r="FK39"/>
+      <c r="FL39"/>
+      <c r="FM39"/>
+      <c r="FN39"/>
+      <c r="FO39"/>
+      <c r="FP39"/>
+      <c r="FQ39"/>
+      <c r="FR39"/>
+      <c r="FS39"/>
+      <c r="FT39"/>
+      <c r="FU39"/>
+      <c r="FV39"/>
+      <c r="FW39"/>
+      <c r="FX39"/>
+      <c r="FY39"/>
+      <c r="FZ39"/>
+      <c r="GA39"/>
+      <c r="GB39"/>
+      <c r="GC39"/>
+      <c r="GD39"/>
+      <c r="GE39"/>
+      <c r="GF39"/>
+      <c r="GG39"/>
+      <c r="GH39"/>
+      <c r="GI39"/>
+      <c r="GJ39"/>
+      <c r="GK39"/>
+      <c r="GL39"/>
+      <c r="GM39"/>
+      <c r="GN39"/>
+      <c r="GO39"/>
+      <c r="GP39"/>
+      <c r="GQ39"/>
+      <c r="GR39"/>
+      <c r="GS39"/>
+      <c r="GT39"/>
+      <c r="GU39"/>
+      <c r="GV39"/>
+      <c r="GW39"/>
+      <c r="GX39"/>
+      <c r="GY39"/>
+      <c r="GZ39"/>
+      <c r="HA39"/>
+      <c r="HB39"/>
+      <c r="HC39"/>
+      <c r="HD39"/>
+      <c r="HE39"/>
+      <c r="HF39"/>
+      <c r="HG39"/>
+      <c r="HH39"/>
+      <c r="HI39"/>
+      <c r="HJ39"/>
+      <c r="HK39"/>
+      <c r="HL39"/>
+      <c r="HM39"/>
+      <c r="HN39"/>
+      <c r="HO39"/>
+      <c r="HP39"/>
+      <c r="HQ39"/>
+      <c r="HR39"/>
+      <c r="HS39"/>
+      <c r="HT39"/>
+      <c r="HU39"/>
+      <c r="HV39"/>
+      <c r="HW39"/>
+      <c r="HX39"/>
+      <c r="HY39"/>
+      <c r="HZ39"/>
+      <c r="IA39"/>
+      <c r="IB39"/>
+      <c r="IC39"/>
+      <c r="ID39"/>
+      <c r="IE39"/>
+      <c r="IF39"/>
+      <c r="IG39"/>
+      <c r="IH39"/>
+      <c r="II39"/>
+      <c r="IJ39"/>
+      <c r="IK39"/>
+      <c r="IL39"/>
+      <c r="IM39"/>
+      <c r="IN39"/>
+      <c r="IO39"/>
+      <c r="IP39"/>
+      <c r="IQ39"/>
+      <c r="IR39"/>
+      <c r="IS39"/>
+      <c r="IT39"/>
+      <c r="IU39"/>
+      <c r="IV39"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3782,7 +4267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV9"/>
   <sheetViews>
@@ -3799,11 +4284,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -4395,9 +4880,9 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1">
-      <c r="A9" s="111"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="113"/>
+      <c r="A9" s="116"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="118"/>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
     </row>
@@ -4414,7 +4899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV15"/>
   <sheetViews>
@@ -4431,11 +4916,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -5141,9 +5626,9 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
-      <c r="A15" s="115"/>
-      <c r="B15" s="116"/>
-      <c r="C15" s="117"/>
+      <c r="A15" s="120"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5158,7 +5643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV16"/>
   <sheetViews>
@@ -5175,11 +5660,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -6645,9 +7130,9 @@
       <c r="IV15" s="73"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
-      <c r="A16" s="111"/>
-      <c r="B16" s="112"/>
-      <c r="C16" s="113"/>
+      <c r="A16" s="116"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="118"/>
       <c r="D16" s="38"/>
       <c r="E16" s="39"/>
       <c r="F16" s="39"/>
@@ -6915,7 +7400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV10"/>
   <sheetViews>
@@ -6930,11 +7415,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -7081,7 +7566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV18"/>
   <sheetViews>
@@ -7361,15 +7846,15 @@
       <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="118" t="s">
+      <c r="A18" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="119"/>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
-      <c r="G18" s="119"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
       <c r="H18" s="69"/>
     </row>
   </sheetData>
@@ -7382,155 +7867,4 @@
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV13"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="37" style="70" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="70" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" style="70" customWidth="1"/>
-    <col min="5" max="5" width="54.85546875" style="70" customWidth="1"/>
-    <col min="6" max="256" width="8.85546875" style="70" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="23"/>
-      <c r="B6" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="23">
-        <v>3</v>
-      </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="24">
-        <v>10</v>
-      </c>
-      <c r="C9" s="24">
-        <v>12</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="71"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="23"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="71"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="23"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" s="72" t="s">
-        <v>98</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización de actividades, correcciones menores a correos, empieza la carga de datos en el perfil del cliente, uso de las mismas clases del diagnóstico para el file
</commit_message>
<xml_diff>
--- a/Scrum Febrero.xlsx
+++ b/Scrum Febrero.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="138">
   <si>
     <t>TOÑO</t>
   </si>
@@ -110,9 +110,6 @@
     <t>BUG - Cuando cambie de cliente ese selecciona nuevo contacto, deja información anterior</t>
   </si>
   <si>
-    <t>Perfil del cliente</t>
-  </si>
-  <si>
     <t>Carga de catálogos</t>
   </si>
   <si>
@@ -425,9 +422,6 @@
     <t>No hay acceso al servidor</t>
   </si>
   <si>
-    <t>Formato de diagnóstico - Subir archivos renombrados y guardar en base de datos</t>
-  </si>
-  <si>
     <t>Mario</t>
   </si>
   <si>
@@ -438,6 +432,12 @@
   </si>
   <si>
     <t>Perfil del cliente - Inserción en base de datos</t>
+  </si>
+  <si>
+    <t>Correos - Correcciones menores</t>
+  </si>
+  <si>
+    <t>Formato de diagnóstico - Subir archivos, renombrarlos y guardar en base de datos</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,14 +508,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="33">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -892,22 +886,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1012,31 +995,17 @@
     <xf numFmtId="14" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1055,9 +1024,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1073,9 +1039,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2286,10 +2250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV25"/>
+  <dimension ref="A1:IV40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2301,11 +2265,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="109" t="s">
-        <v>130</v>
-      </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="A1" s="101" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -2317,7 +2281,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="89" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
@@ -2329,65 +2293,67 @@
       <c r="B3" s="10">
         <v>42834</v>
       </c>
-      <c r="C3" s="125" t="s">
-        <v>131</v>
+      <c r="C3" s="97" t="s">
+        <v>130</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="21" t="s">
-        <v>133</v>
+      <c r="A4" s="99" t="s">
+        <v>137</v>
       </c>
       <c r="B4" s="10">
         <v>42834</v>
       </c>
-      <c r="C4" s="125" t="s">
-        <v>134</v>
+      <c r="C4" s="97" t="s">
+        <v>132</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" s="10">
+      <c r="A5" s="116" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="13">
         <v>42834</v>
       </c>
-      <c r="C5" s="125" t="s">
-        <v>135</v>
+      <c r="C5" s="89" t="s">
+        <v>133</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="127" t="s">
-        <v>136</v>
+      <c r="A6" s="84" t="s">
+        <v>134</v>
       </c>
       <c r="B6" s="10">
         <v>42834</v>
       </c>
-      <c r="C6" s="125" t="s">
-        <v>135</v>
+      <c r="C6" s="97" t="s">
+        <v>133</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="84" t="s">
-        <v>137</v>
+      <c r="A7" s="93" t="s">
+        <v>136</v>
       </c>
       <c r="B7" s="10">
         <v>42834</v>
       </c>
-      <c r="C7" s="89"/>
+      <c r="C7" s="97" t="s">
+        <v>133</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="105" t="s">
-        <v>44</v>
+      <c r="A8" s="84" t="s">
+        <v>135</v>
       </c>
       <c r="B8" s="10">
         <v>42834</v>
@@ -2397,148 +2363,287 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="103"/>
+      <c r="A9" s="93" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="10">
+        <v>42834</v>
+      </c>
       <c r="C9" s="89"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="89"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="112"/>
-      <c r="C11" s="112"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="B12" s="104"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13" s="21"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="22"/>
-      <c r="D13" s="126" t="s">
-        <v>132</v>
-      </c>
+      <c r="D13" s="7"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="105" t="s">
-        <v>123</v>
+      <c r="A14" s="21" t="s">
+        <v>121</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
-      <c r="D14" s="126" t="s">
-        <v>132</v>
+      <c r="D14" s="98" t="s">
+        <v>131</v>
       </c>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A15" s="86"/>
+      <c r="A15" s="93" t="s">
+        <v>122</v>
+      </c>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="98" t="s">
+        <v>131</v>
+      </c>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="107"/>
-      <c r="C16" s="108"/>
-      <c r="D16" s="7"/>
+      <c r="A16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="98"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="19"/>
+      <c r="A17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="98"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="28"/>
+      <c r="A18" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
-      <c r="D18" s="7"/>
+      <c r="D18" s="98"/>
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="29"/>
-      <c r="B19" s="107"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="7"/>
+      <c r="A19" s="83" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="98"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A20" s="29"/>
-      <c r="B20" s="107"/>
-      <c r="C20" s="108"/>
-      <c r="D20" s="7"/>
+    <row r="20" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="98"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A21" s="29"/>
-      <c r="B21" s="107"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="7"/>
+    <row r="21" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A21" s="93" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A22" s="29"/>
-      <c r="B22" s="107"/>
-      <c r="C22" s="108"/>
-      <c r="D22" s="7"/>
+    <row r="22" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="98"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A23" s="29"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="7"/>
+    <row r="23" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="98"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A24" s="113" t="s">
+      <c r="A24" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="98"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A25" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="98"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A26" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A28" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A30" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="94"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A31" s="100"/>
+      <c r="B31" s="96"/>
+      <c r="C31" s="96"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A33" s="28"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="29"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A35" s="29"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A36" s="29"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A37" s="29"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
+      <c r="A38" s="29"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A39" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="114"/>
-      <c r="C24" s="115"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="116" t="s">
+      <c r="B39" s="106"/>
+      <c r="C39" s="107"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A40" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="117"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="31"/>
+      <c r="B40" s="109"/>
+      <c r="C40" s="110"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2565,7 +2670,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -2574,7 +2679,7 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -2583,10 +2688,10 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>87</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>88</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -2594,10 +2699,10 @@
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="42" t="s">
         <v>89</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>90</v>
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -2613,28 +2718,28 @@
     <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="23"/>
       <c r="B6" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="42" t="s">
         <v>91</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>92</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="23">
         <v>3</v>
@@ -2645,7 +2750,7 @@
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="24">
         <v>10</v>
@@ -2672,10 +2777,10 @@
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="A12" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="72" t="s">
         <v>97</v>
-      </c>
-      <c r="B12" s="72" t="s">
-        <v>98</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="23"/>
@@ -2683,7 +2788,7 @@
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -2714,7 +2819,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
       <c r="A1" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -2730,7 +2835,7 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -2739,7 +2844,7 @@
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="74" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -2748,7 +2853,7 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="75" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -2757,7 +2862,7 @@
     </row>
     <row r="6" spans="1:5" ht="45" customHeight="1">
       <c r="A6" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -2773,7 +2878,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="74" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -2782,7 +2887,7 @@
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1">
       <c r="A9" s="75" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -2791,7 +2896,7 @@
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -2830,10 +2935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV19"/>
+  <dimension ref="A1:IV6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2845,11 +2950,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -2866,20 +2971,22 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="10">
         <v>42820</v>
       </c>
-      <c r="C3" s="89"/>
+      <c r="C3" s="89">
+        <v>42819</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="10">
+      <c r="A4" s="88" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="13">
         <v>42820</v>
       </c>
       <c r="C4" s="89">
@@ -2889,134 +2996,25 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="10">
-        <v>42820</v>
-      </c>
-      <c r="C5" s="89"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="88" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="13">
-        <v>42820</v>
-      </c>
-      <c r="C6" s="89">
-        <v>42819</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="111" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="112"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="93"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A14" s="29"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A16" s="29"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A17" s="29"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="113" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="114"/>
-      <c r="C18" s="115"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="116" t="s">
+    <row r="6" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="117"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3028,10 +3026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV17"/>
+  <dimension ref="A1:IV5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -3043,11 +3041,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -3072,7 +3070,7 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="84" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3" s="10">
         <v>42820</v>
@@ -3085,166 +3083,29 @@
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="84" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" s="10">
-        <v>42820</v>
-      </c>
+      <c r="A4" s="35"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="106" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="93"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="29"/>
-      <c r="B12" s="93"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" s="73" customFormat="1" ht="15" hidden="1" customHeight="1">
-      <c r="A14" s="29"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="92" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="93"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="97" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="98"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="31"/>
+    <row r="5" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="111"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3256,10 +3117,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IV39"/>
+  <dimension ref="A1:IV12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A18" sqref="A17:A18"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -3270,19 +3131,19 @@
     <col min="4" max="256" width="8.85546875" style="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="109" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+    <row r="1" spans="1:256" ht="15" customHeight="1">
+      <c r="A1" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:256" ht="15" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3298,7 +3159,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:256" ht="15" customHeight="1">
       <c r="A3" s="20" t="s">
         <v>11</v>
       </c>
@@ -3307,14 +3168,14 @@
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="33"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
       <c r="H3" s="34"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:256" ht="15" customHeight="1">
       <c r="A4" s="86" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="13">
         <v>42799</v>
@@ -3323,14 +3184,14 @@
         <v>42798</v>
       </c>
       <c r="D4" s="33"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
       <c r="H4" s="34"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
+    <row r="5" spans="1:256" ht="15" customHeight="1">
       <c r="A5" s="86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="13">
         <v>42799</v>
@@ -3339,14 +3200,14 @@
         <v>42798</v>
       </c>
       <c r="D5" s="33"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" spans="1:256" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="13">
         <v>42799</v>
@@ -3355,14 +3216,14 @@
         <v>42798</v>
       </c>
       <c r="D6" s="33"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
+    <row r="7" spans="1:256" ht="15" customHeight="1">
       <c r="A7" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" s="13">
         <v>42799</v>
@@ -3371,14 +3232,14 @@
         <v>42798</v>
       </c>
       <c r="D7" s="33"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
       <c r="H7" s="34"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
+    <row r="8" spans="1:256" ht="15" customHeight="1">
       <c r="A8" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="13">
         <v>42799</v>
@@ -3387,14 +3248,14 @@
         <v>42798</v>
       </c>
       <c r="D8" s="33"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
       <c r="H8" s="34"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
+    <row r="9" spans="1:256" ht="15" customHeight="1">
       <c r="A9" s="88" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" s="13">
         <v>42806</v>
@@ -3403,14 +3264,14 @@
         <v>42805</v>
       </c>
       <c r="D9" s="33"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="91"/>
       <c r="H9" s="34"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
+    <row r="10" spans="1:256" ht="15" customHeight="1">
       <c r="A10" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10" s="13">
         <v>42820</v>
@@ -3419,845 +3280,283 @@
         <v>42819</v>
       </c>
       <c r="D10" s="33"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
       <c r="H10" s="34"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
+    <row r="11" spans="1:256" ht="15" customHeight="1">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="33"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
       <c r="H11" s="34"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="34"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="34"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="96"/>
-      <c r="H15" s="34"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="34"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="34"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="34"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
-      <c r="A20" s="119" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="112"/>
-      <c r="C20" s="112"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
-      <c r="A21" s="83" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1">
-      <c r="A22" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="93"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="34"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="105" t="s">
-        <v>129</v>
-      </c>
-      <c r="B23" s="100"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="102"/>
-      <c r="F23" s="102"/>
-      <c r="G23" s="102"/>
-      <c r="H23" s="34"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="93"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="96"/>
-      <c r="G24" s="96"/>
-      <c r="H24" s="34"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="93"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="34"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="B26" s="93"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="96"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="96"/>
-      <c r="H26" s="34"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="93"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="96"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="96"/>
-      <c r="H27" s="34"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
-      <c r="A28" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B28" s="93"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="34"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
-      <c r="A29" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="93"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="96"/>
-      <c r="F29" s="96"/>
-      <c r="G29" s="96"/>
-      <c r="H29" s="34"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="93"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="96"/>
-      <c r="H30" s="34"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1">
-      <c r="A31" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="93"/>
-      <c r="C31" s="94"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="34"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1">
-      <c r="A32" s="84" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="96"/>
-      <c r="F32" s="96"/>
-      <c r="G32" s="96"/>
-      <c r="H32" s="34"/>
-    </row>
-    <row r="33" spans="1:256" ht="15" customHeight="1">
-      <c r="A33" s="84"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="96"/>
-      <c r="F33" s="96"/>
-      <c r="G33" s="96"/>
-      <c r="H33" s="34"/>
-    </row>
-    <row r="34" spans="1:256" ht="15" customHeight="1">
-      <c r="A34" s="15"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="8"/>
-    </row>
-    <row r="35" spans="1:256" ht="15" customHeight="1">
-      <c r="A35" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="34"/>
-    </row>
-    <row r="36" spans="1:256" ht="15" customHeight="1">
-      <c r="A36" s="28"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="96"/>
-      <c r="F36" s="96"/>
-      <c r="G36" s="96"/>
-      <c r="H36" s="34"/>
-    </row>
-    <row r="37" spans="1:256" ht="15" customHeight="1">
-      <c r="A37" s="29"/>
-      <c r="B37" s="93"/>
-      <c r="C37" s="94"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="34"/>
-    </row>
-    <row r="38" spans="1:256" ht="15" customHeight="1">
-      <c r="A38" s="113" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="114"/>
-      <c r="C38" s="115"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="96"/>
-      <c r="F38" s="96"/>
-      <c r="G38" s="96"/>
-      <c r="H38" s="34"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-      <c r="N38"/>
-      <c r="O38"/>
-      <c r="P38"/>
-      <c r="Q38"/>
-      <c r="R38"/>
-      <c r="S38"/>
-      <c r="T38"/>
-      <c r="U38"/>
-      <c r="V38"/>
-      <c r="W38"/>
-      <c r="X38"/>
-      <c r="Y38"/>
-      <c r="Z38"/>
-      <c r="AA38"/>
-      <c r="AB38"/>
-      <c r="AC38"/>
-      <c r="AD38"/>
-      <c r="AE38"/>
-      <c r="AF38"/>
-      <c r="AG38"/>
-      <c r="AH38"/>
-      <c r="AI38"/>
-      <c r="AJ38"/>
-      <c r="AK38"/>
-      <c r="AL38"/>
-      <c r="AM38"/>
-      <c r="AN38"/>
-      <c r="AO38"/>
-      <c r="AP38"/>
-      <c r="AQ38"/>
-      <c r="AR38"/>
-      <c r="AS38"/>
-      <c r="AT38"/>
-      <c r="AU38"/>
-      <c r="AV38"/>
-      <c r="AW38"/>
-      <c r="AX38"/>
-      <c r="AY38"/>
-      <c r="AZ38"/>
-      <c r="BA38"/>
-      <c r="BB38"/>
-      <c r="BC38"/>
-      <c r="BD38"/>
-      <c r="BE38"/>
-      <c r="BF38"/>
-      <c r="BG38"/>
-      <c r="BH38"/>
-      <c r="BI38"/>
-      <c r="BJ38"/>
-      <c r="BK38"/>
-      <c r="BL38"/>
-      <c r="BM38"/>
-      <c r="BN38"/>
-      <c r="BO38"/>
-      <c r="BP38"/>
-      <c r="BQ38"/>
-      <c r="BR38"/>
-      <c r="BS38"/>
-      <c r="BT38"/>
-      <c r="BU38"/>
-      <c r="BV38"/>
-      <c r="BW38"/>
-      <c r="BX38"/>
-      <c r="BY38"/>
-      <c r="BZ38"/>
-      <c r="CA38"/>
-      <c r="CB38"/>
-      <c r="CC38"/>
-      <c r="CD38"/>
-      <c r="CE38"/>
-      <c r="CF38"/>
-      <c r="CG38"/>
-      <c r="CH38"/>
-      <c r="CI38"/>
-      <c r="CJ38"/>
-      <c r="CK38"/>
-      <c r="CL38"/>
-      <c r="CM38"/>
-      <c r="CN38"/>
-      <c r="CO38"/>
-      <c r="CP38"/>
-      <c r="CQ38"/>
-      <c r="CR38"/>
-      <c r="CS38"/>
-      <c r="CT38"/>
-      <c r="CU38"/>
-      <c r="CV38"/>
-      <c r="CW38"/>
-      <c r="CX38"/>
-      <c r="CY38"/>
-      <c r="CZ38"/>
-      <c r="DA38"/>
-      <c r="DB38"/>
-      <c r="DC38"/>
-      <c r="DD38"/>
-      <c r="DE38"/>
-      <c r="DF38"/>
-      <c r="DG38"/>
-      <c r="DH38"/>
-      <c r="DI38"/>
-      <c r="DJ38"/>
-      <c r="DK38"/>
-      <c r="DL38"/>
-      <c r="DM38"/>
-      <c r="DN38"/>
-      <c r="DO38"/>
-      <c r="DP38"/>
-      <c r="DQ38"/>
-      <c r="DR38"/>
-      <c r="DS38"/>
-      <c r="DT38"/>
-      <c r="DU38"/>
-      <c r="DV38"/>
-      <c r="DW38"/>
-      <c r="DX38"/>
-      <c r="DY38"/>
-      <c r="DZ38"/>
-      <c r="EA38"/>
-      <c r="EB38"/>
-      <c r="EC38"/>
-      <c r="ED38"/>
-      <c r="EE38"/>
-      <c r="EF38"/>
-      <c r="EG38"/>
-      <c r="EH38"/>
-      <c r="EI38"/>
-      <c r="EJ38"/>
-      <c r="EK38"/>
-      <c r="EL38"/>
-      <c r="EM38"/>
-      <c r="EN38"/>
-      <c r="EO38"/>
-      <c r="EP38"/>
-      <c r="EQ38"/>
-      <c r="ER38"/>
-      <c r="ES38"/>
-      <c r="ET38"/>
-      <c r="EU38"/>
-      <c r="EV38"/>
-      <c r="EW38"/>
-      <c r="EX38"/>
-      <c r="EY38"/>
-      <c r="EZ38"/>
-      <c r="FA38"/>
-      <c r="FB38"/>
-      <c r="FC38"/>
-      <c r="FD38"/>
-      <c r="FE38"/>
-      <c r="FF38"/>
-      <c r="FG38"/>
-      <c r="FH38"/>
-      <c r="FI38"/>
-      <c r="FJ38"/>
-      <c r="FK38"/>
-      <c r="FL38"/>
-      <c r="FM38"/>
-      <c r="FN38"/>
-      <c r="FO38"/>
-      <c r="FP38"/>
-      <c r="FQ38"/>
-      <c r="FR38"/>
-      <c r="FS38"/>
-      <c r="FT38"/>
-      <c r="FU38"/>
-      <c r="FV38"/>
-      <c r="FW38"/>
-      <c r="FX38"/>
-      <c r="FY38"/>
-      <c r="FZ38"/>
-      <c r="GA38"/>
-      <c r="GB38"/>
-      <c r="GC38"/>
-      <c r="GD38"/>
-      <c r="GE38"/>
-      <c r="GF38"/>
-      <c r="GG38"/>
-      <c r="GH38"/>
-      <c r="GI38"/>
-      <c r="GJ38"/>
-      <c r="GK38"/>
-      <c r="GL38"/>
-      <c r="GM38"/>
-      <c r="GN38"/>
-      <c r="GO38"/>
-      <c r="GP38"/>
-      <c r="GQ38"/>
-      <c r="GR38"/>
-      <c r="GS38"/>
-      <c r="GT38"/>
-      <c r="GU38"/>
-      <c r="GV38"/>
-      <c r="GW38"/>
-      <c r="GX38"/>
-      <c r="GY38"/>
-      <c r="GZ38"/>
-      <c r="HA38"/>
-      <c r="HB38"/>
-      <c r="HC38"/>
-      <c r="HD38"/>
-      <c r="HE38"/>
-      <c r="HF38"/>
-      <c r="HG38"/>
-      <c r="HH38"/>
-      <c r="HI38"/>
-      <c r="HJ38"/>
-      <c r="HK38"/>
-      <c r="HL38"/>
-      <c r="HM38"/>
-      <c r="HN38"/>
-      <c r="HO38"/>
-      <c r="HP38"/>
-      <c r="HQ38"/>
-      <c r="HR38"/>
-      <c r="HS38"/>
-      <c r="HT38"/>
-      <c r="HU38"/>
-      <c r="HV38"/>
-      <c r="HW38"/>
-      <c r="HX38"/>
-      <c r="HY38"/>
-      <c r="HZ38"/>
-      <c r="IA38"/>
-      <c r="IB38"/>
-      <c r="IC38"/>
-      <c r="ID38"/>
-      <c r="IE38"/>
-      <c r="IF38"/>
-      <c r="IG38"/>
-      <c r="IH38"/>
-      <c r="II38"/>
-      <c r="IJ38"/>
-      <c r="IK38"/>
-      <c r="IL38"/>
-      <c r="IM38"/>
-      <c r="IN38"/>
-      <c r="IO38"/>
-      <c r="IP38"/>
-      <c r="IQ38"/>
-      <c r="IR38"/>
-      <c r="IS38"/>
-      <c r="IT38"/>
-      <c r="IU38"/>
-      <c r="IV38"/>
-    </row>
-    <row r="39" spans="1:256" ht="15" customHeight="1">
-      <c r="A39" s="116" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="117"/>
-      <c r="C39" s="118"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="40"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-      <c r="N39"/>
-      <c r="O39"/>
-      <c r="P39"/>
-      <c r="Q39"/>
-      <c r="R39"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-      <c r="X39"/>
-      <c r="Y39"/>
-      <c r="Z39"/>
-      <c r="AA39"/>
-      <c r="AB39"/>
-      <c r="AC39"/>
-      <c r="AD39"/>
-      <c r="AE39"/>
-      <c r="AF39"/>
-      <c r="AG39"/>
-      <c r="AH39"/>
-      <c r="AI39"/>
-      <c r="AJ39"/>
-      <c r="AK39"/>
-      <c r="AL39"/>
-      <c r="AM39"/>
-      <c r="AN39"/>
-      <c r="AO39"/>
-      <c r="AP39"/>
-      <c r="AQ39"/>
-      <c r="AR39"/>
-      <c r="AS39"/>
-      <c r="AT39"/>
-      <c r="AU39"/>
-      <c r="AV39"/>
-      <c r="AW39"/>
-      <c r="AX39"/>
-      <c r="AY39"/>
-      <c r="AZ39"/>
-      <c r="BA39"/>
-      <c r="BB39"/>
-      <c r="BC39"/>
-      <c r="BD39"/>
-      <c r="BE39"/>
-      <c r="BF39"/>
-      <c r="BG39"/>
-      <c r="BH39"/>
-      <c r="BI39"/>
-      <c r="BJ39"/>
-      <c r="BK39"/>
-      <c r="BL39"/>
-      <c r="BM39"/>
-      <c r="BN39"/>
-      <c r="BO39"/>
-      <c r="BP39"/>
-      <c r="BQ39"/>
-      <c r="BR39"/>
-      <c r="BS39"/>
-      <c r="BT39"/>
-      <c r="BU39"/>
-      <c r="BV39"/>
-      <c r="BW39"/>
-      <c r="BX39"/>
-      <c r="BY39"/>
-      <c r="BZ39"/>
-      <c r="CA39"/>
-      <c r="CB39"/>
-      <c r="CC39"/>
-      <c r="CD39"/>
-      <c r="CE39"/>
-      <c r="CF39"/>
-      <c r="CG39"/>
-      <c r="CH39"/>
-      <c r="CI39"/>
-      <c r="CJ39"/>
-      <c r="CK39"/>
-      <c r="CL39"/>
-      <c r="CM39"/>
-      <c r="CN39"/>
-      <c r="CO39"/>
-      <c r="CP39"/>
-      <c r="CQ39"/>
-      <c r="CR39"/>
-      <c r="CS39"/>
-      <c r="CT39"/>
-      <c r="CU39"/>
-      <c r="CV39"/>
-      <c r="CW39"/>
-      <c r="CX39"/>
-      <c r="CY39"/>
-      <c r="CZ39"/>
-      <c r="DA39"/>
-      <c r="DB39"/>
-      <c r="DC39"/>
-      <c r="DD39"/>
-      <c r="DE39"/>
-      <c r="DF39"/>
-      <c r="DG39"/>
-      <c r="DH39"/>
-      <c r="DI39"/>
-      <c r="DJ39"/>
-      <c r="DK39"/>
-      <c r="DL39"/>
-      <c r="DM39"/>
-      <c r="DN39"/>
-      <c r="DO39"/>
-      <c r="DP39"/>
-      <c r="DQ39"/>
-      <c r="DR39"/>
-      <c r="DS39"/>
-      <c r="DT39"/>
-      <c r="DU39"/>
-      <c r="DV39"/>
-      <c r="DW39"/>
-      <c r="DX39"/>
-      <c r="DY39"/>
-      <c r="DZ39"/>
-      <c r="EA39"/>
-      <c r="EB39"/>
-      <c r="EC39"/>
-      <c r="ED39"/>
-      <c r="EE39"/>
-      <c r="EF39"/>
-      <c r="EG39"/>
-      <c r="EH39"/>
-      <c r="EI39"/>
-      <c r="EJ39"/>
-      <c r="EK39"/>
-      <c r="EL39"/>
-      <c r="EM39"/>
-      <c r="EN39"/>
-      <c r="EO39"/>
-      <c r="EP39"/>
-      <c r="EQ39"/>
-      <c r="ER39"/>
-      <c r="ES39"/>
-      <c r="ET39"/>
-      <c r="EU39"/>
-      <c r="EV39"/>
-      <c r="EW39"/>
-      <c r="EX39"/>
-      <c r="EY39"/>
-      <c r="EZ39"/>
-      <c r="FA39"/>
-      <c r="FB39"/>
-      <c r="FC39"/>
-      <c r="FD39"/>
-      <c r="FE39"/>
-      <c r="FF39"/>
-      <c r="FG39"/>
-      <c r="FH39"/>
-      <c r="FI39"/>
-      <c r="FJ39"/>
-      <c r="FK39"/>
-      <c r="FL39"/>
-      <c r="FM39"/>
-      <c r="FN39"/>
-      <c r="FO39"/>
-      <c r="FP39"/>
-      <c r="FQ39"/>
-      <c r="FR39"/>
-      <c r="FS39"/>
-      <c r="FT39"/>
-      <c r="FU39"/>
-      <c r="FV39"/>
-      <c r="FW39"/>
-      <c r="FX39"/>
-      <c r="FY39"/>
-      <c r="FZ39"/>
-      <c r="GA39"/>
-      <c r="GB39"/>
-      <c r="GC39"/>
-      <c r="GD39"/>
-      <c r="GE39"/>
-      <c r="GF39"/>
-      <c r="GG39"/>
-      <c r="GH39"/>
-      <c r="GI39"/>
-      <c r="GJ39"/>
-      <c r="GK39"/>
-      <c r="GL39"/>
-      <c r="GM39"/>
-      <c r="GN39"/>
-      <c r="GO39"/>
-      <c r="GP39"/>
-      <c r="GQ39"/>
-      <c r="GR39"/>
-      <c r="GS39"/>
-      <c r="GT39"/>
-      <c r="GU39"/>
-      <c r="GV39"/>
-      <c r="GW39"/>
-      <c r="GX39"/>
-      <c r="GY39"/>
-      <c r="GZ39"/>
-      <c r="HA39"/>
-      <c r="HB39"/>
-      <c r="HC39"/>
-      <c r="HD39"/>
-      <c r="HE39"/>
-      <c r="HF39"/>
-      <c r="HG39"/>
-      <c r="HH39"/>
-      <c r="HI39"/>
-      <c r="HJ39"/>
-      <c r="HK39"/>
-      <c r="HL39"/>
-      <c r="HM39"/>
-      <c r="HN39"/>
-      <c r="HO39"/>
-      <c r="HP39"/>
-      <c r="HQ39"/>
-      <c r="HR39"/>
-      <c r="HS39"/>
-      <c r="HT39"/>
-      <c r="HU39"/>
-      <c r="HV39"/>
-      <c r="HW39"/>
-      <c r="HX39"/>
-      <c r="HY39"/>
-      <c r="HZ39"/>
-      <c r="IA39"/>
-      <c r="IB39"/>
-      <c r="IC39"/>
-      <c r="ID39"/>
-      <c r="IE39"/>
-      <c r="IF39"/>
-      <c r="IG39"/>
-      <c r="IH39"/>
-      <c r="II39"/>
-      <c r="IJ39"/>
-      <c r="IK39"/>
-      <c r="IL39"/>
-      <c r="IM39"/>
-      <c r="IN39"/>
-      <c r="IO39"/>
-      <c r="IP39"/>
-      <c r="IQ39"/>
-      <c r="IR39"/>
-      <c r="IS39"/>
-      <c r="IT39"/>
-      <c r="IU39"/>
-      <c r="IV39"/>
+    <row r="12" spans="1:256" ht="15" customHeight="1">
+      <c r="A12" s="108"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="40"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12"/>
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12"/>
+      <c r="AJ12"/>
+      <c r="AK12"/>
+      <c r="AL12"/>
+      <c r="AM12"/>
+      <c r="AN12"/>
+      <c r="AO12"/>
+      <c r="AP12"/>
+      <c r="AQ12"/>
+      <c r="AR12"/>
+      <c r="AS12"/>
+      <c r="AT12"/>
+      <c r="AU12"/>
+      <c r="AV12"/>
+      <c r="AW12"/>
+      <c r="AX12"/>
+      <c r="AY12"/>
+      <c r="AZ12"/>
+      <c r="BA12"/>
+      <c r="BB12"/>
+      <c r="BC12"/>
+      <c r="BD12"/>
+      <c r="BE12"/>
+      <c r="BF12"/>
+      <c r="BG12"/>
+      <c r="BH12"/>
+      <c r="BI12"/>
+      <c r="BJ12"/>
+      <c r="BK12"/>
+      <c r="BL12"/>
+      <c r="BM12"/>
+      <c r="BN12"/>
+      <c r="BO12"/>
+      <c r="BP12"/>
+      <c r="BQ12"/>
+      <c r="BR12"/>
+      <c r="BS12"/>
+      <c r="BT12"/>
+      <c r="BU12"/>
+      <c r="BV12"/>
+      <c r="BW12"/>
+      <c r="BX12"/>
+      <c r="BY12"/>
+      <c r="BZ12"/>
+      <c r="CA12"/>
+      <c r="CB12"/>
+      <c r="CC12"/>
+      <c r="CD12"/>
+      <c r="CE12"/>
+      <c r="CF12"/>
+      <c r="CG12"/>
+      <c r="CH12"/>
+      <c r="CI12"/>
+      <c r="CJ12"/>
+      <c r="CK12"/>
+      <c r="CL12"/>
+      <c r="CM12"/>
+      <c r="CN12"/>
+      <c r="CO12"/>
+      <c r="CP12"/>
+      <c r="CQ12"/>
+      <c r="CR12"/>
+      <c r="CS12"/>
+      <c r="CT12"/>
+      <c r="CU12"/>
+      <c r="CV12"/>
+      <c r="CW12"/>
+      <c r="CX12"/>
+      <c r="CY12"/>
+      <c r="CZ12"/>
+      <c r="DA12"/>
+      <c r="DB12"/>
+      <c r="DC12"/>
+      <c r="DD12"/>
+      <c r="DE12"/>
+      <c r="DF12"/>
+      <c r="DG12"/>
+      <c r="DH12"/>
+      <c r="DI12"/>
+      <c r="DJ12"/>
+      <c r="DK12"/>
+      <c r="DL12"/>
+      <c r="DM12"/>
+      <c r="DN12"/>
+      <c r="DO12"/>
+      <c r="DP12"/>
+      <c r="DQ12"/>
+      <c r="DR12"/>
+      <c r="DS12"/>
+      <c r="DT12"/>
+      <c r="DU12"/>
+      <c r="DV12"/>
+      <c r="DW12"/>
+      <c r="DX12"/>
+      <c r="DY12"/>
+      <c r="DZ12"/>
+      <c r="EA12"/>
+      <c r="EB12"/>
+      <c r="EC12"/>
+      <c r="ED12"/>
+      <c r="EE12"/>
+      <c r="EF12"/>
+      <c r="EG12"/>
+      <c r="EH12"/>
+      <c r="EI12"/>
+      <c r="EJ12"/>
+      <c r="EK12"/>
+      <c r="EL12"/>
+      <c r="EM12"/>
+      <c r="EN12"/>
+      <c r="EO12"/>
+      <c r="EP12"/>
+      <c r="EQ12"/>
+      <c r="ER12"/>
+      <c r="ES12"/>
+      <c r="ET12"/>
+      <c r="EU12"/>
+      <c r="EV12"/>
+      <c r="EW12"/>
+      <c r="EX12"/>
+      <c r="EY12"/>
+      <c r="EZ12"/>
+      <c r="FA12"/>
+      <c r="FB12"/>
+      <c r="FC12"/>
+      <c r="FD12"/>
+      <c r="FE12"/>
+      <c r="FF12"/>
+      <c r="FG12"/>
+      <c r="FH12"/>
+      <c r="FI12"/>
+      <c r="FJ12"/>
+      <c r="FK12"/>
+      <c r="FL12"/>
+      <c r="FM12"/>
+      <c r="FN12"/>
+      <c r="FO12"/>
+      <c r="FP12"/>
+      <c r="FQ12"/>
+      <c r="FR12"/>
+      <c r="FS12"/>
+      <c r="FT12"/>
+      <c r="FU12"/>
+      <c r="FV12"/>
+      <c r="FW12"/>
+      <c r="FX12"/>
+      <c r="FY12"/>
+      <c r="FZ12"/>
+      <c r="GA12"/>
+      <c r="GB12"/>
+      <c r="GC12"/>
+      <c r="GD12"/>
+      <c r="GE12"/>
+      <c r="GF12"/>
+      <c r="GG12"/>
+      <c r="GH12"/>
+      <c r="GI12"/>
+      <c r="GJ12"/>
+      <c r="GK12"/>
+      <c r="GL12"/>
+      <c r="GM12"/>
+      <c r="GN12"/>
+      <c r="GO12"/>
+      <c r="GP12"/>
+      <c r="GQ12"/>
+      <c r="GR12"/>
+      <c r="GS12"/>
+      <c r="GT12"/>
+      <c r="GU12"/>
+      <c r="GV12"/>
+      <c r="GW12"/>
+      <c r="GX12"/>
+      <c r="GY12"/>
+      <c r="GZ12"/>
+      <c r="HA12"/>
+      <c r="HB12"/>
+      <c r="HC12"/>
+      <c r="HD12"/>
+      <c r="HE12"/>
+      <c r="HF12"/>
+      <c r="HG12"/>
+      <c r="HH12"/>
+      <c r="HI12"/>
+      <c r="HJ12"/>
+      <c r="HK12"/>
+      <c r="HL12"/>
+      <c r="HM12"/>
+      <c r="HN12"/>
+      <c r="HO12"/>
+      <c r="HP12"/>
+      <c r="HQ12"/>
+      <c r="HR12"/>
+      <c r="HS12"/>
+      <c r="HT12"/>
+      <c r="HU12"/>
+      <c r="HV12"/>
+      <c r="HW12"/>
+      <c r="HX12"/>
+      <c r="HY12"/>
+      <c r="HZ12"/>
+      <c r="IA12"/>
+      <c r="IB12"/>
+      <c r="IC12"/>
+      <c r="ID12"/>
+      <c r="IE12"/>
+      <c r="IF12"/>
+      <c r="IG12"/>
+      <c r="IH12"/>
+      <c r="II12"/>
+      <c r="IJ12"/>
+      <c r="IK12"/>
+      <c r="IL12"/>
+      <c r="IM12"/>
+      <c r="IN12"/>
+      <c r="IO12"/>
+      <c r="IP12"/>
+      <c r="IQ12"/>
+      <c r="IR12"/>
+      <c r="IS12"/>
+      <c r="IT12"/>
+      <c r="IU12"/>
+      <c r="IV12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4284,11 +3583,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -4610,9 +3909,9 @@
     </row>
     <row r="7" spans="1:256" ht="15" customHeight="1">
       <c r="A7" s="88" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" s="103">
+        <v>115</v>
+      </c>
+      <c r="B7" s="92">
         <v>42792</v>
       </c>
       <c r="C7" s="89">
@@ -4880,9 +4179,9 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1">
-      <c r="A9" s="116"/>
-      <c r="B9" s="117"/>
-      <c r="C9" s="118"/>
+      <c r="A9" s="108"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="110"/>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
     </row>
@@ -4916,11 +4215,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -5063,7 +4362,7 @@
         <v>42778</v>
       </c>
       <c r="C10" s="85" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="19"/>
@@ -5353,7 +4652,7 @@
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1">
       <c r="A13" s="88" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="13">
         <v>42792</v>
@@ -5626,9 +4925,9 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
-      <c r="A15" s="120"/>
-      <c r="B15" s="121"/>
-      <c r="C15" s="122"/>
+      <c r="A15" s="111"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5660,11 +4959,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="109" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="A1" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -5689,7 +4988,7 @@
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="13">
         <v>42778</v>
@@ -5705,7 +5004,7 @@
     </row>
     <row r="4" spans="1:256" ht="15" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="13">
         <v>42778</v>
@@ -5721,7 +5020,7 @@
     </row>
     <row r="5" spans="1:256" ht="15" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="13">
         <v>42778</v>
@@ -5737,7 +5036,7 @@
     </row>
     <row r="6" spans="1:256" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="13">
         <v>42778</v>
@@ -5753,7 +5052,7 @@
     </row>
     <row r="7" spans="1:256" ht="15" customHeight="1">
       <c r="A7" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="13">
         <v>42778</v>
@@ -5769,7 +5068,7 @@
     </row>
     <row r="8" spans="1:256" ht="15" customHeight="1">
       <c r="A8" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="13">
         <v>42778</v>
@@ -5785,7 +5084,7 @@
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1">
       <c r="A9" s="79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" s="80">
         <v>42785</v>
@@ -5801,7 +5100,7 @@
     </row>
     <row r="10" spans="1:256" ht="15" customHeight="1">
       <c r="A10" s="79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="80">
         <v>42785</v>
@@ -6329,7 +5628,7 @@
     </row>
     <row r="12" spans="1:256" ht="15" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="13">
         <v>42785</v>
@@ -6593,7 +5892,7 @@
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="13">
         <v>42785</v>
@@ -6857,7 +6156,7 @@
     </row>
     <row r="14" spans="1:256" ht="15" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="13">
         <v>42792</v>
@@ -7130,9 +6429,9 @@
       <c r="IV15" s="73"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
-      <c r="A16" s="116"/>
-      <c r="B16" s="117"/>
-      <c r="C16" s="118"/>
+      <c r="A16" s="108"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="110"/>
       <c r="D16" s="38"/>
       <c r="E16" s="39"/>
       <c r="F16" s="39"/>
@@ -7415,11 +6714,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="109" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="A1" s="101" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -7431,10 +6730,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="19"/>
@@ -7444,10 +6743,10 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>54</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>55</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="7"/>
@@ -7458,10 +6757,10 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="42" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>57</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="7"/>
@@ -7472,10 +6771,10 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="7"/>
@@ -7486,10 +6785,10 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="7"/>
@@ -7500,10 +6799,10 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="7"/>
@@ -7514,10 +6813,10 @@
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="7"/>
@@ -7528,10 +6827,10 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="33"/>
@@ -7542,10 +6841,10 @@
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="30"/>
@@ -7597,27 +6896,27 @@
       <c r="E1" s="45"/>
       <c r="F1" s="46"/>
       <c r="G1" s="47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="50">
         <v>42715</v>
       </c>
       <c r="C2" s="51"/>
       <c r="D2" s="52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="53">
         <v>42714</v>
       </c>
       <c r="F2" s="54"/>
       <c r="G2" s="52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H2" s="55">
         <v>42714</v>
@@ -7625,21 +6924,21 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="16">
         <v>42715</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" s="50">
         <v>42349</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H3" s="58">
         <v>42715</v>
@@ -7647,21 +6946,21 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="53">
         <v>42714</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="10">
         <v>42349</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H4" s="55">
         <v>42714</v>
@@ -7669,7 +6968,7 @@
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="50">
         <v>42715</v>
@@ -7679,7 +6978,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="51"/>
       <c r="G5" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H5" s="55">
         <v>42714</v>
@@ -7687,7 +6986,7 @@
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="16">
         <v>42715</v>
@@ -7701,33 +7000,33 @@
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="63"/>
       <c r="C7" s="54"/>
       <c r="D7" s="64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="63"/>
       <c r="F7" s="54"/>
       <c r="G7" s="64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="65"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="23"/>
       <c r="D8" s="49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="23"/>
       <c r="G8" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H8" s="50">
         <v>42715</v>
@@ -7735,17 +7034,17 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
       <c r="G9" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9" s="23"/>
     </row>
@@ -7777,17 +7076,17 @@
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="23"/>
       <c r="D12" s="49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="23"/>
       <c r="G12" s="49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12" s="21"/>
     </row>
@@ -7796,12 +7095,12 @@
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
       <c r="D13" s="42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H13" s="23"/>
     </row>
@@ -7846,15 +7145,15 @@
       <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="123" t="s">
+      <c r="A18" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="124"/>
-      <c r="C18" s="124"/>
-      <c r="D18" s="124"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="124"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="115"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="115"/>
+      <c r="F18" s="115"/>
+      <c r="G18" s="115"/>
       <c r="H18" s="69"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Speech y correcciones menores al correo
</commit_message>
<xml_diff>
--- a/Scrum Febrero.xlsx
+++ b/Scrum Febrero.xlsx
@@ -20,11 +20,12 @@
     <sheet name="Correo catálogos" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="139">
   <si>
     <t>TOÑO</t>
   </si>
@@ -438,6 +439,9 @@
   </si>
   <si>
     <t>Formato de diagnóstico - Subir archivos, renombrarlos y guardar en base de datos</t>
+  </si>
+  <si>
+    <t>Llamadas - Agregar manejo de objeciones y speech</t>
   </si>
 </sst>
 </file>
@@ -1006,6 +1010,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1039,7 +1044,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2253,7 +2257,7 @@
   <dimension ref="A1:IV40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2265,11 +2269,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -2313,7 +2317,7 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="101" t="s">
         <v>127</v>
       </c>
       <c r="B5" s="13">
@@ -2339,13 +2343,13 @@
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="13">
         <v>42834</v>
       </c>
-      <c r="C7" s="97" t="s">
+      <c r="C7" s="89" t="s">
         <v>133</v>
       </c>
       <c r="D7" s="7"/>
@@ -2374,9 +2378,15 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="92"/>
-      <c r="C10" s="89"/>
+      <c r="A10" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="13">
+        <v>42834</v>
+      </c>
+      <c r="C10" s="89" t="s">
+        <v>133</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
     </row>
@@ -2388,11 +2398,11 @@
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="104"/>
-      <c r="C12" s="104"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="105"/>
       <c r="D12" s="19"/>
       <c r="E12" s="8"/>
     </row>
@@ -2621,20 +2631,20 @@
       <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="105" t="s">
+      <c r="A39" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="106"/>
-      <c r="C39" s="107"/>
+      <c r="B39" s="107"/>
+      <c r="C39" s="108"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="108" t="s">
+      <c r="A40" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="109"/>
-      <c r="C40" s="110"/>
+      <c r="B40" s="110"/>
+      <c r="C40" s="111"/>
       <c r="D40" s="30"/>
       <c r="E40" s="31"/>
     </row>
@@ -2950,11 +2960,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -3003,11 +3013,11 @@
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="108" t="s">
+      <c r="A6" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="110"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="111"/>
       <c r="D6" s="30"/>
       <c r="E6" s="31"/>
     </row>
@@ -3041,11 +3051,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -3093,9 +3103,9 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" s="73" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="111"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="113"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="114"/>
       <c r="D5" s="30"/>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -3132,11 +3142,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -3296,9 +3306,9 @@
       <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:256" ht="15" customHeight="1">
-      <c r="A12" s="108"/>
-      <c r="B12" s="109"/>
-      <c r="C12" s="110"/>
+      <c r="A12" s="109"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="111"/>
       <c r="D12" s="38"/>
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
@@ -3583,11 +3593,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -4179,9 +4189,9 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1">
-      <c r="A9" s="108"/>
-      <c r="B9" s="109"/>
-      <c r="C9" s="110"/>
+      <c r="A9" s="109"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
     </row>
@@ -4215,11 +4225,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -4925,9 +4935,9 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
-      <c r="A15" s="111"/>
-      <c r="B15" s="112"/>
-      <c r="C15" s="113"/>
+      <c r="A15" s="112"/>
+      <c r="B15" s="113"/>
+      <c r="C15" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4959,11 +4969,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -6429,9 +6439,9 @@
       <c r="IV15" s="73"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
-      <c r="A16" s="108"/>
-      <c r="B16" s="109"/>
-      <c r="C16" s="110"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="110"/>
+      <c r="C16" s="111"/>
       <c r="D16" s="38"/>
       <c r="E16" s="39"/>
       <c r="F16" s="39"/>
@@ -6714,11 +6724,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -7145,15 +7155,15 @@
       <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="114" t="s">
+      <c r="A18" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="115"/>
-      <c r="C18" s="115"/>
-      <c r="D18" s="115"/>
-      <c r="E18" s="115"/>
-      <c r="F18" s="115"/>
-      <c r="G18" s="115"/>
+      <c r="B18" s="116"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="116"/>
       <c r="H18" s="69"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nuevos datos de conexión, Todo - Quitar librerías repetidas, BUG - Segundo panel abierto, Base de datos -Quitar horas para now() porque el servidor está en Alemania
</commit_message>
<xml_diff>
--- a/Scrum Febrero.xlsx
+++ b/Scrum Febrero.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="143">
   <si>
     <t>TOÑO</t>
   </si>
@@ -486,12 +486,13 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -943,7 +944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1057,6 +1058,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1075,6 +1086,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1090,28 +1110,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2325,7 +2328,7 @@
   <dimension ref="A1:IV39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:C39"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -2337,11 +2340,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="109" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -2352,7 +2355,7 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="114" t="s">
+      <c r="C2" s="99" t="s">
         <v>126</v>
       </c>
       <c r="D2" s="7"/>
@@ -2398,13 +2401,13 @@
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="124" t="s">
+      <c r="A6" s="106" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="115">
+      <c r="B6" s="100">
         <v>42857</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="101" t="s">
         <v>129</v>
       </c>
       <c r="D6" s="7"/>
@@ -2414,10 +2417,10 @@
       <c r="A7" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="115">
+      <c r="B7" s="100">
         <v>42857</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="101" t="s">
         <v>129</v>
       </c>
       <c r="D7" s="7"/>
@@ -2427,84 +2430,88 @@
       <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="115">
+      <c r="B8" s="100">
         <v>42857</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="101" t="s">
         <v>129</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="102" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="119">
+      <c r="B9" s="103">
         <v>42861</v>
       </c>
-      <c r="C9" s="120" t="s">
+      <c r="C9" s="104" t="s">
         <v>129</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="105" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="119">
+      <c r="B10" s="103">
         <v>42861</v>
       </c>
-      <c r="C10" s="120" t="s">
+      <c r="C10" s="104" t="s">
         <v>129</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="127" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="117">
+      <c r="B11" s="128">
         <v>42861</v>
       </c>
-      <c r="C11" s="123" t="s">
+      <c r="C11" s="129" t="s">
         <v>129</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="130">
         <v>42861</v>
       </c>
-      <c r="C12" s="94" t="s">
+      <c r="C12" s="131" t="s">
         <v>129</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="127" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="87"/>
+      <c r="B13" s="130">
+        <v>42861</v>
+      </c>
+      <c r="C13" s="131" t="s">
+        <v>129</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="105" t="s">
         <v>140</v>
       </c>
-      <c r="B14" s="119">
+      <c r="B14" s="103">
         <v>42861</v>
       </c>
-      <c r="C14" s="120" t="s">
+      <c r="C14" s="104" t="s">
         <v>129</v>
       </c>
       <c r="D14" s="7"/>
@@ -2571,11 +2578,11 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" s="71" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="101" t="s">
+      <c r="A21" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="102"/>
-      <c r="C21" s="102"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="112"/>
       <c r="D21" s="19"/>
       <c r="E21" s="8"/>
     </row>
@@ -2601,8 +2608,8 @@
       <c r="A24" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="125"/>
-      <c r="C24" s="126"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="108"/>
       <c r="D24" s="95"/>
       <c r="E24" s="8"/>
     </row>
@@ -2711,29 +2718,29 @@
       <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5" s="71" customFormat="1" ht="15" customHeight="1">
-      <c r="A37" s="103" t="s">
+      <c r="A37" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="104"/>
-      <c r="C37" s="105"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="115"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5" s="71" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="127" t="s">
+      <c r="A38" s="119" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="128"/>
-      <c r="C38" s="129"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="121"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" s="71" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="106" t="s">
+      <c r="A39" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="107"/>
-      <c r="C39" s="108"/>
+      <c r="B39" s="117"/>
+      <c r="C39" s="118"/>
       <c r="D39" s="28"/>
       <c r="E39" s="29"/>
     </row>
@@ -3050,11 +3057,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -3103,11 +3110,11 @@
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" s="71" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="107"/>
-      <c r="C6" s="108"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="118"/>
       <c r="D6" s="28"/>
       <c r="E6" s="29"/>
     </row>
@@ -3141,11 +3148,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -3193,9 +3200,9 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" s="71" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="109"/>
-      <c r="B5" s="110"/>
-      <c r="C5" s="111"/>
+      <c r="A5" s="122"/>
+      <c r="B5" s="123"/>
+      <c r="C5" s="124"/>
       <c r="D5" s="28"/>
       <c r="E5" s="34"/>
       <c r="F5" s="34"/>
@@ -3232,11 +3239,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -3396,9 +3403,9 @@
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:256" ht="15" customHeight="1">
-      <c r="A12" s="106"/>
-      <c r="B12" s="107"/>
-      <c r="C12" s="108"/>
+      <c r="A12" s="116"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="118"/>
       <c r="D12" s="36"/>
       <c r="E12" s="37"/>
       <c r="F12" s="37"/>
@@ -3683,11 +3690,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
@@ -4279,9 +4286,9 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1">
-      <c r="A9" s="106"/>
-      <c r="B9" s="107"/>
-      <c r="C9" s="108"/>
+      <c r="A9" s="116"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="118"/>
       <c r="D9" s="28"/>
       <c r="E9" s="29"/>
     </row>
@@ -4315,11 +4322,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -5025,9 +5032,9 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
-      <c r="A15" s="109"/>
-      <c r="B15" s="110"/>
-      <c r="C15" s="111"/>
+      <c r="A15" s="122"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5059,11 +5066,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -6529,9 +6536,9 @@
       <c r="IV15" s="71"/>
     </row>
     <row r="16" spans="1:256" ht="15" customHeight="1">
-      <c r="A16" s="106"/>
-      <c r="B16" s="107"/>
-      <c r="C16" s="108"/>
+      <c r="A16" s="116"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="118"/>
       <c r="D16" s="36"/>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
@@ -6814,11 +6821,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -7245,15 +7252,15 @@
       <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="112" t="s">
+      <c r="A18" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="113"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="113"/>
-      <c r="E18" s="113"/>
-      <c r="F18" s="113"/>
-      <c r="G18" s="113"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
       <c r="H18" s="67"/>
     </row>
   </sheetData>

</xml_diff>